<commit_message>
updates jinja template for single search parameters
</commit_message>
<xml_diff>
--- a/SP/uscore-server.xlsx
+++ b/SP/uscore-server.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Python\MyNotebooks\SP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A91663-AD5D-452E-BFD8-DD688C17A535}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5554BC-16E4-4E6F-A89D-742A9B627666}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-615" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="117">
   <si>
     <t>Value</t>
   </si>
@@ -328,9 +328,6 @@
     <t>forbidden_s_combos</t>
   </si>
   <si>
-    <t>modifier</t>
-  </si>
-  <si>
     <t>multipleOr</t>
   </si>
   <si>
@@ -343,21 +340,6 @@
     <t>multipleAnd_conf</t>
   </si>
   <si>
-    <t>modifier_conf</t>
-  </si>
-  <si>
-    <t>comparator_conf</t>
-  </si>
-  <si>
-    <t>comparator</t>
-  </si>
-  <si>
-    <t>chain</t>
-  </si>
-  <si>
-    <t>chain_conf</t>
-  </si>
-  <si>
     <t>base</t>
   </si>
   <si>
@@ -386,6 +368,30 @@
   </si>
   <si>
     <t>foo</t>
+  </si>
+  <si>
+    <t>shall_modifier</t>
+  </si>
+  <si>
+    <t>should_modifier</t>
+  </si>
+  <si>
+    <t>shall_comparator</t>
+  </si>
+  <si>
+    <t>should_comparator</t>
+  </si>
+  <si>
+    <t>shall_chain</t>
+  </si>
+  <si>
+    <t>should_chain</t>
+  </si>
+  <si>
+    <t>contains,foo,bar</t>
+  </si>
+  <si>
+    <t>foo,bar2</t>
   </si>
 </sst>
 </file>
@@ -1244,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7399C2ED-EDEB-47AB-8C1E-1290512B1D2F}">
   <dimension ref="A1:X16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,10 +1264,13 @@
     <col min="9" max="9" width="20.7109375" customWidth="1"/>
     <col min="10" max="10" width="24" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
     <col min="13" max="13" width="16.28515625" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16" customWidth="1"/>
-    <col min="18" max="19" width="49.7109375" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="49.7109375" customWidth="1"/>
+    <col min="19" max="19" width="16" customWidth="1"/>
     <col min="20" max="20" width="45.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -1270,58 +1279,58 @@
   <sheetData>
     <row r="1" spans="1:24" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>63</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>69</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="N1" s="5" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="S1" s="5" t="s">
         <v>104</v>
@@ -1336,10 +1345,10 @@
         <v>4</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1380,7 +1389,7 @@
         <v>31</v>
       </c>
       <c r="X2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -1415,18 +1424,6 @@
       <c r="K3" t="s">
         <v>26</v>
       </c>
-      <c r="M3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>31</v>
-      </c>
-      <c r="R3" t="s">
-        <v>31</v>
-      </c>
       <c r="V3" t="s">
         <v>31</v>
       </c>
@@ -1466,18 +1463,6 @@
       <c r="K4" t="s">
         <v>25</v>
       </c>
-      <c r="M4" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>31</v>
-      </c>
-      <c r="R4" t="s">
-        <v>31</v>
-      </c>
       <c r="T4" t="s">
         <v>91</v>
       </c>
@@ -1523,20 +1508,20 @@
       <c r="K5" t="s">
         <v>25</v>
       </c>
-      <c r="M5" t="s">
-        <v>37</v>
-      </c>
       <c r="N5" t="s">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="O5" t="s">
-        <v>31</v>
+        <v>115</v>
+      </c>
+      <c r="P5" t="s">
+        <v>116</v>
       </c>
       <c r="Q5" t="s">
-        <v>31</v>
+        <v>115</v>
       </c>
       <c r="R5" t="s">
-        <v>31</v>
+        <v>116</v>
       </c>
       <c r="T5" t="s">
         <v>39</v>
@@ -1586,18 +1571,6 @@
       <c r="M6" t="s">
         <v>37</v>
       </c>
-      <c r="N6" t="s">
-        <v>5</v>
-      </c>
-      <c r="O6" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>31</v>
-      </c>
-      <c r="R6" t="s">
-        <v>31</v>
-      </c>
       <c r="T6" t="s">
         <v>92</v>
       </c>
@@ -1643,18 +1616,6 @@
       <c r="K7" t="s">
         <v>25</v>
       </c>
-      <c r="M7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O7" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>31</v>
-      </c>
-      <c r="R7" t="s">
-        <v>31</v>
-      </c>
       <c r="V7" t="s">
         <v>31</v>
       </c>
@@ -1694,18 +1655,6 @@
       <c r="K8" t="s">
         <v>26</v>
       </c>
-      <c r="M8" t="s">
-        <v>31</v>
-      </c>
-      <c r="O8" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>31</v>
-      </c>
-      <c r="R8" t="s">
-        <v>31</v>
-      </c>
       <c r="V8" t="s">
         <v>31</v>
       </c>
@@ -1745,18 +1694,6 @@
       <c r="K9" t="s">
         <v>26</v>
       </c>
-      <c r="M9" t="s">
-        <v>31</v>
-      </c>
-      <c r="O9" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>31</v>
-      </c>
-      <c r="R9" t="s">
-        <v>31</v>
-      </c>
       <c r="V9" t="s">
         <v>31</v>
       </c>
@@ -1796,18 +1733,6 @@
       <c r="K10" t="s">
         <v>25</v>
       </c>
-      <c r="M10" t="s">
-        <v>31</v>
-      </c>
-      <c r="O10" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>31</v>
-      </c>
-      <c r="R10" t="s">
-        <v>31</v>
-      </c>
       <c r="V10" t="s">
         <v>31</v>
       </c>
@@ -1847,20 +1772,11 @@
       <c r="K11" t="s">
         <v>25</v>
       </c>
-      <c r="M11" t="s">
-        <v>31</v>
-      </c>
-      <c r="O11" t="s">
-        <v>31</v>
-      </c>
       <c r="Q11" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="R11" t="s">
-        <v>46</v>
-      </c>
-      <c r="S11" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="T11" t="s">
         <v>86</v>
@@ -1907,18 +1823,6 @@
       <c r="K12" t="s">
         <v>25</v>
       </c>
-      <c r="M12" t="s">
-        <v>31</v>
-      </c>
-      <c r="O12" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>31</v>
-      </c>
-      <c r="R12" t="s">
-        <v>31</v>
-      </c>
       <c r="V12" t="s">
         <v>31</v>
       </c>
@@ -1958,18 +1862,6 @@
       <c r="K13" t="s">
         <v>25</v>
       </c>
-      <c r="M13" t="s">
-        <v>31</v>
-      </c>
-      <c r="O13" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>31</v>
-      </c>
-      <c r="R13" t="s">
-        <v>31</v>
-      </c>
       <c r="T13" t="s">
         <v>90</v>
       </c>
@@ -2015,18 +1907,6 @@
       <c r="K14" t="s">
         <v>25</v>
       </c>
-      <c r="M14" t="s">
-        <v>31</v>
-      </c>
-      <c r="O14" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>31</v>
-      </c>
-      <c r="R14" t="s">
-        <v>31</v>
-      </c>
       <c r="V14" t="s">
         <v>31</v>
       </c>
@@ -2066,18 +1946,6 @@
       <c r="K15" t="s">
         <v>25</v>
       </c>
-      <c r="M15" t="s">
-        <v>31</v>
-      </c>
-      <c r="O15" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>31</v>
-      </c>
-      <c r="R15" t="s">
-        <v>31</v>
-      </c>
       <c r="V15" t="s">
         <v>31</v>
       </c>
@@ -2117,17 +1985,8 @@
       <c r="K16" t="s">
         <v>26</v>
       </c>
-      <c r="M16" t="s">
-        <v>31</v>
-      </c>
       <c r="O16" t="s">
         <v>53</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>31</v>
-      </c>
-      <c r="R16" t="s">
-        <v>31</v>
       </c>
       <c r="V16" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
added patient, encoutner and allergies to sp
</commit_message>
<xml_diff>
--- a/SP/uscore-server.xlsx
+++ b/SP/uscore-server.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="6" autoFilterDateGrouping="1" firstSheet="1" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-28920" yWindow="-615"/>
+    <workbookView activeTab="6" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-28920" yWindow="-615"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="meta" sheetId="1" state="visible" r:id="rId1"/>
@@ -24,7 +24,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -53,6 +53,12 @@
       <family val="2"/>
       <color rgb="FF333333"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <color rgb="FF333333"/>
+      <sz val="9"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -116,7 +122,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
@@ -128,10 +134,11 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -447,8 +454,8 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -477,7 +484,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>assessmentbank</t>
+          <t>uscore-server</t>
         </is>
       </c>
     </row>
@@ -501,7 +508,7 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>http://fhir.org/guides/argonaut-questionnaire/ImplementationGuide/ig,http://hl7.org/fhir/us/core/ImplementationGuide/ig</t>
+          <t>http://hl7.org/fhir/us/core/ImplementationGuide/ig</t>
         </is>
       </c>
     </row>
@@ -548,7 +555,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B4" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" display="http://fhir.org/guides/argonaut-questionnaire/ImplementationGuide/ig,http://hl7.org/fhir/us/core/ImplementationGuide/ig" ref="B4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -563,7 +570,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -655,13 +662,13 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" style="1" width="89"/>
-    <col customWidth="1" max="3" min="3" style="1" width="36.42578125"/>
+    <col customWidth="1" max="3" min="3" style="1" width="44.85546875"/>
     <col customWidth="1" max="4" min="4" style="1" width="16.140625"/>
   </cols>
   <sheetData>
@@ -814,10 +821,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -829,7 +836,7 @@
     <col customWidth="1" max="6" min="5" style="1" width="17.42578125"/>
     <col customWidth="1" max="7" min="7" style="1" width="20.5703125"/>
     <col bestFit="1" customWidth="1" max="8" min="8" style="1" width="13.42578125"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="1" width="19.85546875"/>
+    <col bestFit="1" customWidth="1" max="9" min="9" style="1" width="27.140625"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -926,6 +933,40 @@
         </is>
       </c>
       <c r="C3" t="inlineStr">
+        <is>
+          <t>todo</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SHALL</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>todo</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SHALL</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>todo</t>
         </is>
@@ -1138,15 +1179,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <pane activePane="bottomRight" state="frozen" topLeftCell="E2" xSplit="4" ySplit="1"/>
+      <selection activeCell="E1" pane="topRight" sqref="E1"/>
+      <selection activeCell="A2" pane="bottomLeft" sqref="A2"/>
+      <selection activeCell="C22" pane="bottomRight" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="1" width="63.5703125"/>
+    <col customWidth="1" max="1" min="1" style="1" width="21.5703125"/>
     <col customWidth="1" max="3" min="2" style="1" width="19.7109375"/>
     <col customWidth="1" max="4" min="4" style="1" width="19.5703125"/>
     <col bestFit="1" customWidth="1" max="7" min="7" style="1" width="22.7109375"/>
@@ -1162,9 +1206,10 @@
     <col customWidth="1" max="19" min="18" style="1" width="49.7109375"/>
     <col customWidth="1" max="20" min="20" style="1" width="16"/>
     <col customWidth="1" max="21" min="21" style="1" width="50.85546875"/>
-    <col bestFit="1" customWidth="1" max="22" min="22" style="1" width="11.85546875"/>
-    <col bestFit="1" customWidth="1" max="24" min="24" style="1" width="14.5703125"/>
-    <col customWidth="1" max="25" min="25" style="1" width="14.5703125"/>
+    <col customWidth="1" max="22" min="22" style="1" width="18.5703125"/>
+    <col bestFit="1" customWidth="1" max="23" min="23" style="1" width="68.7109375"/>
+    <col bestFit="1" customWidth="1" max="24" min="24" style="1" width="54.85546875"/>
+    <col bestFit="1" customWidth="1" max="25" min="25" style="1" width="83.5703125"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="18" r="1" s="1" thickBot="1">
@@ -1322,7 +1367,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1394,7 +1439,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -1497,11 +1542,6 @@
           <t>title,publisher,version,context-type-value</t>
         </is>
       </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>SHALL</t>
-        </is>
-      </c>
       <c r="W4" t="inlineStr">
         <is>
           <t>n/a</t>
@@ -1583,29 +1623,19 @@
           <t>contains,foo,bar</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>contains,foo,bar</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
         <is>
           <t>foo,bar2</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>contains,foo,bar</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>foo,bar2</t>
-        </is>
-      </c>
       <c r="U5" t="inlineStr">
         <is>
           <t>version</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>SHOULD</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
@@ -1689,11 +1719,6 @@
           <t>context-type-value,version</t>
         </is>
       </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>SHOULD</t>
-        </is>
-      </c>
       <c r="W6" t="inlineStr">
         <is>
           <t>n/a</t>
@@ -1809,7 +1834,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1880,47 +1905,897 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Resource</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>token</t>
+        </is>
+      </c>
+      <c r="I9">
+        <f>A9&amp;"."&amp;D9</f>
+        <v/>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
           <t>N</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>support searching for all allergies for a patient</t>
+        </is>
+      </c>
+      <c r="X9" s="6" t="inlineStr">
+        <is>
+          <t>GET [base]/AllergyIntolerance?patient=1137192</t>
+        </is>
+      </c>
+      <c r="Y9" s="6" t="inlineStr">
+        <is>
+          <t>Fetches a bundle of all AllergyIntolerance resources for the specified patient</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="10" s="1">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SHALL</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>_id</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>Resource</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>token</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>Questionnaire.id</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
+      <c r="I10">
+        <f>A10&amp;"."&amp;D10</f>
+        <v/>
+      </c>
+      <c r="J10" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>support searching for all allergies for a patient</t>
-        </is>
-      </c>
-      <c r="X9" s="6" t="inlineStr">
-        <is>
-          <t>GET [base]/AllergyIntolerance?patient=1137192</t>
-        </is>
-      </c>
-      <c r="Y9" s="6" t="inlineStr">
-        <is>
-          <t>Fetches a bundle of all AllergyIntolerance resources for the specified patient</t>
+      <c r="W10" s="6" t="inlineStr">
+        <is>
+          <t>support fetching a Patient</t>
+        </is>
+      </c>
+      <c r="X10" s="6" t="inlineStr">
+        <is>
+          <t>GET [base]/Patient/1032702</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SHALL</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>token</t>
+        </is>
+      </c>
+      <c r="I11">
+        <f>A11&amp;"."&amp;D11</f>
+        <v/>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="W11" s="6" t="inlineStr">
+        <is>
+          <t>support searching a Patient by an Identifier such as a MPI</t>
+        </is>
+      </c>
+      <c r="X11" s="6" t="inlineStr">
+        <is>
+          <t>GET [base]/Patient?name=Shaw&amp;birthdate=2007-03-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SHALL</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I12">
+        <f>A12&amp;"."&amp;D12</f>
+        <v/>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>gender,birthdate</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>See combination searches below</t>
+        </is>
+      </c>
+      <c r="Y12" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Search based on at least name and another patient element </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SHALL</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>birthdate</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="I13">
+        <f>A13&amp;"."&amp;D13</f>
+        <v/>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>See combination searches below</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Search based on at least birthdate and another patient element </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SHALL</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>gender</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>token</t>
+        </is>
+      </c>
+      <c r="I14">
+        <f>A14&amp;"."&amp;D14</f>
+        <v/>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>family,given</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>See combination searches below</t>
+        </is>
+      </c>
+      <c r="Y14" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Search based on at least gender  and another patient element </t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>family</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I15" s="7" t="inlineStr">
+        <is>
+          <t>Patient.name.family</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>See combination searches below</t>
+        </is>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Search based on at least family name and another patient element </t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>given</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I16" s="7" t="inlineStr">
+        <is>
+          <t>Patient.name.given</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>See combination searches below</t>
+        </is>
+      </c>
+      <c r="Y16" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Search based on at least given name and another patient element </t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</t>
+        </is>
+      </c>
+      <c r="D17" s="7" t="inlineStr">
+        <is>
+          <t>address</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I17">
+        <f>A17&amp;"."&amp;D17</f>
+        <v/>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>support searching a Patient based on text address</t>
+        </is>
+      </c>
+      <c r="X17" s="6" t="inlineStr">
+        <is>
+          <t>GET [base]/Organization?address=1183 Mountain View C</t>
+        </is>
+      </c>
+      <c r="Y17" s="6" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>telecom</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I18">
+        <f>A18&amp;"."&amp;D18</f>
+        <v/>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>support searching a Patient based on contact information such as phone number or email address</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>GET [base]/Organization?telecom=(707)555-5555</t>
+        </is>
+      </c>
+      <c r="Y18" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="19" s="1">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>SHALL</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>_id</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>token</t>
+        </is>
+      </c>
+      <c r="I19">
+        <f>A19&amp;"."&amp;D19</f>
+        <v/>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="W19" s="6" t="inlineStr">
+        <is>
+          <t>support fetching an Encounter</t>
+        </is>
+      </c>
+      <c r="X19" s="6" t="inlineStr">
+        <is>
+          <t>GET [base]/Encounter/12354</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="20" s="1">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SHALL</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>patient</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>reference</t>
+        </is>
+      </c>
+      <c r="I20">
+        <f>A20&amp;"."&amp;D20</f>
+        <v/>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>support searching for all encounters for a patient</t>
+        </is>
+      </c>
+      <c r="X20" s="6" t="inlineStr">
+        <is>
+          <t>GET [base]/Encounter?patient=1137192</t>
+        </is>
+      </c>
+      <c r="Y20" s="6" t="inlineStr">
+        <is>
+          <t>Fetches a bundle of all Encounter resources for the specified patient</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="21" s="1">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SHALL</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="I21">
+        <f>A21&amp;"."&amp;D21</f>
+        <v/>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>gt,lt,ge,le</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>patient</t>
+        </is>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>support searching for all encounters by date</t>
+        </is>
+      </c>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>See combination searches below</t>
+        </is>
+      </c>
+      <c r="Y21" s="6" t="inlineStr">
+        <is>
+          <t>Search based on date and patient parameter</t>
         </is>
       </c>
     </row>
@@ -1954,7 +2829,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1963,29 +2838,29 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="9" t="inlineStr">
         <is>
           <t>Base Type</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="9" t="inlineStr">
         <is>
           <t>Combo</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="D1" s="9" t="inlineStr">
         <is>
           <t>Conformance</t>
         </is>
       </c>
-      <c r="E1" s="8" t="inlineStr">
+      <c r="E1" s="9" t="inlineStr">
         <is>
           <t>Parameter Types</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="n">
+      <c r="A2" s="9" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -1995,7 +2870,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>context-type-value+publisher</t>
+          <t>['context-type-value', 'publisher']</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2010,7 +2885,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="n">
+      <c r="A3" s="9" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -2020,7 +2895,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>context-type-value+publisher+status</t>
+          <t>['context-type-value', 'publisher', 'status']</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2030,12 +2905,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['composite', 'token', 'string']</t>
+          <t>['composite', 'string', 'token']</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="n">
+      <c r="A4" s="9" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -2045,7 +2920,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>context-type-value+status</t>
+          <t>['context-type-value', 'status']</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2060,7 +2935,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="n">
+      <c r="A5" s="9" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -2070,7 +2945,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>publisher+status</t>
+          <t>['publisher', 'status']</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2080,12 +2955,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>['token', 'string']</t>
+          <t>['string', 'token']</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="n">
+      <c r="A6" s="9" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -2095,7 +2970,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>publisher+status+version</t>
+          <t>['publisher', 'status', 'version']</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2105,12 +2980,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>['token', 'string']</t>
+          <t>['string', 'token']</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="n">
+      <c r="A7" s="9" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -2120,7 +2995,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>publisher+version</t>
+          <t>['publisher', 'version']</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -2130,12 +3005,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>['token', 'string']</t>
+          <t>['string', 'token']</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="8" t="n">
+      <c r="A8" s="9" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -2145,7 +3020,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>status+title+version</t>
+          <t>['status', 'title', 'version']</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -2155,12 +3030,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>['token', 'string']</t>
+          <t>['string', 'token']</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="8" t="n">
+      <c r="A9" s="9" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -2170,7 +3045,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>status+version</t>
+          <t>['status', 'version']</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -2185,7 +3060,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="8" t="n">
+      <c r="A10" s="9" t="n">
         <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
@@ -2195,7 +3070,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>title+version</t>
+          <t>['title', 'version']</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -2205,97 +3080,97 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>['token', 'string']</t>
+          <t>['string', 'token']</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="8" t="n">
+      <c r="A11" s="9" t="n">
         <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Questionnaire</t>
+          <t>Patient</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>context-type-value+publisher</t>
+          <t>['birthdate', 'name']</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>SHALL</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>['date', 'string']</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>['family', 'gender']</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>SHOULD</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>['composite', 'string']</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="8" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Questionnaire</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>context-type-value+publisher+status</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>['string', 'token']</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>['gender', 'given']</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
         <is>
           <t>SHOULD</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>['composite', 'token', 'string']</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="8" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Questionnaire</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>context-type-value+status</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>SHOULD</t>
-        </is>
-      </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>['composite', 'token']</t>
+          <t>['string', 'token']</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="8" t="n">
+      <c r="A14" s="9" t="n">
         <v>12</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Questionnaire</t>
+          <t>Patient</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>publisher+status</t>
+          <t>['gender', 'name']</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -2305,132 +3180,32 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>['token', 'string']</t>
+          <t>['string', 'token']</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="8" t="n">
+      <c r="A15" s="9" t="n">
         <v>13</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Questionnaire</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>publisher+status+version</t>
+          <t>['date', 'patient']</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>SHOULD</t>
+          <t>SHALL</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>['token', 'string']</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="8" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Questionnaire</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>publisher+version</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>SHOULD</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>['token', 'string']</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Questionnaire</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>status+title+version</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>SHOULD</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>['token', 'string']</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="8" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Questionnaire</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>status+version</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>SHOULD</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>['token']</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="8" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Questionnaire</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>title+version</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>SHOULD</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>['token', 'string']</t>
+          <t>['reference', 'date']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update to sp make so hide sp from quick start.
</commit_message>
<xml_diff>
--- a/SP/uscore-server.xlsx
+++ b/SP/uscore-server.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="6" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-28920" yWindow="-615"/>
+    <workbookView activeTab="7" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-28920" yWindow="-615"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="meta" sheetId="1" state="visible" r:id="rId1"/>
@@ -13,8 +13,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ops" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="interactions" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sps" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sp_combos" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sp_combos" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="generated_combos" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1" refMode="R1C1"/>
@@ -824,7 +824,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -969,6 +969,11 @@
       <c r="C5" t="inlineStr">
         <is>
           <t>todo</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>given|gender,given|birthdate,gender|birthdate</t>
         </is>
       </c>
     </row>
@@ -1179,36 +1184,35 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y21"/>
+  <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane activePane="bottomRight" state="frozen" topLeftCell="E2" xSplit="4" ySplit="1"/>
       <selection activeCell="E1" pane="topRight" sqref="E1"/>
       <selection activeCell="A2" pane="bottomLeft" sqref="A2"/>
-      <selection activeCell="C22" pane="bottomRight" sqref="C22"/>
+      <selection activeCell="H25" pane="bottomRight" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="1" width="21.5703125"/>
     <col customWidth="1" max="3" min="2" style="1" width="19.7109375"/>
-    <col customWidth="1" max="4" min="4" style="1" width="19.5703125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="1" width="22.7109375"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="1" width="36.140625"/>
-    <col customWidth="1" max="10" min="10" style="1" width="20.7109375"/>
-    <col customWidth="1" max="11" min="11" style="1" width="24"/>
-    <col customWidth="1" max="12" min="12" style="1" width="14.28515625"/>
-    <col customWidth="1" max="13" min="13" style="1" width="15.28515625"/>
-    <col customWidth="1" max="14" min="14" style="1" width="16.28515625"/>
-    <col bestFit="1" customWidth="1" max="15" min="15" style="1" width="18"/>
-    <col bestFit="1" customWidth="1" max="16" min="16" style="1" width="19"/>
-    <col bestFit="1" customWidth="1" max="17" min="17" style="1" width="21.140625"/>
-    <col customWidth="1" max="19" min="18" style="1" width="49.7109375"/>
-    <col customWidth="1" max="20" min="20" style="1" width="16"/>
-    <col customWidth="1" max="21" min="21" style="1" width="50.85546875"/>
-    <col customWidth="1" max="22" min="22" style="1" width="18.5703125"/>
+    <col customWidth="1" max="5" min="4" style="1" width="19.5703125"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" style="1" width="22.7109375"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="1" width="36.140625"/>
+    <col customWidth="1" max="11" min="11" style="1" width="20.7109375"/>
+    <col customWidth="1" max="12" min="12" style="1" width="24"/>
+    <col customWidth="1" max="13" min="13" style="1" width="14.28515625"/>
+    <col customWidth="1" max="14" min="14" style="1" width="15.28515625"/>
+    <col customWidth="1" max="15" min="15" style="1" width="16.28515625"/>
+    <col bestFit="1" customWidth="1" max="16" min="16" style="1" width="18"/>
+    <col bestFit="1" customWidth="1" max="17" min="17" style="1" width="19"/>
+    <col bestFit="1" customWidth="1" max="18" min="18" style="1" width="21.140625"/>
+    <col customWidth="1" max="20" min="19" style="1" width="49.7109375"/>
+    <col customWidth="1" max="21" min="21" style="1" width="16"/>
+    <col customWidth="1" max="22" min="22" style="1" width="50.85546875"/>
     <col bestFit="1" customWidth="1" max="23" min="23" style="1" width="68.7109375"/>
-    <col bestFit="1" customWidth="1" max="24" min="24" style="1" width="54.85546875"/>
+    <col customWidth="1" max="24" min="24" style="1" width="72.28515625"/>
     <col bestFit="1" customWidth="1" max="25" min="25" style="1" width="83.5703125"/>
   </cols>
   <sheetData>
@@ -1235,92 +1239,92 @@
       </c>
       <c r="E1" s="5" t="inlineStr">
         <is>
+          <t>display</t>
+        </is>
+      </c>
+      <c r="F1" s="5" t="inlineStr">
+        <is>
           <t>exists</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>update</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="H1" s="5" t="inlineStr">
         <is>
           <t>XBase</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="I1" s="5" t="inlineStr">
+      <c r="J1" s="5" t="inlineStr">
         <is>
           <t>expression</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="K1" s="5" t="inlineStr">
         <is>
           <t>multipleOr</t>
         </is>
       </c>
-      <c r="K1" s="5" t="inlineStr">
+      <c r="L1" s="5" t="inlineStr">
         <is>
           <t>multipleOr_conf</t>
         </is>
       </c>
-      <c r="L1" s="5" t="inlineStr">
+      <c r="M1" s="5" t="inlineStr">
         <is>
           <t>multipleAnd</t>
         </is>
       </c>
-      <c r="M1" s="5" t="inlineStr">
+      <c r="N1" s="5" t="inlineStr">
         <is>
           <t>multipleAnd_conf</t>
         </is>
       </c>
-      <c r="N1" s="5" t="inlineStr">
+      <c r="O1" s="5" t="inlineStr">
         <is>
           <t>shall_modifier</t>
         </is>
       </c>
-      <c r="O1" s="5" t="inlineStr">
+      <c r="P1" s="5" t="inlineStr">
         <is>
           <t>should_modifier</t>
         </is>
       </c>
-      <c r="P1" s="5" t="inlineStr">
+      <c r="Q1" s="5" t="inlineStr">
         <is>
           <t>shall_comparator</t>
         </is>
       </c>
-      <c r="Q1" s="5" t="inlineStr">
+      <c r="R1" s="5" t="inlineStr">
         <is>
           <t>should_comparator</t>
         </is>
       </c>
-      <c r="R1" s="5" t="inlineStr">
+      <c r="S1" s="5" t="inlineStr">
         <is>
           <t>shall_chain</t>
         </is>
       </c>
-      <c r="S1" s="5" t="inlineStr">
+      <c r="T1" s="5" t="inlineStr">
         <is>
           <t>should_chain</t>
         </is>
       </c>
-      <c r="T1" s="5" t="inlineStr">
+      <c r="U1" s="5" t="inlineStr">
         <is>
           <t>references</t>
         </is>
       </c>
-      <c r="U1" s="5" t="inlineStr">
+      <c r="V1" s="5" t="inlineStr">
         <is>
           <t>combo_pairs</t>
-        </is>
-      </c>
-      <c r="V1" s="5" t="inlineStr">
-        <is>
-          <t>combo_conf</t>
         </is>
       </c>
       <c r="W1" s="5" t="inlineStr">
@@ -1360,10 +1364,8 @@
           <t>_id</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="E2" t="b">
+        <v>1</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -1372,25 +1374,30 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>Resource</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>token</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Questionnaire.id</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -1432,10 +1439,8 @@
           <t>url</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="E3" t="b">
+        <v>1</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -1444,24 +1449,29 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>Questionnaire</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>uri</t>
         </is>
       </c>
-      <c r="I3">
+      <c r="J3">
         <f>A3&amp;"."&amp;D3</f>
         <v/>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -1503,10 +1513,8 @@
           <t>status</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="E4" t="b">
+        <v>1</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -1515,29 +1523,34 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
           <t>Questionnaire</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>token</t>
         </is>
       </c>
-      <c r="I4">
+      <c r="J4">
         <f>A4&amp;"."&amp;D4</f>
         <v/>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
         <is>
           <t>title,publisher,version,context-type-value</t>
         </is>
@@ -1579,10 +1592,8 @@
           <t>title</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="E5" t="b">
+        <v>1</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -1591,49 +1602,54 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
           <t>Questionnaire</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>string</t>
         </is>
       </c>
-      <c r="I5">
+      <c r="J5">
         <f>A5&amp;"."&amp;D5</f>
         <v/>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
         <is>
           <t>foo,bar2</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>contains,foo,bar</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>contains,foo,bar</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>foo,bar2</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr">
+      <c r="V5" t="inlineStr">
         <is>
           <t>version</t>
         </is>
@@ -1675,10 +1691,8 @@
           <t>publisher</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="E6" t="b">
+        <v>1</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -1687,34 +1701,39 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
           <t>Questionnaire</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>string</t>
         </is>
       </c>
-      <c r="I6">
+      <c r="J6">
         <f>A6&amp;"."&amp;D6</f>
         <v/>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
         <is>
           <t>contains</t>
         </is>
       </c>
-      <c r="U6" t="inlineStr">
+      <c r="V6" t="inlineStr">
         <is>
           <t>context-type-value,version</t>
         </is>
@@ -1756,10 +1775,8 @@
           <t>version</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="E7" t="b">
+        <v>1</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -1768,24 +1785,29 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
           <t>Questionnaire</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>token</t>
         </is>
       </c>
-      <c r="I7">
+      <c r="J7">
         <f>A7&amp;"."&amp;D7</f>
         <v/>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -1827,36 +1849,39 @@
           <t>context-type-value</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="G8" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
           <t>Questionnaire</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>composite</t>
         </is>
       </c>
-      <c r="I8">
+      <c r="J8">
         <f>A8&amp;"."&amp;D8</f>
         <v/>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -1898,10 +1923,8 @@
           <t>_id</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="E9" t="b">
+        <v>1</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -1910,24 +1933,29 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
           <t>Resource</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>token</t>
         </is>
       </c>
-      <c r="I9">
+      <c r="J9">
         <f>A9&amp;"."&amp;D9</f>
         <v/>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -1969,10 +1997,8 @@
           <t>_id</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="E10" t="b">
+        <v>1</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -1981,24 +2007,29 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
           <t>Resource</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>token</t>
         </is>
       </c>
-      <c r="I10">
+      <c r="J10">
         <f>A10&amp;"."&amp;D10</f>
         <v/>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -2035,10 +2066,8 @@
           <t>identifier</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="E11" t="b">
+        <v>1</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -2047,36 +2076,41 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
           <t>Patient</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>token</t>
         </is>
       </c>
-      <c r="I11">
+      <c r="J11">
         <f>A11&amp;"."&amp;D11</f>
         <v/>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
       </c>
       <c r="W11" s="6" t="inlineStr">
         <is>
-          <t>support searching a Patient by an Identifier such as a MPI</t>
-        </is>
-      </c>
-      <c r="X11" s="6" t="inlineStr">
-        <is>
-          <t>GET [base]/Patient?name=Shaw&amp;birthdate=2007-03-20</t>
+          <t>support searching a Patient by an identifier such as a MPI</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>GET [base]/Patient?identifier=http://hospital.smarthealthit.org|1032702</t>
         </is>
       </c>
     </row>
@@ -2101,10 +2135,8 @@
           <t>name</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="E12" t="b">
+        <v>1</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -2113,29 +2145,34 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
           <t>Patient</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>string</t>
         </is>
       </c>
-      <c r="I12">
+      <c r="J12">
         <f>A12&amp;"."&amp;D12</f>
         <v/>
       </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="U12" t="inlineStr">
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
         <is>
           <t>gender,birthdate</t>
         </is>
@@ -2177,10 +2214,8 @@
           <t>birthdate</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="E13" t="b">
+        <v>0</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -2189,26 +2224,36 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
           <t>Patient</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>date</t>
         </is>
       </c>
-      <c r="I13">
+      <c r="J13">
         <f>A13&amp;"."&amp;D13</f>
         <v/>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
         <is>
           <t>N</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>family</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
@@ -2248,10 +2293,8 @@
           <t>gender</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="E14" t="b">
+        <v>0</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -2260,31 +2303,36 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
           <t>Patient</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>token</t>
         </is>
       </c>
-      <c r="I14">
+      <c r="J14">
         <f>A14&amp;"."&amp;D14</f>
         <v/>
       </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="U14" t="inlineStr">
-        <is>
-          <t>family,given</t>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>family</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
@@ -2324,10 +2372,8 @@
           <t>family</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="E15" t="b">
+        <v>0</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -2336,25 +2382,30 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
           <t>Patient</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>string</t>
         </is>
       </c>
-      <c r="I15" s="7" t="inlineStr">
+      <c r="J15" s="7" t="inlineStr">
         <is>
           <t>Patient.name.family</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -2396,10 +2447,8 @@
           <t>given</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="E16" t="b">
+        <v>0</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -2408,25 +2457,30 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
           <t>Patient</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>string</t>
         </is>
       </c>
-      <c r="I16" s="7" t="inlineStr">
+      <c r="J16" s="7" t="inlineStr">
         <is>
           <t>Patient.name.given</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -2450,54 +2504,57 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>!Patient</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</t>
+        </is>
+      </c>
+      <c r="D17" s="7" t="inlineStr">
+        <is>
+          <t>address</t>
+        </is>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
           <t>Patient</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>SHOULD</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</t>
-        </is>
-      </c>
-      <c r="D17" s="7" t="inlineStr">
-        <is>
-          <t>address</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Patient</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>string</t>
         </is>
       </c>
-      <c r="I17">
+      <c r="J17">
         <f>A17&amp;"."&amp;D17</f>
         <v/>
       </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -2517,54 +2574,57 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>!Patient</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>telecom</t>
+        </is>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
           <t>Patient</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>SHOULD</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>telecom</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Patient</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>string</t>
         </is>
       </c>
-      <c r="I18">
+      <c r="J18">
         <f>A18&amp;"."&amp;D18</f>
         <v/>
       </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -2602,10 +2662,8 @@
           <t>_id</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="E19" t="b">
+        <v>1</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -2614,24 +2672,29 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Encounter</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
           <t>token</t>
         </is>
       </c>
-      <c r="I19">
+      <c r="J19">
         <f>A19&amp;"."&amp;D19</f>
         <v/>
       </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -2668,10 +2731,8 @@
           <t>patient</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="E20" t="b">
+        <v>1</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -2680,26 +2741,36 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Encounter</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
           <t>reference</t>
         </is>
       </c>
-      <c r="I20">
+      <c r="J20">
         <f>A20&amp;"."&amp;D20</f>
         <v/>
       </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
         <is>
           <t>N</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>date,class,type,status</t>
         </is>
       </c>
       <c r="W20" t="inlineStr">
@@ -2739,10 +2810,8 @@
           <t>date</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="E21" t="b">
+        <v>1</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -2751,36 +2820,41 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Encounter</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
           <t>date</t>
         </is>
       </c>
-      <c r="I21">
+      <c r="J21">
         <f>A21&amp;"."&amp;D21</f>
         <v/>
       </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="P21" t="inlineStr">
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
         <is>
           <t>gt,lt,ge,le</t>
         </is>
       </c>
-      <c r="U21" t="inlineStr">
-        <is>
-          <t>patient</t>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>class,type</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
@@ -2796,6 +2870,307 @@
       <c r="Y21" s="6" t="inlineStr">
         <is>
           <t>Search based on date and patient parameter</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>token</t>
+        </is>
+      </c>
+      <c r="J22">
+        <f>A22&amp;"."&amp;D22</f>
+        <v/>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="W22" s="6" t="inlineStr">
+        <is>
+          <t>support searching a Encounter by an identifier</t>
+        </is>
+      </c>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>GET [base]/Encounter?identifier=http://hospital.smarthealthit.org|1032702</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="23" s="1">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>token</t>
+        </is>
+      </c>
+      <c r="J23">
+        <f>A23&amp;"."&amp;D23</f>
+        <v/>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t>class,type</t>
+        </is>
+      </c>
+      <c r="W23" s="6" t="inlineStr">
+        <is>
+          <t>support fetching an Encounter by status</t>
+        </is>
+      </c>
+      <c r="X23" s="6" t="inlineStr">
+        <is>
+          <t>GET [base]/Encounter?status=completed</t>
+        </is>
+      </c>
+      <c r="Y23" s="6" t="inlineStr">
+        <is>
+          <t>Fetches a bundle of all Encounter resources for the specified patient</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="24" s="1">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>class</t>
+        </is>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>token</t>
+        </is>
+      </c>
+      <c r="J24">
+        <f>A24&amp;"."&amp;D24</f>
+        <v/>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="V24" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="W24" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">support fetching an Encounter by the category of the encounter  such as ambulatory (outpatient), inpatient, emergency,  or others </t>
+        </is>
+      </c>
+      <c r="X24" s="6" t="inlineStr">
+        <is>
+          <t>GET [base]/Encounter?status=http://terminology.hl7.org/CodeSystem/v3-ActCode|AMB</t>
+        </is>
+      </c>
+      <c r="Y24" s="6" t="inlineStr">
+        <is>
+          <t>Fetches a bundle of all Encounter resources for the specified patient</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="25" s="1">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>token</t>
+        </is>
+      </c>
+      <c r="J25">
+        <f>A25&amp;"."&amp;D25</f>
+        <v/>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="W25" s="6" t="inlineStr">
+        <is>
+          <t>support fetching an Encounter by the encounter type</t>
+        </is>
+      </c>
+      <c r="X25" s="6" t="inlineStr">
+        <is>
+          <t>GET [base]/Encounter?http://www.ama-assn.org/go/cpt|99201</t>
+        </is>
+      </c>
+      <c r="Y25" s="6" t="inlineStr">
+        <is>
+          <t>Fetches a bundle of all Encounter resources for the specified patient</t>
         </is>
       </c>
     </row>
@@ -2811,15 +3186,770 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="1" width="13.85546875"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="1" width="38.7109375"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="1" width="12.85546875"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="1" width="27"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="1" width="68.7109375"/>
+    <col customWidth="1" max="6" min="6" style="1" width="72.28515625"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="1" width="83.5703125"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="18" r="1" s="1" thickBot="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>base</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>combo</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>combo_conf</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>types</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="F1" s="5" t="inlineStr">
+        <is>
+          <t>example</t>
+        </is>
+      </c>
+      <c r="G1" s="5" t="inlineStr">
+        <is>
+          <t>imp_note</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="2" s="1" thickTop="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>class,date</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>date,token</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>class,date,patient</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>date,reference,token</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>class,date,patient,type</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>date,reference,token</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>class,date,type</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>date,token</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>class,patient</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>reference,token</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>class,patient,status</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>reference,token</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>class,patient,status,type</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>reference,token</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>class,patient,type</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>reference,token</t>
+        </is>
+      </c>
+      <c r="F9" s="6" t="n"/>
+      <c r="G9" s="6" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>class,status</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>token</t>
+        </is>
+      </c>
+      <c r="E10" s="6" t="n"/>
+      <c r="F10" s="6" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>class,status,type</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>token</t>
+        </is>
+      </c>
+      <c r="E11" s="6" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>class,type</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>token</t>
+        </is>
+      </c>
+      <c r="G12" s="6" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>date,patient</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>SHALL</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>date,reference</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>date,patient,type</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>date,reference,token</t>
+        </is>
+      </c>
+      <c r="G14" s="6" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>date,type</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>date,token</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>patient,status</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>reference,token</t>
+        </is>
+      </c>
+      <c r="G16" s="6" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>patient,status,type</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>reference,token</t>
+        </is>
+      </c>
+      <c r="F17" s="6" t="n"/>
+      <c r="G17" s="6" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>patient,type</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>reference,token</t>
+        </is>
+      </c>
+      <c r="G18" s="6" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>status,type</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>token</t>
+        </is>
+      </c>
+      <c r="E19" s="6" t="n"/>
+      <c r="F19" s="6" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Questionnaire</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>context-type-value,publisher</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>composite,string</t>
+        </is>
+      </c>
+      <c r="F20" s="6" t="n"/>
+      <c r="G20" s="6" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Questionnaire</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>context-type-value,publisher,status</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>composite,string,token</t>
+        </is>
+      </c>
+      <c r="G21" s="6" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Questionnaire</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>context-type-value,status</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>composite,token</t>
+        </is>
+      </c>
+      <c r="E22" s="6" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Questionnaire</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>publisher,status</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>SHALL</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>string,token</t>
+        </is>
+      </c>
+      <c r="E23" s="6" t="n"/>
+      <c r="F23" s="6" t="n"/>
+      <c r="G23" s="6" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Questionnaire</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>publisher,status,version</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>string,token</t>
+        </is>
+      </c>
+      <c r="E24" s="6" t="n"/>
+      <c r="F24" s="6" t="n"/>
+      <c r="G24" s="6" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Questionnaire</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>publisher,version</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>string,token</t>
+        </is>
+      </c>
+      <c r="E25" s="6" t="n"/>
+      <c r="F25" s="6" t="n"/>
+      <c r="G25" s="6" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Questionnaire</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>status,title,version</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>string,token</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Questionnaire</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>status,version</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>token</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Questionnaire</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>title,version</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>string,token</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>birthdate,family</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>date,string</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>birthdate,name</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>SHALL</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>date,string</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>family,gender</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>string,token</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>gender,name</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>SHALL</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>string,token</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -2829,7 +3959,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2865,12 +3995,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Questionnaire</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['context-type-value', 'publisher']</t>
+          <t>['class', 'date']</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2880,7 +4010,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['composite', 'string']</t>
+          <t>['date', 'token']</t>
         </is>
       </c>
     </row>
@@ -2890,12 +4020,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Questionnaire</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['context-type-value', 'publisher', 'status']</t>
+          <t>['class', 'date', 'patient']</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2905,7 +4035,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['composite', 'string', 'token']</t>
+          <t>['date', 'reference', 'token']</t>
         </is>
       </c>
     </row>
@@ -2915,12 +4045,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Questionnaire</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['context-type-value', 'status']</t>
+          <t>['class', 'date', 'patient', 'type']</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2930,7 +4060,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>['composite', 'token']</t>
+          <t>['date', 'reference', 'token']</t>
         </is>
       </c>
     </row>
@@ -2940,22 +4070,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Questionnaire</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['publisher', 'status']</t>
+          <t>['class', 'date', 'type']</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>SHALL</t>
+          <t>SHOULD</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>['string', 'token']</t>
+          <t>['date', 'token']</t>
         </is>
       </c>
     </row>
@@ -2965,12 +4095,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Questionnaire</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['publisher', 'status', 'version']</t>
+          <t>['class', 'patient']</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2980,7 +4110,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>['string', 'token']</t>
+          <t>['reference', 'token']</t>
         </is>
       </c>
     </row>
@@ -2990,12 +4120,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Questionnaire</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>['publisher', 'version']</t>
+          <t>['class', 'patient', 'status']</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -3005,7 +4135,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>['string', 'token']</t>
+          <t>['reference', 'token']</t>
         </is>
       </c>
     </row>
@@ -3015,12 +4145,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Questionnaire</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>['status', 'title', 'version']</t>
+          <t>['class', 'patient', 'status', 'type']</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -3030,7 +4160,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>['string', 'token']</t>
+          <t>['reference', 'token']</t>
         </is>
       </c>
     </row>
@@ -3040,12 +4170,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Questionnaire</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>['status', 'version']</t>
+          <t>['class', 'patient', 'type']</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -3055,7 +4185,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>['token']</t>
+          <t>['reference', 'token']</t>
         </is>
       </c>
     </row>
@@ -3065,12 +4195,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Questionnaire</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>['title', 'version']</t>
+          <t>['class', 'status']</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -3080,7 +4210,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>['string', 'token']</t>
+          <t>['token']</t>
         </is>
       </c>
     </row>
@@ -3090,22 +4220,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Patient</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>['birthdate', 'name']</t>
+          <t>['class', 'status', 'type']</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>SHALL</t>
+          <t>SHOULD</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>['date', 'string']</t>
+          <t>['token']</t>
         </is>
       </c>
     </row>
@@ -3115,12 +4245,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Patient</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>['family', 'gender']</t>
+          <t>['class', 'type']</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -3130,7 +4260,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>['string', 'token']</t>
+          <t>['token']</t>
         </is>
       </c>
     </row>
@@ -3140,22 +4270,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Patient</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>['gender', 'given']</t>
+          <t>['date', 'patient']</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>SHOULD</t>
+          <t>SHALL</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>['string', 'token']</t>
+          <t>['date', 'reference']</t>
         </is>
       </c>
     </row>
@@ -3165,22 +4295,22 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Patient</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>['gender', 'name']</t>
+          <t>['date', 'patient', 'type']</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>SHALL</t>
+          <t>SHOULD</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>['string', 'token']</t>
+          <t>['date', 'reference', 'token']</t>
         </is>
       </c>
     </row>
@@ -3195,17 +4325,442 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>['date', 'patient']</t>
+          <t>['date', 'type']</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>['date', 'token']</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="9" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>['patient', 'status']</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>['reference', 'token']</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="9" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>['patient', 'status', 'type']</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>['reference', 'token']</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>['patient', 'type']</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>['reference', 'token']</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>['status', 'type']</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>['token']</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="9" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Questionnaire</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>['context-type-value', 'publisher']</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>['composite', 'string']</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="9" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Questionnaire</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>['context-type-value', 'publisher', 'status']</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>['composite', 'string', 'token']</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="9" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Questionnaire</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>['context-type-value', 'status']</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>['composite', 'token']</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="9" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Questionnaire</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>['publisher', 'status']</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
           <t>SHALL</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>['reference', 'date']</t>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>['string', 'token']</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="9" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Questionnaire</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>['publisher', 'status', 'version']</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>['string', 'token']</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="9" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Questionnaire</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>['publisher', 'version']</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>['string', 'token']</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="9" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Questionnaire</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>['status', 'title', 'version']</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>['string', 'token']</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="9" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Questionnaire</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>['status', 'version']</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>['token']</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="9" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Questionnaire</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>['title', 'version']</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>['string', 'token']</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="9" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>['birthdate', 'family']</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>['date', 'string']</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="9" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>['birthdate', 'name']</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>SHALL</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>['date', 'string']</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="9" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>['family', 'gender']</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>SHOULD</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>['string', 'token']</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>['gender', 'name']</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>SHALL</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>['string', 'token']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add links to sps
</commit_message>
<xml_diff>
--- a/SP/uscore-server.xlsx
+++ b/SP/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/Python/MyNotebooks/SP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBA1405-E76A-F14E-B78E-ABE5315F5E45}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E1366A-E58C-7841-B2FB-1821AFA59527}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11420" windowHeight="18000" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-68800" yWindow="-10800" windowWidth="68800" windowHeight="28800" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="264">
   <si>
     <t>Element</t>
   </si>
@@ -295,9 +295,6 @@
     <t>imp_note</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-q-test</t>
-  </si>
-  <si>
     <t>_id</t>
   </si>
   <si>
@@ -313,12 +310,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>example for testing</t>
-  </si>
-  <si>
     <t>url</t>
   </si>
   <si>
@@ -385,9 +376,6 @@
     <t>support searching a Patient by an identifier such as a MPI</t>
   </si>
   <si>
-    <t>GET [base]/Patient?identifier=http://hospital.smarthealthit.org|1032702</t>
-  </si>
-  <si>
     <t>gender,birthdate</t>
   </si>
   <si>
@@ -406,30 +394,18 @@
     <t>family</t>
   </si>
   <si>
-    <t xml:space="preserve">Search based on at least birthdate and another patient element </t>
-  </si>
-  <si>
     <t>gender</t>
   </si>
   <si>
-    <t xml:space="preserve">Search based on at least gender  and another patient element </t>
-  </si>
-  <si>
     <t>Patient.name.family</t>
   </si>
   <si>
-    <t xml:space="preserve">Search based on at least family name and another patient element </t>
-  </si>
-  <si>
     <t>given</t>
   </si>
   <si>
     <t>Patient.name.given</t>
   </si>
   <si>
-    <t xml:space="preserve">Search based on at least given name and another patient element </t>
-  </si>
-  <si>
     <t>!Patient</t>
   </si>
   <si>
@@ -451,9 +427,6 @@
     <t>GET [base]/Organization?telecom=(707)555-5555</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</t>
-  </si>
-  <si>
     <t>support fetching an Encounter</t>
   </si>
   <si>
@@ -472,48 +445,18 @@
     <t>support searching for all encounters for a patient</t>
   </si>
   <si>
-    <t>Fetches a bundle of all Encounter resources for the specified patient</t>
-  </si>
-  <si>
     <t>gt,lt,ge,le</t>
   </si>
   <si>
     <t>class,type</t>
   </si>
   <si>
-    <t>support searching for all encounters by date</t>
-  </si>
-  <si>
-    <t>Search based on date and patient parameter</t>
-  </si>
-  <si>
     <t>support searching a Encounter by an identifier</t>
   </si>
   <si>
-    <t>GET [base]/Encounter?identifier=http://hospital.smarthealthit.org|1032702</t>
-  </si>
-  <si>
-    <t>support fetching an Encounter by status</t>
-  </si>
-  <si>
-    <t>GET [base]/Encounter?status=completed</t>
-  </si>
-  <si>
     <t>class</t>
   </si>
   <si>
-    <t xml:space="preserve">support fetching an Encounter by the category of the encounter  such as ambulatory (outpatient), inpatient, emergency,  or others </t>
-  </si>
-  <si>
-    <t>GET [base]/Encounter?status=http://terminology.hl7.org/CodeSystem/v3-ActCode|AMB</t>
-  </si>
-  <si>
-    <t>support fetching an Encounter by the encounter type</t>
-  </si>
-  <si>
-    <t>GET [base]/Encounter?http://www.ama-assn.org/go/cpt|99201</t>
-  </si>
-  <si>
     <t>combo</t>
   </si>
   <si>
@@ -775,9 +718,6 @@
     <t>Condition</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</t>
-  </si>
-  <si>
     <t>clinical-status</t>
   </si>
   <si>
@@ -835,18 +775,12 @@
     <t>onset-date</t>
   </si>
   <si>
-    <t>support searching for all *active*  or "inactive* allergies for a patient</t>
-  </si>
-  <si>
     <t>support searching for all *active* conditions for a patient</t>
   </si>
   <si>
     <t>GET [base/Condition?patient=[id]&amp;clinical-status=active,recurrance,remission</t>
   </si>
   <si>
-    <t>GET [base]/Condition?patient=[id]&amp;code=[system|code]</t>
-  </si>
-  <si>
     <t>GET [base]/AllergyIntolerance?patient=[id]&amp;clinical-status=active</t>
   </si>
   <si>
@@ -860,6 +794,45 @@
   </si>
   <si>
     <t>!Questionnaire</t>
+  </si>
+  <si>
+    <t>GET [base]/Patient?identifier=http://hospital.smarthealthit.org\|1032702</t>
+  </si>
+  <si>
+    <t>GET [base]/Encounter?identifier=http://hospital.smarthealthit.org\|1032702</t>
+  </si>
+  <si>
+    <t>Immunization</t>
+  </si>
+  <si>
+    <t>support searching for all *active*  or *inactive* allergies for a patient</t>
+  </si>
+  <si>
+    <t>support searching for all immunizationss for a patient for a specified time period</t>
+  </si>
+  <si>
+    <t>GET [base]/Condition?patient=[id]&amp;code=[system\|code]</t>
+  </si>
+  <si>
+    <t>support searching for all completed immunizations for a patient</t>
+  </si>
+  <si>
+    <t>GET [base]/Immunization?patient=1137192&amp;status=completed</t>
+  </si>
+  <si>
+    <t>GET [base]/Immunization?patient=1137192&amp;date=ge2019-01-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fetches a bundle of all Immunization resources for the specified patient and date. </t>
+  </si>
+  <si>
+    <t>patient,date</t>
+  </si>
+  <si>
+    <t>rel_url</t>
+  </si>
+  <si>
+    <t>!EXAMPLE PATIENT SEARCH</t>
   </si>
 </sst>
 </file>
@@ -976,8 +949,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
@@ -1795,13 +1768,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:Y31"/>
+  <dimension ref="A1:Z35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="X44" sqref="X44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1810,7 +1783,7 @@
     <col min="2" max="2" width="21.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="1" customWidth="1"/>
     <col min="10" max="10" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.1640625" style="1" customWidth="1"/>
@@ -1825,13 +1798,14 @@
     <col min="21" max="21" width="16" style="1" customWidth="1"/>
     <col min="22" max="22" width="50.83203125" style="1" customWidth="1"/>
     <col min="23" max="23" width="68.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="72.33203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="90.6640625" style="1" customWidth="1"/>
     <col min="25" max="25" width="83.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>64</v>
@@ -1905,100 +1879,111 @@
       <c r="Y1" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="Z1" s="10" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J2" t="str">
         <f>B2&amp;"."&amp;C2</f>
         <v>!Patient.address</v>
       </c>
       <c r="K2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="Y2" s="6"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z2" t="str">
+        <f>"SearchParameter-us-core-"&amp;LOWER((B2)&amp;"-"&amp;C2&amp;".html")</f>
+        <v>SearchParameter-us-core-!patient-address.html</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J3" t="str">
         <f>B3&amp;"."&amp;C3</f>
         <v>!Patient.telecom</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="Y3" s="6"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z3" s="1" t="str">
+        <f t="shared" ref="Z3:Z34" si="0">"SearchParameter-us-core-"&amp;LOWER((B3)&amp;"-"&amp;C3&amp;".html")</f>
+        <v>SearchParameter-us-core-!patient-telecom.html</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2006,41 +1991,45 @@
         <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
       <c r="G4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" t="s">
         <v>86</v>
-      </c>
-      <c r="H4" t="s">
-        <v>86</v>
-      </c>
-      <c r="I4" t="s">
-        <v>87</v>
       </c>
       <c r="J4" t="str">
         <f>B4&amp;"."&amp;C4</f>
         <v>AllergyIntolerance.clinical-status</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V4"/>
       <c r="X4" s="6"/>
       <c r="Y4" s="6"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-allergyintolerance-clinical-status.html</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2048,35 +2037,35 @@
         <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I5" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="J5" t="str">
         <f>B5&amp;"."&amp;C5</f>
         <v>AllergyIntolerance.patient</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P5"/>
       <c r="Q5"/>
@@ -2084,7 +2073,7 @@
       <c r="T5"/>
       <c r="V5"/>
       <c r="W5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="X5" s="6" t="str">
         <f>"GET [base]/"&amp;B5&amp;"?patient=1137192"</f>
@@ -2094,145 +2083,154 @@
         <f>"Fetches a bundle of all "&amp;B5&amp; " resources for the specified patient"</f>
         <v>Fetches a bundle of all AllergyIntolerance resources for the specified patient</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-allergyintolerance-patient.html</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="C6" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>244</v>
+        <v>101</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <f t="shared" ref="E6:E34" si="1">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B6)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
       </c>
       <c r="G6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" t="s">
         <v>86</v>
-      </c>
-      <c r="H6" t="s">
-        <v>86</v>
-      </c>
-      <c r="I6" t="s">
-        <v>87</v>
       </c>
       <c r="J6" t="str">
         <f>B6&amp;"."&amp;C6</f>
         <v>Condition.category</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O6"/>
       <c r="V6" t="s">
         <v>31</v>
       </c>
-      <c r="W6" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="X6" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="Y6" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-condition-category.html</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="C7" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>244</v>
+      <c r="E7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
       </c>
       <c r="G7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" t="s">
         <v>86</v>
-      </c>
-      <c r="H7" t="s">
-        <v>86</v>
-      </c>
-      <c r="I7" t="s">
-        <v>87</v>
       </c>
       <c r="J7" t="str">
         <f>B7&amp;"."&amp;C7</f>
         <v>Condition.clinical-status</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="Y7" s="6"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-condition-clinical-status.html</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="C8" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>244</v>
+      <c r="E8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I8" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="J8" t="str">
         <f>B8&amp;"."&amp;C8</f>
         <v>Condition.patient</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="X8" s="6" t="str">
         <f>"GET [base]/"&amp;B8&amp;"?patient=1137192"</f>
@@ -2242,8 +2240,12 @@
         <f>"Fetches a bundle of all "&amp;B8&amp; " resources for the specified patient"</f>
         <v>Fetches a bundle of all Condition resources for the specified patient</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-condition-patient.html</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2251,44 +2253,49 @@
         <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s">
-        <v>136</v>
+      <c r="E9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
       </c>
       <c r="G9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" t="s">
         <v>86</v>
-      </c>
-      <c r="H9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I9" t="s">
-        <v>87</v>
       </c>
       <c r="J9" t="str">
         <f>B9&amp;"."&amp;C9</f>
         <v>Encounter._id</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="W9" s="6" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="X9" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="Z9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-encounter-_id.html</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2296,50 +2303,49 @@
         <v>46</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>136</v>
+        <v>101</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="F10" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="J10" s="1" t="str">
         <f>B10&amp;"."&amp;C10</f>
         <v>Encounter.class</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W10" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="X10" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="Y10" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-encounter-class.html</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2347,53 +2353,50 @@
         <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" t="s">
-        <v>136</v>
+      <c r="E11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J11" t="str">
         <f>B11&amp;"."&amp;C11</f>
         <v>Encounter.date</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="X11" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y11" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-encounter-date.html</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2401,44 +2404,49 @@
         <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E12" t="s">
-        <v>136</v>
+        <v>101</v>
+      </c>
+      <c r="E12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
       </c>
       <c r="G12" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" t="s">
         <v>86</v>
-      </c>
-      <c r="H12" t="s">
-        <v>86</v>
-      </c>
-      <c r="I12" t="s">
-        <v>87</v>
       </c>
       <c r="J12" t="str">
         <f>B12&amp;"."&amp;C12</f>
         <v>Encounter.identifier</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="W12" s="6" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="X12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+      <c r="Z12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-encounter-identifier.html</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2446,41 +2454,42 @@
         <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
       </c>
-      <c r="E13" t="s">
-        <v>136</v>
+      <c r="E13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I13" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="J13" s="1" t="str">
         <f>B13&amp;"."&amp;C13</f>
         <v>Encounter.patient</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V13" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="W13" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="X13" s="6" t="str">
         <f>"GET [base]/"&amp;B13&amp;"?patient=1137192"</f>
@@ -2490,8 +2499,12 @@
         <f>"Fetches a bundle of all "&amp;B13&amp; " resources for the specified patient"</f>
         <v>Fetches a bundle of all Encounter resources for the specified patient</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-encounter-patient.html</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2499,50 +2512,49 @@
         <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D14" t="s">
-        <v>104</v>
-      </c>
-      <c r="E14" t="s">
-        <v>136</v>
+        <v>101</v>
+      </c>
+      <c r="E14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="F14" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G14" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" t="s">
+        <v>85</v>
+      </c>
+      <c r="I14" t="s">
         <v>86</v>
-      </c>
-      <c r="H14" t="s">
-        <v>86</v>
-      </c>
-      <c r="I14" t="s">
-        <v>87</v>
       </c>
       <c r="J14" t="str">
         <f>B14&amp;"."&amp;C14</f>
         <v>Encounter.status</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V14" t="s">
-        <v>145</v>
-      </c>
-      <c r="W14" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="X14" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="Y14" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-encounter-status.html</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2553,45 +2565,44 @@
         <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E15" t="s">
-        <v>136</v>
+        <v>101</v>
+      </c>
+      <c r="E15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="F15" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G15" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" t="s">
+        <v>85</v>
+      </c>
+      <c r="I15" t="s">
         <v>86</v>
-      </c>
-      <c r="H15" t="s">
-        <v>86</v>
-      </c>
-      <c r="I15" t="s">
-        <v>87</v>
       </c>
       <c r="J15" s="1" t="str">
         <f>B15&amp;"."&amp;C15</f>
         <v>Encounter.type</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V15"/>
-      <c r="W15" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="X15" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="Y15" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-encounter-type.html</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2599,45 +2610,50 @@
         <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16" t="s">
         <v>20</v>
       </c>
-      <c r="E16" t="s">
-        <v>109</v>
+      <c r="E16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
       </c>
       <c r="G16" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I16" t="s">
         <v>86</v>
-      </c>
-      <c r="H16" t="s">
-        <v>86</v>
-      </c>
-      <c r="I16" t="s">
-        <v>87</v>
       </c>
       <c r="J16" s="1" t="str">
         <f>B16&amp;"."&amp;C16</f>
         <v>Patient._id</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="W16" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="X16" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="Y16"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-patient-_id.html</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2645,50 +2661,47 @@
         <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D17" t="s">
         <v>20</v>
       </c>
-      <c r="E17" t="s">
-        <v>109</v>
+      <c r="E17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I17" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J17" s="1" t="str">
         <f>B17&amp;"."&amp;C17</f>
         <v>Patient.birthdate</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="W17" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="X17" t="s">
         <v>116</v>
       </c>
-      <c r="Y17" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="X17"/>
+      <c r="Z17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-patient-birthdate.html</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2696,46 +2709,43 @@
         <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D18" t="s">
-        <v>104</v>
-      </c>
-      <c r="E18" t="s">
-        <v>109</v>
+        <v>101</v>
+      </c>
+      <c r="E18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I18" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="W18" t="s">
-        <v>90</v>
-      </c>
-      <c r="X18" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y18" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="W18"/>
+      <c r="Z18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-patient-family.html</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2743,50 +2753,48 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D19" t="s">
         <v>20</v>
       </c>
-      <c r="E19" t="s">
-        <v>109</v>
+      <c r="E19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
       </c>
       <c r="G19" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" t="s">
+        <v>85</v>
+      </c>
+      <c r="I19" t="s">
         <v>86</v>
-      </c>
-      <c r="H19" t="s">
-        <v>86</v>
-      </c>
-      <c r="I19" t="s">
-        <v>87</v>
       </c>
       <c r="J19" t="str">
         <f>B19&amp;"."&amp;C19</f>
         <v>Patient.gender</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="W19" t="s">
-        <v>90</v>
-      </c>
-      <c r="X19" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="Y19" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W19"/>
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-patient-gender.html</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2794,46 +2802,43 @@
         <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D20" t="s">
-        <v>104</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
+      </c>
+      <c r="E20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="W20" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="X20" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y20" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-patient-given.html</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2841,45 +2846,50 @@
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D21" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>109</v>
+      <c r="E21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="F21" t="b">
         <v>1</v>
       </c>
       <c r="G21" t="s">
+        <v>85</v>
+      </c>
+      <c r="H21" t="s">
+        <v>85</v>
+      </c>
+      <c r="I21" t="s">
         <v>86</v>
-      </c>
-      <c r="H21" t="s">
-        <v>86</v>
-      </c>
-      <c r="I21" t="s">
-        <v>87</v>
       </c>
       <c r="J21" t="str">
         <f>B21&amp;"."&amp;C21</f>
         <v>Patient.identifier</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V21"/>
       <c r="W21" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+      <c r="Z21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-patient-identifier.html</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2892,46 +2902,49 @@
       <c r="D22" t="s">
         <v>20</v>
       </c>
-      <c r="E22" t="s">
-        <v>109</v>
+      <c r="E22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="F22" t="b">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I22" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J22" t="str">
         <f>B22&amp;"."&amp;C22</f>
         <v>Patient.name</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q22"/>
       <c r="V22" t="s">
-        <v>115</v>
-      </c>
-      <c r="W22" t="s">
-        <v>90</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="W22"/>
       <c r="X22" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Y22" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="Z22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-patient-name.html</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2939,46 +2952,42 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D23" t="s">
         <v>20</v>
       </c>
-      <c r="E23" t="s">
-        <v>84</v>
+      <c r="E23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaire</v>
       </c>
       <c r="F23" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G23" t="s">
+        <v>85</v>
+      </c>
+      <c r="H23" t="s">
+        <v>85</v>
+      </c>
+      <c r="I23" t="s">
         <v>86</v>
       </c>
-      <c r="H23" t="s">
-        <v>86</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>87</v>
       </c>
-      <c r="J23" t="s">
-        <v>88</v>
-      </c>
       <c r="K23" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="W23" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="X23" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y23" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="Z23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-questionnaire-_id.html</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2986,48 +2995,44 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D24" t="s">
-        <v>104</v>
-      </c>
-      <c r="E24" t="s">
-        <v>84</v>
+        <v>101</v>
+      </c>
+      <c r="E24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaire</v>
       </c>
       <c r="F24" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I24" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J24" t="str">
         <f>B24&amp;"."&amp;C24</f>
         <v>Questionnaire.context-type-value</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V24"/>
-      <c r="W24" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="X24" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y24" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-questionnaire-context-type-value.html</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3035,53 +3040,49 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D25" t="s">
         <v>20</v>
       </c>
-      <c r="E25" t="s">
-        <v>84</v>
+      <c r="E25" s="1" t="str">
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B25)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaire</v>
       </c>
       <c r="F25" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I25" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J25" t="str">
         <f>B25&amp;"."&amp;C25</f>
         <v>Questionnaire.publisher</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="V25" t="s">
-        <v>103</v>
-      </c>
-      <c r="W25" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="X25" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y25" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="Z25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-questionnaire-publisher.html</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3089,50 +3090,46 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D26" t="s">
         <v>20</v>
       </c>
-      <c r="E26" t="s">
-        <v>84</v>
+      <c r="E26" s="1" t="str">
+        <f t="shared" ref="E26:E34" si="2">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B26)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaire</v>
       </c>
       <c r="F26" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G26" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" t="s">
+        <v>85</v>
+      </c>
+      <c r="I26" t="s">
         <v>86</v>
-      </c>
-      <c r="H26" t="s">
-        <v>86</v>
-      </c>
-      <c r="I26" t="s">
-        <v>87</v>
       </c>
       <c r="J26" t="str">
         <f>B26&amp;"."&amp;C26</f>
         <v>Questionnaire.status</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="W26" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="X26" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y26" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+      <c r="Z26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-questionnaire-status.html</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3140,62 +3137,58 @@
         <v>24</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>84</v>
+      <c r="E27" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaire</v>
       </c>
       <c r="F27" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J27" s="1" t="str">
         <f>B27&amp;"."&amp;C27</f>
         <v>Questionnaire.title</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="V27" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="W27" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="X27" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y27" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="Z27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-questionnaire-title.html</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3203,47 +3196,43 @@
         <v>24</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>84</v>
+      <c r="E28" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaire</v>
       </c>
       <c r="F28" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J28" s="1" t="str">
         <f>B28&amp;"."&amp;C28</f>
         <v>Questionnaire.url</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="W28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="X28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y28" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="Z28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-questionnaire-url.html</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3251,130 +3240,355 @@
         <v>24</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>84</v>
+        <v>101</v>
+      </c>
+      <c r="E29" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaire</v>
       </c>
       <c r="F29" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="J29" s="1" t="str">
         <f>B29&amp;"."&amp;C29</f>
         <v>Questionnaire.version</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="W29" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="X29" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y29" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="Z29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-questionnaire-version.html</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>263</v>
-      </c>
       <c r="D30" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>244</v>
+        <v>101</v>
+      </c>
+      <c r="E30" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="F30" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J30" s="1" t="str">
         <f>B30&amp;"."&amp;C30</f>
         <v>Condition.onset-date</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="Y30" s="6"/>
-    </row>
-    <row r="31" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Z30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-condition-onset-date.html</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>244</v>
+        <v>101</v>
+      </c>
+      <c r="E31" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="F31" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="J31" s="1" t="str">
         <f>B31&amp;"."&amp;C31</f>
         <v>Condition.code</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="W31" s="6"/>
       <c r="X31" s="6"/>
       <c r="Y31" s="6"/>
+      <c r="Z31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-condition-code.html</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
+      </c>
+      <c r="F32" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J32" s="1" t="str">
+        <f>B32&amp;"."&amp;C32</f>
+        <v>Immunization.patient</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="V32" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="W32" s="1" t="str">
+        <f>"support searching for all "&amp;LOWER(B32)&amp;"s for a patient"</f>
+        <v>support searching for all immunizations for a patient</v>
+      </c>
+      <c r="X32" s="6" t="str">
+        <f>"GET [base]/"&amp;B32&amp;"?patient=1137192"</f>
+        <v>GET [base]/Immunization?patient=1137192</v>
+      </c>
+      <c r="Y32" s="6" t="str">
+        <f>"Fetches a bundle of all "&amp;B32&amp; " resources for the specified patient"</f>
+        <v>Fetches a bundle of all Immunization resources for the specified patient</v>
+      </c>
+      <c r="Z32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-immunization-patient.html</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
+      </c>
+      <c r="F33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J33" s="1" t="str">
+        <f>B33&amp;"."&amp;C33</f>
+        <v>Immunization.status</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="V33" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="W33" s="6"/>
+      <c r="X33" s="6"/>
+      <c r="Y33" s="6"/>
+      <c r="Z33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-immunization-status.html</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
+      </c>
+      <c r="F34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J34" s="1" t="str">
+        <f>B34&amp;"."&amp;C34</f>
+        <v>Immunization.date</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="V34" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y34" s="6"/>
+      <c r="Z34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SearchParameter-us-core-immunization-date.html</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="1" t="str">
+        <f t="shared" ref="E35" si="3">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B35)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example patient search</v>
+      </c>
+      <c r="F35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J35" s="1" t="str">
+        <f>B35&amp;"."&amp;C35</f>
+        <v>!EXAMPLE PATIENT SEARCH.patient</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="W35" s="1" t="str">
+        <f>"support searching for all "&amp;LOWER(B35)&amp;"s for a patient"</f>
+        <v>support searching for all !example patient searchs for a patient</v>
+      </c>
+      <c r="X35" s="6" t="str">
+        <f>"GET [base]/"&amp;B35&amp;"?patient=1137192"</f>
+        <v>GET [base]/!EXAMPLE PATIENT SEARCH?patient=1137192</v>
+      </c>
+      <c r="Y35" s="6" t="str">
+        <f>"Fetches a bundle of all "&amp;B35&amp; " resources for the specified patient"</f>
+        <v>Fetches a bundle of all !EXAMPLE PATIENT SEARCH resources for the specified patient</v>
+      </c>
+      <c r="Z35" s="1" t="str">
+        <f t="shared" ref="Z35" si="4">"SearchParameter-us-core-"&amp;LOWER((B35)&amp;"-"&amp;C35&amp;".html")</f>
+        <v>SearchParameter-us-core-!example patient search-patient.html</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y29">
@@ -3387,10 +3601,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A29" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3407,19 +3621,19 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>4</v>
@@ -3439,13 +3653,13 @@
         <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -3453,16 +3667,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="C3" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E3" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -3470,16 +3684,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="C4" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E4" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -3487,16 +3701,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E5" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -3507,13 +3721,13 @@
         <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E6" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -3521,16 +3735,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="C7" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="D7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E7" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -3538,16 +3752,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="C8" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="D8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E8" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -3555,16 +3769,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="C9" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="D9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E9" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -3574,16 +3788,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="C10" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="D10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -3593,16 +3807,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="D11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F11" s="6"/>
     </row>
@@ -3611,16 +3825,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H12" s="6"/>
     </row>
@@ -3632,13 +3846,13 @@
         <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -3646,16 +3860,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="C14" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="D14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E14" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="H14" s="6"/>
     </row>
@@ -3664,16 +3878,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="C15" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="D15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E15" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -3684,13 +3898,13 @@
         <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="D16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E16" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="H16" s="6"/>
     </row>
@@ -3699,16 +3913,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="C17" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="D17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E17" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -3721,13 +3935,13 @@
         <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="D18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E18" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="H18" s="6"/>
     </row>
@@ -3736,16 +3950,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="C19" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="D19" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -3755,16 +3969,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="C20" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="D20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E20" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -3774,16 +3988,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="C21" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="D21" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E21" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="H21" s="6"/>
     </row>
@@ -3792,16 +4006,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="C22" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="D22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E22" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="F22" s="6"/>
     </row>
@@ -3810,16 +4024,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="C23" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="D23" t="s">
         <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -3830,16 +4044,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="C24" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="D24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E24" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
@@ -3850,16 +4064,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="C25" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="D25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E25" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -3870,16 +4084,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="C26" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="D26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E26" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -3887,16 +4101,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="C27" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="D27" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -3904,16 +4118,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="C28" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="D28" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E28" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -3924,13 +4138,13 @@
         <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="D29" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E29" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -3941,13 +4155,13 @@
         <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="D30" t="s">
         <v>20</v>
       </c>
       <c r="E30" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -3958,13 +4172,13 @@
         <v>45</v>
       </c>
       <c r="C31" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="D31" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E31" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -3975,13 +4189,13 @@
         <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="D32" t="s">
         <v>20</v>
       </c>
       <c r="E32" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="18" x14ac:dyDescent="0.2">
@@ -3989,25 +4203,25 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>251</v>
+        <v>245</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -4015,25 +4229,25 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -4041,25 +4255,25 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4067,25 +4281,25 @@
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>269</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -4096,22 +4310,81 @@
         <v>43</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>270</v>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="H39" s="6" t="str">
+        <f>"Fetches a bundle of all "&amp;B38&amp;" resources for the specified "&amp;SUBSTITUTE(C38,","," and ")</f>
+        <v>Fetches a bundle of all Immunization resources for the specified patient and date</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H40" s="6" t="str">
+        <f>"Fetches a bundle of all "&amp;B39&amp;" resources for the specified "&amp;SUBSTITUTE(C39,","," and ")</f>
+        <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
       </c>
     </row>
   </sheetData>
@@ -4126,19 +4399,22 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="37.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="8" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -4149,13 +4425,13 @@
         <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -4166,13 +4442,13 @@
         <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E3" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -4183,13 +4459,13 @@
         <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E4" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -4200,13 +4476,13 @@
         <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E5" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -4217,13 +4493,13 @@
         <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E6" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -4234,13 +4510,13 @@
         <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="D7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E7" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -4251,13 +4527,13 @@
         <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="D8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E8" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -4268,13 +4544,13 @@
         <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="D9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E9" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -4285,13 +4561,13 @@
         <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="D10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E10" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -4302,13 +4578,13 @@
         <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="D11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E11" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -4319,13 +4595,13 @@
         <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="D12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E12" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -4336,13 +4612,13 @@
         <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -4353,13 +4629,13 @@
         <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="D14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E14" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -4370,13 +4646,13 @@
         <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="D15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E15" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -4387,13 +4663,13 @@
         <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="D16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E16" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -4404,13 +4680,13 @@
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="D17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E17" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -4421,13 +4697,13 @@
         <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="D18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E18" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -4438,13 +4714,13 @@
         <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="D19" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E19" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -4455,13 +4731,13 @@
         <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="D20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E20" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -4472,13 +4748,13 @@
         <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="D21" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E21" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -4489,13 +4765,13 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="D22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E22" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -4506,13 +4782,13 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="D23" t="s">
         <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -4523,13 +4799,13 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="D24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E24" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -4540,13 +4816,13 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="D25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E25" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -4557,13 +4833,13 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="D26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E26" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -4574,13 +4850,13 @@
         <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="D27" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E27" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -4591,13 +4867,13 @@
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="D28" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E28" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -4608,13 +4884,13 @@
         <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="D29" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E29" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -4625,13 +4901,13 @@
         <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="D30" t="s">
         <v>20</v>
       </c>
       <c r="E30" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -4642,13 +4918,13 @@
         <v>45</v>
       </c>
       <c r="C31" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="D31" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E31" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -4659,13 +4935,13 @@
         <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="D32" t="s">
         <v>20</v>
       </c>
       <c r="E32" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final edits to SP maker
</commit_message>
<xml_diff>
--- a/SP/uscore-server.xlsx
+++ b/SP/uscore-server.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Python\MyNotebooks\SP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3518B7-490D-46C1-A237-B83FA9804FB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B18A705-5D66-48E9-AE9D-1F2BA8031329}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-68805" yWindow="-10800" windowWidth="68805" windowHeight="28800" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="466">
   <si>
     <t>Element</t>
   </si>
@@ -746,15 +746,9 @@
     <t>patient,clinical-status</t>
   </si>
   <si>
-    <t>Fetches a bundle of all Condition resources for the specified patient and all “active” statuses (active,relapse,remission). This will not return any “entered in error” resources because of the conditional presence of the clinicalStatus element.</t>
-  </si>
-  <si>
     <t>patient,category</t>
   </si>
   <si>
-    <t>GET [base]/Condition?patient=1032702&amp;category=problem,GET [base]/Condition?patient=1032702&amp;category=health-concern,GET [base]/Condition?patient=1032702&amp;category=encounter-diagnosis</t>
-  </si>
-  <si>
     <t>Fetches a bundle of all Condition resources for the specified patient and category.</t>
   </si>
   <si>
@@ -788,18 +782,9 @@
     <t>support searching for all *active* conditions for a patient</t>
   </si>
   <si>
-    <t>GET [base/Condition?patient=[id]&amp;clinical-status=active,recurrance,remission</t>
-  </si>
-  <si>
-    <t>GET [base]/AllergyIntolerance?patient=[id]&amp;clinical-status=active</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fetches a bundle of all Condition resources for the specified patient and date. </t>
   </si>
   <si>
-    <t>Fetches a bundle of all Condition resources for the specified patient and status code.  This will not return any “entered in error” resources because of the conditional presence of the clinicalStatus element.</t>
-  </si>
-  <si>
     <t>!Encounter</t>
   </si>
   <si>
@@ -818,9 +803,6 @@
     <t>support searching for all *active*  or *inactive* allergies for a patient</t>
   </si>
   <si>
-    <t>GET [base]/Condition?patient=[id]&amp;code=[system\|code]</t>
-  </si>
-  <si>
     <t>GET [base]/Immunization?patient=1137192&amp;status=completed</t>
   </si>
   <si>
@@ -983,9 +965,6 @@
     <t>MedicationRequest:medication</t>
   </si>
   <si>
-    <t>GET [base]/MedicationRequest?patient=14676,GET [base]/MedicationRequest?patient=14676&amp;_include=MedicationRequest:medication</t>
-  </si>
-  <si>
     <t>support searching a patient based on text address</t>
   </si>
   <si>
@@ -1007,9 +986,6 @@
     <t>support searching for all medication statements for a patient. The server application represents the medication using either an inline code or a contained or external reference to the Medication resource.</t>
   </si>
   <si>
-    <t>GET [base]/MedicationStatement?patient=14676,GET [base]/MedicationStatement?patient=14676&amp;_include=MedicationStatement:medication</t>
-  </si>
-  <si>
     <t>GET [base]/Procedure?patient=1291938</t>
   </si>
   <si>
@@ -1025,9 +1001,6 @@
     <t>GET [base]/Observation?patient=1134281&amp;category=http://hl7.org/fhir/observation-category\|laboratory</t>
   </si>
   <si>
-    <t>GET [base]/Observation?patient=1134281&amp;code=http://loinc.org\|2339-0,GET [base]/Observation?patient=1134281&amp;code=http://loinc.org\|2339-0,http://loinc.org\|25428-4,2514-8</t>
-  </si>
-  <si>
     <t>GET [base]Observation?patient=555580&amp;category=http://hl7.org/fhir/observation-category\|laboratory&amp;date=ge2018-03-14</t>
   </si>
   <si>
@@ -1235,12 +1208,6 @@
     <t>support searching for a practitioner by a string match of any part of name</t>
   </si>
   <si>
-    <t>support searching a practiitioner by an identifier such as an NPI</t>
-  </si>
-  <si>
-    <t>GET [base]/Practitioner?identifier=http://hl7.org/fhir/sid/us-npi%7C1497860456</t>
-  </si>
-  <si>
     <t>GET [base]/Practitioner?name=Smith</t>
   </si>
   <si>
@@ -1250,12 +1217,6 @@
     <t>specialty</t>
   </si>
   <si>
-    <t>support searching practiitioner role by specialty</t>
-  </si>
-  <si>
-    <t>GET [base]/PractitionerRole?specialty=http://hl7.org/fhir/practitioner-specialty%7Ccardio</t>
-  </si>
-  <si>
     <t>practitioner</t>
   </si>
   <si>
@@ -1268,9 +1229,6 @@
     <t>support searching practitioner role by practitioner name and identifier using chained parameters</t>
   </si>
   <si>
-    <t>GET [base]/PractitionerRole?practitioner.identifier=http://hl7.org/fhir/sid/us-npi%7C14|97860456&amp;_include=PractitionerRole:practitioner&amp;_include=PractitionerRole?endpoint,GET [base]/PractitionerRole?practitioner.name=Henry&amp;_include=PractitionerRole:practitioner&amp;_include=PractitionerRole?endpoint</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-smokingstatus</t>
   </si>
   <si>
@@ -1322,18 +1280,6 @@
     <t>support fetching a DocumentReference</t>
   </si>
   <si>
-    <t>GET [base]/Patient/1032702,GET [base]/Patient?_id=1032702</t>
-  </si>
-  <si>
-    <t>GET [base]/DocumentReference/2169591,GET [base]/DocumentReference?_id=2169591</t>
-  </si>
-  <si>
-    <t>GET [base]/Encounter/12354,GET [base]/Encounter?_id=12354</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>Fetches a single DocumentReference. The document itself is represented as a base64 encoded binary data element or retrieved using the link provided by the resource. If the document is a  relative link to a [Binary] resource like a resource reference, it can be subsequently retrieved using: `GET [base]/Binary/[id]`.</t>
   </si>
   <si>
@@ -1418,33 +1364,12 @@
     <t>support searching for all encounter for a patient by status (for example, all finished encounters)</t>
   </si>
   <si>
-    <t>clinical-status=active,recurrance,remission</t>
-  </si>
-  <si>
-    <t>category=http://terminology.hl7.org/CodeSystem/v2-0074\|LAB</t>
-  </si>
-  <si>
     <t>status=active</t>
   </si>
   <si>
     <t>support searching for all administered immunizations for a patient</t>
   </si>
   <si>
-    <t>category=http://hl7.org/fhir/observation-category\|laboratory</t>
-  </si>
-  <si>
-    <t>category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan</t>
-  </si>
-  <si>
-    <t>code=http://loinc.org\|72166-2</t>
-  </si>
-  <si>
-    <t>category=http://hl7.org/fhir/observation-category\|vital-signs</t>
-  </si>
-  <si>
-    <t>category=http://hl7.org/fhir/us/core/CodeSystem/us-core-documentreference-category\|clinical-note</t>
-  </si>
-  <si>
     <t>lifecycle-status</t>
   </si>
   <si>
@@ -1476,6 +1401,81 @@
   </si>
   <si>
     <t>!Observation</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all Observation resources for the specified patient and category = `laboratory` and status</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all Condition resources for the specified patient and all "active" statuses (active,relapse,remission). This will not return any "entered in error" resources because of the conditional presence of the clinicalStatus element.</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all Condition resources for the specified patient and status code.  This will not return any "entered in error" resources because of the conditional presence of the clinicalStatus element.</t>
+  </si>
+  <si>
+    <t>support searching a practitioner by an identifier such as an NPI</t>
+  </si>
+  <si>
+    <t>support searching practitioner role by specialty</t>
+  </si>
+  <si>
+    <t>GET [base]/AllergyIntolerance?patient=[id]&amp;clinical-status=http://terminology.hl7.org/CodeSystem/allergyintolerance-clinical\|active</t>
+  </si>
+  <si>
+    <t>category=http://terminology.hl7.org/CodeSystem/v2-0074|LAB</t>
+  </si>
+  <si>
+    <t>category=http://hl7.org/fhir/observation-category|laboratory</t>
+  </si>
+  <si>
+    <t>category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category|assess-plan</t>
+  </si>
+  <si>
+    <t>code=http://loinc.org|72166-2</t>
+  </si>
+  <si>
+    <t>category=http://hl7.org/fhir/observation-category|vital-signs</t>
+  </si>
+  <si>
+    <t>category=http://hl7.org/fhir/us/core/CodeSystem/us-core-documentreference-category|clinical-note</t>
+  </si>
+  <si>
+    <t>clinical-status=http://terminology.hl7.org/CodeSystem/condition-clinical|active,http://terminology.hl7.org/CodeSystem/condition-clinical|recurrance,http://terminology.hl7.org/CodeSystem/condition-clinical|remission</t>
+  </si>
+  <si>
+    <t>GET [base/Condition?patient=1032702&amp;clinical-status=http://terminology.hl7.org/CodeSystem/condition-clinical\|active,http://terminology.hl7.org/CodeSystem/condition-clinical\|recurrance,http://terminology.hl7.org/CodeSystem/condition-clinical\|remission</t>
+  </si>
+  <si>
+    <t>GET [base]/Condition?patient=1032702&amp;code=[http://snomed.info/sct\|442311008]</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1134281&amp;code=http://loinc.org\|2339-0~GET [base]/Observation?patient=1134281&amp;code=http://loinc.org\|2339-0,http://loinc.org\|25428-4,2514-8</t>
+  </si>
+  <si>
+    <t>GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|problem~GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|health-concern~GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|encounter-diagnosis</t>
+  </si>
+  <si>
+    <t>GET [base]/Encounter/12354~GET [base]/Encounter?_id=12354</t>
+  </si>
+  <si>
+    <t>GET [base]/Patient/1032702~GET [base]/Patient?_id=1032702</t>
+  </si>
+  <si>
+    <t>GET [base]/DocumentReference/2169591~GET [base]/DocumentReference?_id=2169591</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationRequest?patient=14676~GET [base]/MedicationRequest?patient=14676&amp;_include=MedicationRequest:medication</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationStatement?patient=14676~GET [base]/MedicationStatement?patient=14676&amp;_include=MedicationStatement:medication</t>
+  </si>
+  <si>
+    <t>GET [base]/PractitionerRole?practitioner.identifier=http://hl7.org/fhir/sid/us-npi\|97860456&amp;_include=PractitionerRole:practitioner&amp;_include=PractitionerRole?endpoint~GET [base]/PractitionerRole?practitioner.name=Henry&amp;_include=PractitionerRole:practitioner&amp;_include=PractitionerRole?endpoint</t>
+  </si>
+  <si>
+    <t>GET [base]/PractitionerRole?specialty=http://nucc.org/provider-taxonomy\|208D0000X</t>
+  </si>
+  <si>
+    <t>GET [base]/Practitioner?identifier=http://hl7.org/fhir/sid/us-npi\|97860456</t>
   </si>
 </sst>
 </file>
@@ -2449,10 +2449,10 @@
   <dimension ref="A1:AB92"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="Z82" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="Z94" sqref="Z94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2544,10 +2544,10 @@
         <v>79</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>462</v>
+        <v>437</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>463</v>
+        <v>438</v>
       </c>
       <c r="W1" s="5" t="s">
         <v>80</v>
@@ -2565,7 +2565,7 @@
         <v>83</v>
       </c>
       <c r="AB1" s="10" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="1" customFormat="1" ht="15.75" thickTop="1">
@@ -2573,7 +2573,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>217</v>
@@ -2623,7 +2623,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>51</v>
@@ -2670,7 +2670,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>111</v>
@@ -2724,7 +2724,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>122</v>
@@ -2783,7 +2783,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>91</v>
@@ -2867,7 +2867,7 @@
         <v>85</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="Z7" s="6" t="s">
         <v>119</v>
@@ -2917,7 +2917,7 @@
         <v>85</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="Z8" s="1" t="s">
         <v>121</v>
@@ -3230,13 +3230,13 @@
         <v>85</v>
       </c>
       <c r="Y14" s="6" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="Z14" s="6" t="s">
-        <v>416</v>
+        <v>458</v>
       </c>
       <c r="AA14" s="3" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="AB14" s="1" t="str">
         <f t="shared" si="8"/>
@@ -3387,10 +3387,10 @@
         <v>85</v>
       </c>
       <c r="Y17" s="6" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="Z17" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="AA17" s="14" t="str">
         <f>"Fetches a bundle containing any "&amp;B17&amp;" resources matching the identifier"</f>
@@ -3600,10 +3600,7 @@
         <v>107</v>
       </c>
       <c r="Z21" s="6" t="s">
-        <v>414</v>
-      </c>
-      <c r="AA21" s="3" t="s">
-        <v>417</v>
+        <v>459</v>
       </c>
       <c r="AB21" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B21)&amp;"-"&amp;SUBSTITUTE(C21,"_","")&amp;".html")</f>
@@ -3839,10 +3836,10 @@
       </c>
       <c r="X26"/>
       <c r="Y26" s="6" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="Z26" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="AA26" s="14" t="str">
         <f>"Fetches a bundle containing any "&amp;B26&amp;" resources matching the identifier"</f>
@@ -3897,10 +3894,10 @@
         <v>109</v>
       </c>
       <c r="Y27" s="6" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="Z27" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AA27" s="14" t="str">
         <f>"Fetches a bundle of all "&amp;B27&amp;" resources matching the name"</f>
@@ -4254,7 +4251,7 @@
         <v>215</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>101</v>
@@ -4349,7 +4346,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>122</v>
@@ -4408,7 +4405,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>91</v>
@@ -4458,7 +4455,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>111</v>
@@ -4512,7 +4509,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>84</v>
@@ -4547,13 +4544,13 @@
         <v>85</v>
       </c>
       <c r="Y40" s="6" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
       <c r="Z40" s="6" t="s">
-        <v>415</v>
+        <v>460</v>
       </c>
       <c r="AA40" s="3" t="s">
-        <v>418</v>
+        <v>400</v>
       </c>
       <c r="AB40" s="1" t="str">
         <f t="shared" ref="AB40" si="13">"SearchParameter-us-core-"&amp;LOWER((B40)&amp;"-"&amp;C40&amp;".html")</f>
@@ -4565,7 +4562,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>91</v>
@@ -4615,7 +4612,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>122</v>
@@ -4674,7 +4671,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>217</v>
@@ -4724,7 +4721,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>31</v>
@@ -4771,7 +4768,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>111</v>
@@ -4825,10 +4822,10 @@
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>101</v>
@@ -4850,7 +4847,7 @@
         <v>111</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>419</v>
+        <v>401</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>85</v>
@@ -4878,7 +4875,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>91</v>
@@ -4928,7 +4925,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>122</v>
@@ -4987,7 +4984,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>217</v>
@@ -5037,7 +5034,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>51</v>
@@ -5087,7 +5084,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>111</v>
@@ -5141,10 +5138,10 @@
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>455</v>
+        <v>430</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>101</v>
@@ -5191,7 +5188,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>122</v>
@@ -5250,10 +5247,10 @@
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>456</v>
+        <v>431</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>101</v>
@@ -5304,7 +5301,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>91</v>
@@ -5354,7 +5351,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>122</v>
@@ -5388,18 +5385,18 @@
       <c r="M56" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="U56" s="9" t="s">
-        <v>300</v>
-      </c>
-      <c r="V56" s="9"/>
+      <c r="U56" s="9"/>
+      <c r="V56" s="9" t="s">
+        <v>294</v>
+      </c>
       <c r="X56" s="1" t="s">
         <v>124</v>
       </c>
       <c r="Y56" s="1" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="Z56" s="14" t="s">
-        <v>301</v>
+        <v>461</v>
       </c>
       <c r="AA56" s="14" t="str">
         <f>"Fetches a bundle of all "&amp;B56&amp; " resources for the specified patient. Mandatory for client to support the _include parameter. Optional for server to support the _include parameter."</f>
@@ -5415,10 +5412,10 @@
         <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>101</v>
@@ -5469,7 +5466,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>91</v>
@@ -5519,7 +5516,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>122</v>
@@ -5553,14 +5550,17 @@
       <c r="M59" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="V59" s="9" t="s">
+        <v>294</v>
+      </c>
       <c r="X59" s="1" t="s">
         <v>124</v>
       </c>
       <c r="Y59" s="1" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="Z59" s="14" t="s">
-        <v>309</v>
+        <v>462</v>
       </c>
       <c r="AA59" s="14" t="str">
         <f>"Fetches a bundle of all "&amp;B59&amp; " resources for the specified patient. Mandatory for client to support the _include parameter. Optional for server to support the _include parameter."</f>
@@ -5576,10 +5576,10 @@
         <v>58</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>101</v>
@@ -5630,7 +5630,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>91</v>
@@ -5680,7 +5680,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>122</v>
@@ -5722,7 +5722,7 @@
         <v>support searching for all procedures for a patient</v>
       </c>
       <c r="Z62" s="6" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="AA62" s="14" t="str">
         <f>"Fetches a bundle of all "&amp;B62&amp; " resources for the specified patient"</f>
@@ -5738,7 +5738,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>111</v>
@@ -5792,7 +5792,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>51</v>
@@ -5842,7 +5842,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>91</v>
@@ -5892,7 +5892,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>217</v>
@@ -5942,7 +5942,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>51</v>
@@ -5992,7 +5992,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>111</v>
@@ -6046,7 +6046,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>122</v>
@@ -6105,7 +6105,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>217</v>
@@ -6155,7 +6155,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>458</v>
+        <v>433</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>51</v>
@@ -6202,7 +6202,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>111</v>
@@ -6256,7 +6256,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>122</v>
@@ -6315,7 +6315,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>91</v>
@@ -6365,7 +6365,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>122</v>
@@ -6424,7 +6424,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>91</v>
@@ -6474,7 +6474,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>122</v>
@@ -6533,7 +6533,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>48</v>
@@ -6568,10 +6568,10 @@
         <v>85</v>
       </c>
       <c r="Y78" s="1" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="Z78" s="9" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="AA78" s="14" t="str">
         <f>"Fetches a bundle of all "&amp;B78&amp; " resources that match the name"</f>
@@ -6587,7 +6587,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>118</v>
@@ -6622,10 +6622,10 @@
         <v>85</v>
       </c>
       <c r="Y79" s="1" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="Z79" s="9" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="AA79" s="14" t="str">
         <f>"Fetches a bundle of all "&amp;B79&amp; " resources that match the address string"</f>
@@ -6641,10 +6641,10 @@
         <v>78</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>101</v>
@@ -6676,10 +6676,10 @@
         <v>85</v>
       </c>
       <c r="Y80" s="1" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="Z80" s="9" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="AA80" s="14" t="str">
         <f>"Fetches a bundle of all "&amp;B80&amp; " resources for the city"</f>
@@ -6695,10 +6695,10 @@
         <v>79</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>459</v>
+        <v>434</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>101</v>
@@ -6730,10 +6730,10 @@
         <v>85</v>
       </c>
       <c r="Y81" s="1" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="Z81" s="9" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="AA81" s="14" t="str">
         <f>"Fetches a bundle of all "&amp;B81&amp; " resources for the state"</f>
@@ -6749,10 +6749,10 @@
         <v>80</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>101</v>
@@ -6784,10 +6784,10 @@
         <v>85</v>
       </c>
       <c r="Y82" s="1" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="Z82" s="9" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="AA82" s="14" t="str">
         <f>"Fetches a bundle of all "&amp;B82&amp; " resources for the ZIP code"</f>
@@ -6803,7 +6803,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>48</v>
@@ -6838,10 +6838,10 @@
         <v>85</v>
       </c>
       <c r="Y83" s="1" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="Z83" s="9" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="AA83" s="14" t="str">
         <f>"Fetches a bundle of all "&amp;B83&amp; " resources that match the name"</f>
@@ -6857,7 +6857,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>118</v>
@@ -6892,10 +6892,10 @@
         <v>85</v>
       </c>
       <c r="Y84" s="1" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="Z84" s="9" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="AA84" s="14" t="str">
         <f>"Fetches a bundle of all "&amp;B84&amp; " resources that match the address string"</f>
@@ -6911,10 +6911,10 @@
         <v>83</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>101</v>
@@ -6946,10 +6946,10 @@
         <v>85</v>
       </c>
       <c r="Y85" s="1" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="Z85" s="9" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="AA85" s="14" t="str">
         <f>"Fetches a bundle of all "&amp;B85&amp; " resources for the city"</f>
@@ -6965,10 +6965,10 @@
         <v>84</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>101</v>
@@ -7000,10 +7000,10 @@
         <v>85</v>
       </c>
       <c r="Y86" s="1" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="Z86" s="9" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="AA86" s="14" t="str">
         <f>"Fetches a bundle of all "&amp;B86&amp; " resources for the state"</f>
@@ -7019,10 +7019,10 @@
         <v>85</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>101</v>
@@ -7054,10 +7054,10 @@
         <v>85</v>
       </c>
       <c r="Y87" s="1" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="Z87" s="9" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="AA87" s="14" t="str">
         <f>"Fetches a bundle of all "&amp;B87&amp; " resources for the ZIP code"</f>
@@ -7073,7 +7073,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>48</v>
@@ -7111,10 +7111,10 @@
         <v>109</v>
       </c>
       <c r="Y88" s="6" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="Z88" s="9" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="AA88" s="14" t="str">
         <f>"Fetches a bundle of all "&amp;B88&amp;" resources matching the name"</f>
@@ -7130,7 +7130,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>108</v>
@@ -7165,10 +7165,10 @@
         <v>85</v>
       </c>
       <c r="Y89" s="6" t="s">
-        <v>385</v>
+        <v>444</v>
       </c>
       <c r="Z89" s="9" t="s">
-        <v>386</v>
+        <v>465</v>
       </c>
       <c r="AA89" s="14" t="str">
         <f>"Fetches a bundle containing any "&amp;B89&amp;" resources matching the identifier"</f>
@@ -7184,10 +7184,10 @@
         <v>88</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>20</v>
@@ -7218,11 +7218,14 @@
       <c r="M90" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="V90" s="1" t="s">
+        <v>381</v>
+      </c>
       <c r="Y90" s="6" t="s">
-        <v>390</v>
+        <v>445</v>
       </c>
       <c r="Z90" s="9" t="s">
-        <v>391</v>
+        <v>464</v>
       </c>
       <c r="AA90" s="14" t="str">
         <f>"Fetches a bundle containing  "&amp;B90&amp;" resources matching the specialty"</f>
@@ -7238,10 +7241,10 @@
         <v>89</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>20</v>
@@ -7273,16 +7276,16 @@
         <v>85</v>
       </c>
       <c r="S91" s="1" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="V91" s="1" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="Y91" s="6" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="Z91" s="9" t="s">
-        <v>396</v>
+        <v>463</v>
       </c>
       <c r="AA91" s="14" t="str">
         <f>"Fetches a bundle containing  "&amp;B91&amp;" resources matching the chained parameter practitioner.name or practitioner.identifier. SHOULD support the _include for PractionerRole.practitioner and PractitionerRole.endpoint."</f>
@@ -7311,8 +7314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C69" sqref="C68:C69"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -7325,7 +7328,7 @@
     <col min="6" max="6" width="27" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" customWidth="1"/>
     <col min="8" max="8" width="84.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="57.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="68.28515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="83.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7349,7 +7352,7 @@
         <v>131</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>436</v>
+        <v>418</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>4</v>
@@ -7366,7 +7369,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C2" s="1" t="str">
         <f t="shared" ref="C2:C5" si="0">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
@@ -7391,7 +7394,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C3" s="1" t="str">
         <f t="shared" si="0"/>
@@ -7416,7 +7419,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -7441,7 +7444,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -7482,10 +7485,10 @@
         <v>139</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>440</v>
+        <v>422</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>441</v>
+        <v>423</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="1"/>
@@ -7497,7 +7500,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" ref="C7:C58" si="2">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B7)</f>
@@ -7522,7 +7525,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C8" s="1" t="str">
         <f t="shared" si="2"/>
@@ -7547,7 +7550,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C9" s="1" t="str">
         <f t="shared" si="2"/>
@@ -7573,7 +7576,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C10" s="1" t="str">
         <f t="shared" si="2"/>
@@ -7600,7 +7603,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C11" s="1" t="str">
         <f t="shared" si="2"/>
@@ -7626,7 +7629,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C12" s="1" t="str">
         <f t="shared" si="2"/>
@@ -7667,10 +7670,10 @@
         <v>146</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>438</v>
+        <v>420</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>442</v>
+        <v>424</v>
       </c>
       <c r="J13" s="6" t="str">
         <f t="shared" si="1"/>
@@ -7682,7 +7685,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C14" s="1" t="str">
         <f t="shared" si="2"/>
@@ -7707,7 +7710,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C15" s="1" t="str">
         <f t="shared" si="2"/>
@@ -7748,10 +7751,10 @@
         <v>139</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>439</v>
+        <v>421</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>443</v>
+        <v>425</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="1"/>
@@ -7763,7 +7766,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -7805,10 +7808,10 @@
         <v>139</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>445</v>
+        <v>427</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>444</v>
+        <v>426</v>
       </c>
       <c r="J18" s="6" t="str">
         <f t="shared" si="1"/>
@@ -7820,7 +7823,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C19" s="1" t="str">
         <f t="shared" si="2"/>
@@ -7847,7 +7850,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C20" s="1" t="str">
         <f t="shared" si="2"/>
@@ -7873,7 +7876,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C21" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B21)</f>
@@ -7898,7 +7901,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C22" s="1" t="str">
         <f t="shared" si="2"/>
@@ -7924,7 +7927,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C23" s="1" t="str">
         <f t="shared" si="2"/>
@@ -7951,7 +7954,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C24" s="1" t="str">
         <f t="shared" si="2"/>
@@ -7978,7 +7981,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C25" s="1" t="str">
         <f t="shared" si="2"/>
@@ -8005,7 +8008,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C26" s="1" t="str">
         <f t="shared" si="2"/>
@@ -8030,7 +8033,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C27" s="1" t="str">
         <f t="shared" si="2"/>
@@ -8055,7 +8058,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C28" s="1" t="str">
         <f t="shared" si="2"/>
@@ -8096,10 +8099,10 @@
         <v>167</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="J29" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B29&amp;" resources matching the specified "&amp;SUBSTITUTE(D29,","," and ")</f>
@@ -8127,10 +8130,10 @@
         <v>167</v>
       </c>
       <c r="H30" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="I30" s="6" t="s">
         <v>254</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>260</v>
       </c>
       <c r="J30" s="6" t="str">
         <f t="shared" ref="J30:J32" si="3">"Fetches a bundle of all "&amp;B30&amp;" resources matching the specified "&amp;SUBSTITUTE(D30,","," and ")</f>
@@ -8158,10 +8161,10 @@
         <v>160</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="J31" s="6" t="str">
         <f t="shared" si="3"/>
@@ -8189,10 +8192,10 @@
         <v>160</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="J32" s="6" t="str">
         <f t="shared" si="3"/>
@@ -8220,16 +8223,16 @@
         <v>139</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>446</v>
+        <v>453</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>236</v>
+        <v>454</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>222</v>
+        <v>442</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -8244,7 +8247,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>101</v>
@@ -8253,13 +8256,13 @@
         <v>139</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>224</v>
+        <v>457</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -8274,7 +8277,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>101</v>
@@ -8283,13 +8286,13 @@
         <v>139</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>246</v>
+        <v>455</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="1" customFormat="1">
@@ -8304,22 +8307,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -8343,13 +8346,13 @@
         <v>139</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>237</v>
+        <v>446</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>239</v>
+        <v>443</v>
       </c>
     </row>
     <row r="38" spans="1:10" s="1" customFormat="1">
@@ -8357,14 +8360,14 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C38" s="1" t="str">
         <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>101</v>
@@ -8373,10 +8376,10 @@
         <v>146</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="J38" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B38&amp;" resources for the specified "&amp;SUBSTITUTE(D38,","," and ")</f>
@@ -8388,7 +8391,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C39" s="1" t="str">
         <f t="shared" si="2"/>
@@ -8401,13 +8404,13 @@
         <v>101</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>449</v>
+        <v>429</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="J39" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B39&amp;" resources for the specified "&amp;SUBSTITUTE(D39,","," and ")</f>
@@ -8419,10 +8422,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>149</v>
@@ -8434,10 +8437,10 @@
         <v>139</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="J40" s="6" t="str">
         <f t="shared" ref="J40:J59" si="4">"Fetches a bundle of all "&amp;B40&amp;" resources for the specified "&amp;SUBSTITUTE(D40,","," and ")</f>
@@ -8449,13 +8452,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>20</v>
@@ -8467,10 +8470,10 @@
         <v>447</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="J41" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B41&amp;" resources for the specified patient and  a category code = `LAB`"</f>
@@ -8482,13 +8485,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>20</v>
@@ -8497,10 +8500,10 @@
         <v>139</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="J42" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B42&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -8512,28 +8515,28 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>447</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="I43" s="11" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="J43" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B43&amp;" resources for the specified patient and date and a category code = `LAB`"</f>
@@ -8545,25 +8548,25 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="H44" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>326</v>
-      </c>
       <c r="I44" s="6" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="J44" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B44&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -8575,10 +8578,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>149</v>
@@ -8590,10 +8593,10 @@
         <v>139</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="J45" s="6" t="str">
         <f t="shared" ref="J45" si="5">"Fetches a bundle of all "&amp;B45&amp;" resources for the specified "&amp;SUBSTITUTE(D45,","," and ")</f>
@@ -8605,13 +8608,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>20</v>
@@ -8620,10 +8623,10 @@
         <v>139</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="J46" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified patient and  a category code specified in US Core DiagnosticReport Category Codes"</f>
@@ -8635,13 +8638,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>20</v>
@@ -8650,10 +8653,10 @@
         <v>139</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="J47" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B47&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -8665,25 +8668,25 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="J48" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B48&amp;" resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes"</f>
@@ -8695,25 +8698,25 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="J49" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B49&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -8725,14 +8728,14 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C50" s="1" t="str">
         <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>460</v>
+        <v>435</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>101</v>
@@ -8741,10 +8744,10 @@
         <v>139</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>461</v>
+        <v>436</v>
       </c>
       <c r="J50" s="6" t="str">
         <f t="shared" si="4"/>
@@ -8756,26 +8759,26 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C51" s="1" t="str">
         <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>457</v>
+        <v>432</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="J51" s="6" t="str">
         <f t="shared" ref="J51" si="6">"Fetches a bundle of all "&amp;B51&amp;" resources for the specified "&amp;SUBSTITUTE(D51,","," and ")</f>
@@ -8787,7 +8790,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C52" s="1" t="str">
         <f t="shared" si="2"/>
@@ -8803,13 +8806,13 @@
         <v>139</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="1" customFormat="1">
@@ -8817,29 +8820,29 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C53" s="1" t="str">
         <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="1" customFormat="1">
@@ -8847,7 +8850,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C54" s="1" t="str">
         <f t="shared" si="2"/>
@@ -8863,10 +8866,10 @@
         <v>139</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="J54" s="6" t="str">
         <f t="shared" si="4"/>
@@ -8878,29 +8881,29 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C55" s="1" t="str">
         <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationstatement</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="1" customFormat="1">
@@ -8908,7 +8911,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C56" s="1" t="str">
         <f t="shared" si="2"/>
@@ -8924,10 +8927,10 @@
         <v>139</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="J56" s="6" t="str">
         <f t="shared" si="4"/>
@@ -8939,14 +8942,14 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C57" s="1" t="str">
         <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>20</v>
@@ -8955,10 +8958,10 @@
         <v>139</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="J57" s="6" t="str">
         <f t="shared" ref="J57" si="7">"Fetches a bundle of all "&amp;B57&amp;" resources for the specified "&amp;SUBSTITUTE(D57,","," and ")</f>
@@ -8970,26 +8973,26 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C58" s="1" t="str">
         <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="J58" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B58&amp;" resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes."</f>
@@ -9001,13 +9004,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>101</v>
@@ -9015,15 +9018,17 @@
       <c r="F59" s="1" t="s">
         <v>139</v>
       </c>
+      <c r="G59" s="1" t="s">
+        <v>448</v>
+      </c>
       <c r="H59" s="6" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="I59" s="6" t="s">
-        <v>403</v>
-      </c>
-      <c r="J59" s="6" t="str">
-        <f t="shared" si="4"/>
-        <v>Fetches a bundle of all Observation resources for the specified patient and category and status</v>
+        <v>389</v>
+      </c>
+      <c r="J59" s="6" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="1" customFormat="1">
@@ -9031,13 +9036,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>20</v>
@@ -9046,13 +9051,13 @@
         <v>139</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="I60" s="6" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="J60" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B60&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -9064,13 +9069,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>20</v>
@@ -9079,14 +9084,14 @@
         <v>139</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>315</v>
+        <v>456</v>
       </c>
       <c r="J61" s="6" t="str">
-        <f>"Fetches a bundle of all "&amp;B61&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation “code” parameter searches `Observation.code only."</f>
-        <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation “code” parameter searches `Observation.code only.</v>
+        <f>"Fetches a bundle of all "&amp;B61&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only."</f>
+        <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="1" customFormat="1">
@@ -9094,28 +9099,28 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C62" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>284</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="J62" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -9127,25 +9132,25 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="J63" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B63&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -9157,10 +9162,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>465</v>
+        <v>440</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>149</v>
@@ -9172,10 +9177,10 @@
         <v>139</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="J64" s="6" t="str">
         <f t="shared" ref="J64" si="8">"Fetches a bundle of all "&amp;B64&amp;" resources for the specified "&amp;SUBSTITUTE(D64,","," and ")</f>
@@ -9187,13 +9192,13 @@
         <v>58</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>20</v>
@@ -9202,13 +9207,13 @@
         <v>139</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="J65" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B65&amp;" resources for the specified "&amp;SUBSTITUTE(D65,","," and ")&amp;"=`assess-plan`"</f>
@@ -9220,31 +9225,31 @@
         <v>59</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="J66" s="6" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
     </row>
     <row r="67" spans="1:16" s="1" customFormat="1">
@@ -9252,13 +9257,13 @@
         <v>61</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>101</v>
@@ -9267,16 +9272,16 @@
         <v>139</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="H67" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="J67" s="6" t="s">
         <v>346</v>
-      </c>
-      <c r="I67" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="J67" s="6" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="68" spans="1:16" s="1" customFormat="1">
@@ -9284,31 +9289,31 @@
         <v>62</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="H68" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="J68" s="6" t="s">
         <v>347</v>
-      </c>
-      <c r="I68" s="6" t="s">
-        <v>353</v>
-      </c>
-      <c r="J68" s="6" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="69" spans="1:16" s="1" customFormat="1">
@@ -9316,7 +9321,7 @@
         <v>63</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="C69" s="1" t="str">
         <f t="shared" ref="C69" si="9">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B69)</f>
@@ -9332,16 +9337,16 @@
         <v>139</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>448</v>
+        <v>428</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="I69" s="6" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="J69" s="6" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="70" spans="1:16" ht="15.75">
@@ -9349,13 +9354,13 @@
         <v>64</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>20</v>
@@ -9364,13 +9369,13 @@
         <v>139</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="J70" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified patient and observation code."</f>
@@ -9388,13 +9393,13 @@
         <v>58</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>464</v>
+        <v>439</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>101</v>
@@ -9402,11 +9407,14 @@
       <c r="F71" s="1" t="s">
         <v>139</v>
       </c>
+      <c r="G71" s="1" t="s">
+        <v>451</v>
+      </c>
       <c r="H71" s="6" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="J71" s="6" t="str">
         <f t="shared" ref="J71" si="10">"Fetches a bundle of all "&amp;B71&amp;" resources for the specified "&amp;SUBSTITUTE(D71,","," and ")</f>
@@ -9418,13 +9426,13 @@
         <v>59</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>464</v>
+        <v>439</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>20</v>
@@ -9433,13 +9441,13 @@
         <v>139</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="I72" s="6" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="J72" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B72&amp;" resources for the specified patient and a category code = `vital-signs`"</f>
@@ -9451,13 +9459,13 @@
         <v>60</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>464</v>
+        <v>439</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>20</v>
@@ -9465,15 +9473,18 @@
       <c r="F73" s="1" t="s">
         <v>139</v>
       </c>
+      <c r="G73" s="1" t="s">
+        <v>451</v>
+      </c>
       <c r="H73" s="6" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="I73" s="6" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="J73" s="6" t="str">
-        <f>"Fetches a bundle of all "&amp;B73&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple codes. The Observation “code” parameter searches `Observation.code only."</f>
-        <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple codes. The Observation “code” parameter searches `Observation.code only.</v>
+        <f>"Fetches a bundle of all "&amp;B73&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple codes. The Observation `code` parameter searches `Observation.code only."</f>
+        <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
     <row r="74" spans="1:16" s="1" customFormat="1">
@@ -9481,28 +9492,28 @@
         <v>61</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>464</v>
+        <v>439</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="I74" s="6" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="J74" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B74&amp;" resources for the specified patient and date and a category code = `vital-signs`"</f>
@@ -9514,25 +9525,25 @@
         <v>62</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>464</v>
+        <v>439</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="I75" s="6" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="J75" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B75&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple codes."</f>
@@ -9544,7 +9555,7 @@
         <v>39</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C76" s="1" t="str">
         <f t="shared" ref="C76:C81" si="11">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B76)</f>
@@ -9560,10 +9571,10 @@
         <v>139</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>422</v>
+        <v>404</v>
       </c>
       <c r="I76" s="6" t="s">
-        <v>424</v>
+        <v>406</v>
       </c>
       <c r="J76" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B76&amp;" resources for the specified "&amp;SUBSTITUTE(D76,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
@@ -9575,23 +9586,23 @@
         <v>43</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
       <c r="C77" s="1" t="str">
         <f t="shared" ref="C77" si="12">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B77)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!documentreference</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>420</v>
+        <v>402</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>422</v>
+        <v>404</v>
       </c>
       <c r="I77" s="6"/>
       <c r="J77" s="6" t="str">
@@ -9604,14 +9615,14 @@
         <v>40</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C78" s="1" t="str">
         <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>20</v>
@@ -9620,16 +9631,16 @@
         <v>139</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>426</v>
+        <v>408</v>
       </c>
       <c r="I78" s="6" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
       <c r="J78" s="6" t="s">
-        <v>425</v>
+        <v>407</v>
       </c>
     </row>
     <row r="79" spans="1:16" s="1" customFormat="1" ht="15.75">
@@ -9637,32 +9648,32 @@
         <v>42</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C79" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B79)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>428</v>
+        <v>410</v>
       </c>
       <c r="I79" s="11" t="s">
-        <v>427</v>
+        <v>409</v>
       </c>
       <c r="J79" s="6" t="s">
-        <v>430</v>
+        <v>412</v>
       </c>
     </row>
     <row r="80" spans="1:16" s="1" customFormat="1">
@@ -9670,7 +9681,7 @@
         <v>41</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C80" s="1" t="str">
         <f t="shared" si="11"/>
@@ -9686,13 +9697,13 @@
         <v>139</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
       <c r="I80" s="6" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
       <c r="J80" s="6" t="s">
-        <v>429</v>
+        <v>411</v>
       </c>
     </row>
     <row r="81" spans="1:10" s="1" customFormat="1">
@@ -9700,26 +9711,26 @@
         <v>43</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C81" s="1" t="str">
         <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="H81" s="6" t="s">
-        <v>434</v>
+        <v>416</v>
       </c>
       <c r="I81" s="6" t="s">
-        <v>435</v>
+        <v>417</v>
       </c>
       <c r="J81" s="6" t="str">
         <f>"Fetches a bundle of all "&amp;B81&amp;" resources for the specified "&amp;SUBSTITUTE(D81,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>

</xml_diff>

<commit_message>
updates to all to all documentation generators and spreadsheets
</commit_message>
<xml_diff>
--- a/SP/uscore-server.xlsx
+++ b/SP/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Python\MyNotebooks\SP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED23464-87FA-4725-8A69-5B9DCB456C55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4045BD2E-366C-4C8B-A214-7EEE95459E1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68805" yWindow="-10800" windowWidth="68805" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-68805" yWindow="-10800" windowWidth="68805" windowHeight="28800" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
     <author>User</author>
   </authors>
   <commentList>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{CAFAF164-B5B4-4280-B703-1E7EE7F64AEA}">
+    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{CAFAF164-B5B4-4280-B703-1E7EE7F64AEA}">
       <text>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1925" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1953" uniqueCount="497">
   <si>
     <t>Element</t>
   </si>
@@ -730,9 +730,6 @@
     <t>GET [base]/DiagnosticReport?patient=1137192&amp;status=completed</t>
   </si>
   <si>
-    <t>GET [base]/MedicationRequest?patient=1137192&amp;status=active</t>
-  </si>
-  <si>
     <t>support searching for all prescriptions for a patient for a given status (for example all active prescriptions)</t>
   </si>
   <si>
@@ -742,9 +739,6 @@
     <t>support searching for all medications for a patient for a given status (for example all active medications)</t>
   </si>
   <si>
-    <t>GET [base]/MedicationStatement?patient=1137192&amp;status=active</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport-lab</t>
   </si>
   <si>
@@ -901,12 +895,6 @@
     <t>support searching for all prescriptions for a patient by date</t>
   </si>
   <si>
-    <t>GET [base]/Goal?patient=1137192&amp;date=ge2015-01-14&amp;date=le2019-01-14</t>
-  </si>
-  <si>
-    <t>GET [base]/MeidcationRequest?patient=1137192&amp;date=ge2019</t>
-  </si>
-  <si>
     <t>support searching for all medications for a patient by date</t>
   </si>
   <si>
@@ -916,9 +904,6 @@
     <t>patient,effective</t>
   </si>
   <si>
-    <t>GET [base]/MedicationStatement?patient=1137192&amp;effective=ge2019</t>
-  </si>
-  <si>
     <t>Fetches a bundle of all MedicationRequest resources for the specified patient and status</t>
   </si>
   <si>
@@ -958,15 +943,9 @@
     <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan</t>
   </si>
   <si>
-    <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;date=ge2019</t>
-  </si>
-  <si>
     <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;status=active</t>
   </si>
   <si>
-    <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;status=active&amp;date=ge2019</t>
-  </si>
-  <si>
     <t>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan` and date</t>
   </si>
   <si>
@@ -1217,12 +1196,6 @@
   </si>
   <si>
     <t>lifecycle-status</t>
-  </si>
-  <si>
-    <t>start-date</t>
-  </si>
-  <si>
-    <t>patient,start-date</t>
   </si>
   <si>
     <t>!CarePlan</t>
@@ -1592,10 +1565,61 @@
  `GET /MedicationStatement?patient=[id]&amp;_include=MedicationStatement:medication`</t>
   </si>
   <si>
-    <t>hl7.fhir.us.core.r4-4.0.0-server</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/ImplementationGuide/hl7.fhir.us.core.r4-4.0.0-server</t>
+    <t>us-core-server</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/ImplementationGuide/hl7.fhir.us.core.r4-4.0.0</t>
+  </si>
+  <si>
+    <t>versioning_conf</t>
+  </si>
+  <si>
+    <t>readHistory_conf</t>
+  </si>
+  <si>
+    <t>updateCreate_conf</t>
+  </si>
+  <si>
+    <t>conditionalCreate_conf</t>
+  </si>
+  <si>
+    <t>conditionalRead_conf</t>
+  </si>
+  <si>
+    <t>conditionalUpdate_conf</t>
+  </si>
+  <si>
+    <t>conditionalDelete_conf</t>
+  </si>
+  <si>
+    <t>referencePolicy_conf</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationRequest?patient=1137192&amp;status=active~GET [base]/MedicationRequest?patient=1137192&amp;status=active&amp;_include=MedicationRequest:medication</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationStatement?patient=1137192&amp;status=active~GET [base]/MedicationStatement?patient=1137192&amp;status=active&amp;_include=MedicationStatement:medication</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationRequest?patient=1137192&amp;effective=ge2019~GET [base]/MedicationStatement?patient=1137192&amp;effective=ge2019&amp;_include=MedicationRequest:medication</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationStatement?patient=1137192&amp;date=ge2019~GET [base]/MedicationRequest?patient=1137192&amp;date=ge2019&amp;_include=MedicationStatement:medication</t>
+  </si>
+  <si>
+    <t>target-date</t>
+  </si>
+  <si>
+    <t>patient,target-date</t>
+  </si>
+  <si>
+    <t>GET [base]/Goal?patient=1137192&amp;target-date=ge2015-01-14&amp;target-date=le2019-01-14</t>
+  </si>
+  <si>
+    <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;date=ge2019~GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;date=ge2018&amp;date=le2018</t>
+  </si>
+  <si>
+    <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;status=active&amp;date=ge2019~GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;status=active&amp;date=ge2018&amp;date=le2019</t>
   </si>
 </sst>
 </file>
@@ -2064,8 +2088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2087,7 +2111,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="105" customHeight="1">
@@ -2095,7 +2119,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2103,7 +2127,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2119,7 +2143,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="103.5" customHeight="1">
@@ -2127,7 +2151,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -2163,7 +2187,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2190,25 +2214,25 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="B2" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="B3" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -2220,31 +2244,31 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -2253,7 +2277,7 @@
         <v>91</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -2265,10 +2289,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -2280,10 +2304,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -2295,10 +2319,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
@@ -2310,10 +2334,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
@@ -2325,10 +2349,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>14</v>
@@ -2340,10 +2364,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>14</v>
@@ -2355,25 +2379,25 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
@@ -2385,10 +2409,10 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>14</v>
@@ -2400,25 +2424,25 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>14</v>
@@ -2430,10 +2454,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>14</v>
@@ -2445,40 +2469,40 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>14</v>
@@ -2490,25 +2514,25 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>14</v>
@@ -2520,10 +2544,10 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>14</v>
@@ -2538,7 +2562,7 @@
         <v>89</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>14</v>
@@ -2592,10 +2616,10 @@
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2606,7 +2630,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>205</v>
@@ -2620,10 +2644,10 @@
         <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2634,10 +2658,10 @@
         <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2648,7 +2672,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>32</v>
@@ -2662,7 +2686,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>180</v>
@@ -2676,7 +2700,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>204</v>
@@ -2690,7 +2714,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>199</v>
@@ -2701,7 +2725,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>202</v>
@@ -2712,7 +2736,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>156</v>
@@ -2723,7 +2747,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>33</v>
@@ -2734,10 +2758,10 @@
         <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2745,7 +2769,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>204</v>
@@ -2756,7 +2780,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>203</v>
@@ -2767,10 +2791,10 @@
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -2778,7 +2802,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>204</v>
@@ -2789,7 +2813,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>200</v>
@@ -2800,10 +2824,10 @@
         <v>14</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -2811,10 +2835,10 @@
         <v>14</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -2822,7 +2846,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>201</v>
@@ -2833,10 +2857,10 @@
         <v>14</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -2844,7 +2868,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>204</v>
@@ -2855,7 +2879,7 @@
         <v>14</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>200</v>
@@ -2866,7 +2890,7 @@
         <v>14</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>31</v>
@@ -2879,13 +2903,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:P59"/>
+  <dimension ref="A1:X59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Q17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2893,14 +2917,17 @@
     <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="49.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="1" customWidth="1"/>
-    <col min="5" max="10" width="17.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" style="1" customWidth="1"/>
-    <col min="12" max="15" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" customWidth="1"/>
+    <col min="6" max="12" width="17.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" style="1" customWidth="1"/>
+    <col min="14" max="17" width="17.42578125" style="1" customWidth="1"/>
+    <col min="18" max="19" width="20.42578125" style="1" customWidth="1"/>
+    <col min="20" max="23" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" thickBot="1">
+    <row r="1" spans="1:24" ht="18" thickBot="1">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2913,44 +2940,68 @@
       <c r="D1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>476</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="K1" t="s">
+        <v>466</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="R1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>477</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>478</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="S1" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="X1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="38.25" customHeight="1" thickTop="1">
+    <row r="2" spans="1:24" ht="38.25" customHeight="1" thickTop="1">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -2959,142 +3010,178 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2"/>
-      <c r="E2"/>
-      <c r="K2" t="s">
+      <c r="F2"/>
+      <c r="R2" t="s">
         <v>29</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="X2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:24">
       <c r="A3" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="S3" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" s="1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="S4" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5" s="1" t="s">
         <v>156</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P5" t="s">
+      <c r="S5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="X5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:24">
       <c r="A6" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="S6" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" s="1" t="s">
         <v>200</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="S7" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" s="1" t="s">
         <v>199</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="S8" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="S9" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10" s="1" t="s">
         <v>201</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="S10" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11" s="1" t="s">
         <v>180</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="R11" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="S11" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
       <c r="A12" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="105">
+      <c r="S12" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="105">
       <c r="A13" s="1" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="K13" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="R13" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="315">
+      <c r="S13" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="315">
       <c r="A14" s="1" t="s">
         <v>202</v>
       </c>
@@ -3102,16 +3189,19 @@
         <v>14</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="K14" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="R14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M14" s="7" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="315">
+      <c r="S14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="U14" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="315">
       <c r="A15" s="1" t="s">
         <v>205</v>
       </c>
@@ -3119,103 +3209,124 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="K15" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="R15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M15" s="7" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="S15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
       <c r="A16" s="1" t="s">
         <v>204</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="R16" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="S16" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" s="1" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="S17" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="R18" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="S18" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="U20" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" s="1" t="s">
         <v>203</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="R21" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="S21" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:21">
       <c r="A23"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:21">
       <c r="A24"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:21">
       <c r="A25"/>
     </row>
-    <row r="56" spans="12:15" ht="18">
-      <c r="L56" s="7"/>
-      <c r="N56" s="7"/>
-      <c r="O56" s="7"/>
-    </row>
-    <row r="59" spans="12:15" ht="18">
-      <c r="O59" s="7"/>
+    <row r="56" spans="20:23" ht="18">
+      <c r="T56" s="7"/>
+      <c r="V56" s="7"/>
+      <c r="W56" s="7"/>
+    </row>
+    <row r="59" spans="20:23" ht="18">
+      <c r="W59" s="7"/>
     </row>
   </sheetData>
   <sortState ref="A2:A21">
@@ -3262,10 +3373,10 @@
     </row>
     <row r="2" spans="1:5" ht="120.75" thickBot="1">
       <c r="A2" s="15" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="B2" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>199</v>
@@ -3274,7 +3385,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3306,64 +3417,64 @@
         <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>459</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -3961,10 +4072,10 @@
   <dimension ref="A1:AB93"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="U48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="Y56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U60" sqref="U60"/>
+      <selection pane="bottomRight" activeCell="Y54" sqref="Y54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -4056,10 +4167,10 @@
         <v>64</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="W1" s="4" t="s">
         <v>65</v>
@@ -4085,7 +4196,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>158</v>
@@ -4135,7 +4246,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>38</v>
@@ -4182,7 +4293,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>96</v>
@@ -4295,7 +4406,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>76</v>
@@ -4379,7 +4490,7 @@
         <v>70</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="Z7" s="5" t="s">
         <v>104</v>
@@ -4429,7 +4540,7 @@
         <v>70</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="Z8" s="1" t="s">
         <v>106</v>
@@ -4742,10 +4853,10 @@
         <v>70</v>
       </c>
       <c r="Y14" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="Z14" s="5" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="AA14" s="2" t="s">
         <v>191</v>
@@ -4899,7 +5010,7 @@
         <v>70</v>
       </c>
       <c r="Y17" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="Z17" t="s">
         <v>179</v>
@@ -5112,7 +5223,7 @@
         <v>92</v>
       </c>
       <c r="Z21" s="5" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="AB21" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B21)&amp;"-"&amp;SUBSTITUTE(C21,"_","")&amp;".html")</f>
@@ -5348,7 +5459,7 @@
       </c>
       <c r="X26"/>
       <c r="Y26" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="Z26" s="1" t="s">
         <v>178</v>
@@ -6056,13 +6167,13 @@
         <v>70</v>
       </c>
       <c r="Y40" s="5" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="Z40" s="5" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="AA40" s="2" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="AB40" s="1" t="str">
         <f t="shared" ref="AB40" si="13">"SearchParameter-us-core-"&amp;LOWER((B40)&amp;"-"&amp;C40&amp;".html")</f>
@@ -6337,7 +6448,7 @@
         <v>199</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>42</v>
@@ -6359,7 +6470,7 @@
         <v>96</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>70</v>
@@ -6653,7 +6764,7 @@
         <v>201</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>42</v>
@@ -6762,7 +6873,7 @@
         <v>201</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>370</v>
+        <v>492</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>42</v>
@@ -6785,7 +6896,7 @@
       </c>
       <c r="J54" s="1" t="str">
         <f t="shared" ref="J54" si="26">B54&amp;"."&amp;C54</f>
-        <v>Goal.start-date</v>
+        <v>Goal.target-date</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>70</v>
@@ -6805,7 +6916,7 @@
       <c r="AA54" s="12"/>
       <c r="AB54" s="1" t="str">
         <f t="shared" si="25"/>
-        <v>SearchParameter-us-core-goal-start-date.html</v>
+        <v>SearchParameter-us-core-goal-target-date.html</v>
       </c>
     </row>
     <row r="55" spans="1:28" s="1" customFormat="1">
@@ -6899,16 +7010,16 @@
       </c>
       <c r="U56" s="7"/>
       <c r="V56" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="X56" s="1" t="s">
         <v>109</v>
       </c>
       <c r="Y56" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="Z56" s="12" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="AA56" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B56&amp; " resources for the specified patient. Mandatory for client to support the _include parameter. Optional for server to support the _include parameter."</f>
@@ -6927,7 +7038,7 @@
         <v>202</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>42</v>
@@ -7063,16 +7174,16 @@
         <v>70</v>
       </c>
       <c r="V59" s="7" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="X59" s="1" t="s">
         <v>109</v>
       </c>
       <c r="Y59" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="Z59" s="12" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="AA59" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B59&amp; " resources for the specified patient. Mandatory for client to support the _include parameter. Optional for server to support the _include parameter."</f>
@@ -7091,7 +7202,7 @@
         <v>205</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>42</v>
@@ -7234,7 +7345,7 @@
         <v>support searching for all procedures for a patient</v>
       </c>
       <c r="Z62" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="AA62" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B62&amp; " resources for the specified patient"</f>
@@ -7617,7 +7728,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>158</v>
@@ -7667,7 +7778,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>38</v>
@@ -7714,7 +7825,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>96</v>
@@ -7768,7 +7879,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>107</v>
@@ -7827,7 +7938,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>76</v>
@@ -7877,7 +7988,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>107</v>
@@ -7936,7 +8047,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>76</v>
@@ -7986,7 +8097,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>107</v>
@@ -8045,7 +8156,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>22</v>
@@ -8087,7 +8198,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>35</v>
@@ -8122,10 +8233,10 @@
         <v>70</v>
       </c>
       <c r="Y79" s="1" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="Z79" s="7" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="AA79" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B79&amp; " resources that match the name"</f>
@@ -8141,7 +8252,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>103</v>
@@ -8176,10 +8287,10 @@
         <v>70</v>
       </c>
       <c r="Y80" s="1" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="Z80" s="7" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="AA80" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B80&amp; " resources that match the address string"</f>
@@ -8195,10 +8306,10 @@
         <v>79</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>86</v>
@@ -8230,10 +8341,10 @@
         <v>70</v>
       </c>
       <c r="Y81" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="Z81" s="7" t="s">
         <v>300</v>
-      </c>
-      <c r="Z81" s="7" t="s">
-        <v>307</v>
       </c>
       <c r="AA81" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B81&amp; " resources for the city"</f>
@@ -8249,10 +8360,10 @@
         <v>80</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>86</v>
@@ -8284,10 +8395,10 @@
         <v>70</v>
       </c>
       <c r="Y82" s="1" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="Z82" s="7" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="AA82" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B82&amp; " resources for the state"</f>
@@ -8303,10 +8414,10 @@
         <v>81</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>86</v>
@@ -8338,10 +8449,10 @@
         <v>70</v>
       </c>
       <c r="Y83" s="1" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="Z83" s="7" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="AA83" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B83&amp; " resources for the ZIP code"</f>
@@ -8357,7 +8468,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>35</v>
@@ -8392,10 +8503,10 @@
         <v>70</v>
       </c>
       <c r="Y84" s="1" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="Z84" s="7" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="AA84" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B84&amp; " resources that match the name"</f>
@@ -8411,7 +8522,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>103</v>
@@ -8446,10 +8557,10 @@
         <v>70</v>
       </c>
       <c r="Y85" s="1" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="Z85" s="7" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="AA85" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B85&amp; " resources that match the address string"</f>
@@ -8465,10 +8576,10 @@
         <v>84</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>86</v>
@@ -8500,10 +8611,10 @@
         <v>70</v>
       </c>
       <c r="Y86" s="1" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="Z86" s="7" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="AA86" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B86&amp; " resources for the city"</f>
@@ -8519,10 +8630,10 @@
         <v>85</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>86</v>
@@ -8554,10 +8665,10 @@
         <v>70</v>
       </c>
       <c r="Y87" s="1" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="Z87" s="7" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="AA87" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B87&amp; " resources for the state"</f>
@@ -8573,10 +8684,10 @@
         <v>86</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>86</v>
@@ -8608,10 +8719,10 @@
         <v>70</v>
       </c>
       <c r="Y88" s="1" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="Z88" s="7" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="AA88" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B88&amp; " resources for the ZIP code"</f>
@@ -8627,7 +8738,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>35</v>
@@ -8665,10 +8776,10 @@
         <v>94</v>
       </c>
       <c r="Y89" s="5" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Z89" s="7" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="AA89" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources matching the name"</f>
@@ -8684,7 +8795,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>93</v>
@@ -8719,10 +8830,10 @@
         <v>70</v>
       </c>
       <c r="Y90" s="5" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="Z90" s="7" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="AA90" s="12" t="str">
         <f>"Fetches a bundle containing any "&amp;B90&amp;" resources matching the identifier"</f>
@@ -8738,10 +8849,10 @@
         <v>89</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>14</v>
@@ -8773,13 +8884,13 @@
         <v>70</v>
       </c>
       <c r="V91" s="1" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="Y91" s="5" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="Z91" s="7" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="AA91" s="12" t="str">
         <f>"Fetches a bundle containing  "&amp;B91&amp;" resources matching the specialty"</f>
@@ -8795,10 +8906,10 @@
         <v>90</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>14</v>
@@ -8830,16 +8941,16 @@
         <v>70</v>
       </c>
       <c r="S92" s="1" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="V92" s="1" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="Y92" s="5" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="Z92" s="7" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="AA92" s="12" t="str">
         <f>"Fetches a bundle containing  "&amp;B92&amp;" resources matching the chained parameter practitioner.name or practitioner.identifier. SHOULD support the _include for PractionerRole.practitioner and PractitionerRole.endpoint."</f>
@@ -8868,21 +8979,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="I71" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="I41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C96" sqref="C96"/>
+      <selection pane="bottomRight" activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="1"/>
     <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="66" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" customWidth="1"/>
     <col min="8" max="8" width="84.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="68.28515625" style="1" customWidth="1"/>
@@ -8909,7 +9020,7 @@
         <v>116</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>3</v>
@@ -9042,10 +9153,10 @@
         <v>124</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="J6" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9227,10 +9338,10 @@
         <v>131</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="J13" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9308,10 +9419,10 @@
         <v>124</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="J16" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9365,10 +9476,10 @@
         <v>124</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="J18" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9780,16 +9891,16 @@
         <v>124</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>174</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -9816,7 +9927,7 @@
         <v>168</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>164</v>
@@ -9846,7 +9957,7 @@
         <v>169</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="J35" s="5" t="s">
         <v>170</v>
@@ -9906,10 +10017,10 @@
         <v>181</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
     </row>
     <row r="38" spans="1:10" s="1" customFormat="1">
@@ -9964,7 +10075,7 @@
         <v>167</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>182</v>
@@ -9982,7 +10093,7 @@
         <v>200</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>134</v>
@@ -9994,7 +10105,7 @@
         <v>124</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I40" s="5" t="s">
         <v>206</v>
@@ -10012,7 +10123,7 @@
         <v>200</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>163</v>
@@ -10024,13 +10135,13 @@
         <v>124</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J41" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B41&amp;" resources for the specified patient and  a category code = `LAB`"</f>
@@ -10045,7 +10156,7 @@
         <v>200</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>165</v>
@@ -10057,10 +10168,10 @@
         <v>124</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J42" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B42&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -10075,25 +10186,25 @@
         <v>200</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="H43" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="I43" s="9" t="s">
         <v>220</v>
-      </c>
-      <c r="I43" s="9" t="s">
-        <v>222</v>
       </c>
       <c r="J43" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B43&amp;" resources for the specified patient and date and a category code = `LAB`"</f>
@@ -10108,22 +10219,22 @@
         <v>200</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="I44" s="5" t="s">
         <v>249</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>251</v>
       </c>
       <c r="J44" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B44&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -10138,7 +10249,7 @@
         <v>200</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>134</v>
@@ -10150,7 +10261,7 @@
         <v>124</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="I45" s="5" t="s">
         <v>206</v>
@@ -10168,22 +10279,22 @@
         <v>200</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>124</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J46" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified patient and  a category code specified in US Core DiagnosticReport Category Codes"</f>
@@ -10198,7 +10309,7 @@
         <v>200</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>165</v>
@@ -10210,10 +10321,10 @@
         <v>124</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J47" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B47&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -10228,22 +10339,22 @@
         <v>200</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H48" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="I48" s="5" t="s">
         <v>227</v>
-      </c>
-      <c r="I48" s="5" t="s">
-        <v>229</v>
       </c>
       <c r="J48" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B48&amp;" resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes"</f>
@@ -10258,22 +10369,22 @@
         <v>200</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="I49" s="5" t="s">
         <v>249</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>251</v>
       </c>
       <c r="J49" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B49&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -10292,7 +10403,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>86</v>
@@ -10301,10 +10412,10 @@
         <v>124</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="J50" s="5" t="str">
         <f t="shared" si="4"/>
@@ -10323,7 +10434,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>371</v>
+        <v>493</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>86</v>
@@ -10332,14 +10443,14 @@
         <v>167</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>264</v>
+        <v>494</v>
       </c>
       <c r="J51" s="5" t="str">
         <f t="shared" ref="J51" si="6">"Fetches a bundle of all "&amp;B51&amp;" resources for the specified "&amp;SUBSTITUTE(D51,","," and ")</f>
-        <v>Fetches a bundle of all Goal resources for the specified patient and start-date</v>
+        <v>Fetches a bundle of all Goal resources for the specified patient and target-date</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="1" customFormat="1">
@@ -10363,13 +10474,13 @@
         <v>124</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>207</v>
+        <v>488</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="1" customFormat="1">
@@ -10384,7 +10495,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>86</v>
@@ -10393,13 +10504,13 @@
         <v>167</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>269</v>
+        <v>490</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="1" customFormat="1">
@@ -10423,10 +10534,10 @@
         <v>124</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>211</v>
+        <v>489</v>
       </c>
       <c r="J54" s="5" t="str">
         <f t="shared" si="4"/>
@@ -10445,7 +10556,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationstatement</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>86</v>
@@ -10454,13 +10565,13 @@
         <v>167</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>265</v>
+        <v>491</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="1" customFormat="1">
@@ -10484,10 +10595,10 @@
         <v>124</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J56" s="5" t="str">
         <f t="shared" si="4"/>
@@ -10515,10 +10626,10 @@
         <v>124</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J57" s="5" t="str">
         <f t="shared" ref="J57" si="7">"Fetches a bundle of all "&amp;B57&amp;" resources for the specified "&amp;SUBSTITUTE(D57,","," and ")</f>
@@ -10537,19 +10648,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J58" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B58&amp;" resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes."</f>
@@ -10564,10 +10675,10 @@
         <v>204</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>86</v>
@@ -10576,16 +10687,16 @@
         <v>124</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="1" customFormat="1">
@@ -10596,7 +10707,7 @@
         <v>204</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>163</v>
@@ -10608,13 +10719,13 @@
         <v>124</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J60" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B60&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -10629,7 +10740,7 @@
         <v>204</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>165</v>
@@ -10641,10 +10752,10 @@
         <v>124</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="J61" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B61&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only."</f>
@@ -10659,25 +10770,25 @@
         <v>204</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F62" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="I62" s="5" t="s">
         <v>246</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="H62" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="I62" s="5" t="s">
-        <v>248</v>
       </c>
       <c r="J62" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -10692,22 +10803,22 @@
         <v>204</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J63" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B63&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -10719,10 +10830,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>134</v>
@@ -10734,10 +10845,10 @@
         <v>124</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J64" s="5" t="str">
         <f t="shared" ref="J64" si="8">"Fetches a bundle of all "&amp;B64&amp;" resources for the specified "&amp;SUBSTITUTE(D64,","," and ")</f>
@@ -10749,10 +10860,10 @@
         <v>58</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>163</v>
@@ -10764,13 +10875,13 @@
         <v>124</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="J65" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B65&amp;" resources for the specified "&amp;SUBSTITUTE(D65,","," and ")&amp;"=`assess-plan`"</f>
@@ -10782,31 +10893,31 @@
         <v>59</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C66" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="H66" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="H66" s="5" t="s">
-        <v>280</v>
-      </c>
       <c r="I66" s="5" t="s">
-        <v>283</v>
+        <v>495</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="67" spans="1:16" s="1" customFormat="1">
@@ -10814,13 +10925,13 @@
         <v>61</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>86</v>
@@ -10829,16 +10940,16 @@
         <v>124</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="H67" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="I67" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="I67" s="5" t="s">
-        <v>284</v>
-      </c>
       <c r="J67" s="5" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="68" spans="1:16" s="1" customFormat="1">
@@ -10846,31 +10957,31 @@
         <v>62</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>285</v>
+        <v>496</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
     </row>
     <row r="69" spans="1:16" s="1" customFormat="1">
@@ -10878,7 +10989,7 @@
         <v>63</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="C69" s="1" t="str">
         <f t="shared" ref="C69" si="9">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B69)</f>
@@ -10894,16 +11005,16 @@
         <v>124</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
     </row>
     <row r="70" spans="1:16" ht="15.75">
@@ -10914,7 +11025,7 @@
         <v>204</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>165</v>
@@ -10926,13 +11037,13 @@
         <v>124</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="J70" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified patient and observation code."</f>
@@ -10953,10 +11064,10 @@
         <v>204</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>86</v>
@@ -10965,13 +11076,13 @@
         <v>124</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="I71" s="5" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="J71" s="5" t="str">
         <f t="shared" ref="J71" si="10">"Fetches a bundle of all "&amp;B71&amp;" resources for the specified "&amp;SUBSTITUTE(D71,","," and ")</f>
@@ -10986,7 +11097,7 @@
         <v>204</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>163</v>
@@ -10998,13 +11109,13 @@
         <v>124</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="J72" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B72&amp;" resources for the specified patient and a category code = `vital-signs`"</f>
@@ -11019,7 +11130,7 @@
         <v>204</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>165</v>
@@ -11031,13 +11142,13 @@
         <v>124</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="J73" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B73&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple codes. The Observation `code` parameter searches `Observation.code only."</f>
@@ -11052,25 +11163,25 @@
         <v>204</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="J74" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B74&amp;" resources for the specified patient and date and a category code = `vital-signs`"</f>
@@ -11085,22 +11196,22 @@
         <v>204</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="I75" s="5" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="J75" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B75&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple codes."</f>
@@ -11128,10 +11239,10 @@
         <v>124</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="J76" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B76&amp;" resources for the specified "&amp;SUBSTITUTE(D76,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
@@ -11143,14 +11254,14 @@
         <v>43</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="C77" s="1" t="str">
         <f t="shared" ref="C77" si="12">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B77)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!documentreference</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>86</v>
@@ -11159,7 +11270,7 @@
         <v>167</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="I77" s="5"/>
       <c r="J77" s="5" t="str">
@@ -11188,16 +11299,16 @@
         <v>124</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="I78" s="5" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="J78" s="5" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
     </row>
     <row r="79" spans="1:16" s="1" customFormat="1" ht="15.75">
@@ -11212,25 +11323,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="I79" s="9" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="J79" s="5" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
     </row>
     <row r="80" spans="1:16" s="1" customFormat="1">
@@ -11254,13 +11365,13 @@
         <v>124</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="I80" s="5" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
     </row>
     <row r="81" spans="1:10" s="1" customFormat="1">
@@ -11275,19 +11386,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="I81" s="5" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
       <c r="J81" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B81&amp;" resources for the specified "&amp;SUBSTITUTE(D81,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
@@ -11299,7 +11410,7 @@
         <v>41</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C82" s="1" t="str">
         <f t="shared" ref="C82" si="13">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B82)</f>
@@ -11315,13 +11426,13 @@
         <v>124</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
       <c r="I82" s="5" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add  or and ands
</commit_message>
<xml_diff>
--- a/SP/uscore-server.xlsx
+++ b/SP/uscore-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Python\MyNotebooks\SP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/Python/MyNotebooks/SP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4045BD2E-366C-4C8B-A214-7EEE95459E1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238668DE-96DB-DE4E-BDB6-9E5B76D944B2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68805" yWindow="-10800" windowWidth="68805" windowHeight="28800" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -52,7 +53,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -61,7 +62,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 not used -for algorithmic generation of combos</t>
@@ -86,7 +87,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -95,7 +96,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 not being used since enumerating for US Core</t>
@@ -1626,7 +1627,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1676,14 +1677,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -2092,13 +2093,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="95.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="95.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2106,7 +2107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2114,7 +2115,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="105" customHeight="1">
+    <row r="3" spans="1:2" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2122,7 +2123,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2130,7 +2131,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2138,7 +2139,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="351.75" customHeight="1">
+    <row r="6" spans="1:2" ht="351.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2146,7 +2147,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="103.5" customHeight="1">
+    <row r="7" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2167,9 +2168,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -2190,15 +2191,15 @@
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="94" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -2212,7 +2213,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>397</v>
       </c>
@@ -2227,7 +2228,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>399</v>
       </c>
@@ -2242,7 +2243,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>401</v>
       </c>
@@ -2257,7 +2258,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>402</v>
       </c>
@@ -2272,7 +2273,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>91</v>
       </c>
@@ -2287,7 +2288,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>404</v>
       </c>
@@ -2302,7 +2303,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>317</v>
       </c>
@@ -2317,7 +2318,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>407</v>
       </c>
@@ -2332,7 +2333,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>409</v>
       </c>
@@ -2347,7 +2348,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>411</v>
       </c>
@@ -2362,7 +2363,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>413</v>
       </c>
@@ -2377,7 +2378,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>414</v>
       </c>
@@ -2392,7 +2393,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>416</v>
       </c>
@@ -2407,7 +2408,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>417</v>
       </c>
@@ -2422,7 +2423,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>419</v>
       </c>
@@ -2437,7 +2438,7 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>211</v>
       </c>
@@ -2452,7 +2453,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>212</v>
       </c>
@@ -2467,7 +2468,7 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>424</v>
       </c>
@@ -2482,7 +2483,7 @@
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>270</v>
       </c>
@@ -2497,7 +2498,7 @@
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>427</v>
       </c>
@@ -2512,7 +2513,7 @@
       </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>429</v>
       </c>
@@ -2527,7 +2528,7 @@
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>431</v>
       </c>
@@ -2542,7 +2543,7 @@
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>210</v>
       </c>
@@ -2557,7 +2558,7 @@
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>89</v>
       </c>
@@ -2586,15 +2587,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="89" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="59.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="59.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -2608,7 +2609,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2622,7 +2623,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2636,7 +2637,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2650,7 +2651,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2664,7 +2665,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2678,7 +2679,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2692,7 +2693,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2706,7 +2707,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -2720,7 +2721,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
@@ -2731,7 +2732,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
@@ -2742,7 +2743,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
@@ -2753,7 +2754,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2764,7 +2765,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
@@ -2775,7 +2776,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
@@ -2786,7 +2787,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2797,7 +2798,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
@@ -2808,7 +2809,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
@@ -2819,7 +2820,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
@@ -2830,7 +2831,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>14</v>
       </c>
@@ -2841,7 +2842,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
@@ -2852,7 +2853,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>14</v>
       </c>
@@ -2863,7 +2864,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>14</v>
       </c>
@@ -2874,7 +2875,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
@@ -2885,7 +2886,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>14</v>
       </c>
@@ -2912,22 +2913,22 @@
       <selection pane="bottomRight" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="12" width="17.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" style="1" customWidth="1"/>
-    <col min="14" max="17" width="17.42578125" style="1" customWidth="1"/>
-    <col min="18" max="19" width="20.42578125" style="1" customWidth="1"/>
-    <col min="20" max="23" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="27.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5" style="1" customWidth="1"/>
+    <col min="14" max="17" width="17.5" style="1" customWidth="1"/>
+    <col min="18" max="19" width="20.5" style="1" customWidth="1"/>
+    <col min="20" max="23" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18" thickBot="1">
+    <row r="1" spans="1:24" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -3001,7 +3002,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="38.25" customHeight="1" thickTop="1">
+    <row r="2" spans="1:24" ht="38.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -3021,7 +3022,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>268</v>
       </c>
@@ -3035,7 +3036,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>282</v>
       </c>
@@ -3049,7 +3050,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>156</v>
       </c>
@@ -3066,7 +3067,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>286</v>
       </c>
@@ -3080,7 +3081,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>200</v>
       </c>
@@ -3094,7 +3095,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>199</v>
       </c>
@@ -3108,7 +3109,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -3122,7 +3123,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>201</v>
       </c>
@@ -3136,7 +3137,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>180</v>
       </c>
@@ -3150,7 +3151,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>287</v>
       </c>
@@ -3164,7 +3165,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="105">
+    <row r="13" spans="1:24" ht="80" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>421</v>
       </c>
@@ -3181,7 +3182,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="315">
+    <row r="14" spans="1:24" ht="288" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>202</v>
       </c>
@@ -3201,7 +3202,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="315">
+    <row r="15" spans="1:24" ht="288" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>205</v>
       </c>
@@ -3221,7 +3222,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>204</v>
       </c>
@@ -3235,7 +3236,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>301</v>
       </c>
@@ -3249,7 +3250,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -3263,7 +3264,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>308</v>
       </c>
@@ -3277,7 +3278,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>311</v>
       </c>
@@ -3294,7 +3295,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>203</v>
       </c>
@@ -3308,28 +3309,28 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22"/>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23"/>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24"/>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25"/>
     </row>
-    <row r="56" spans="20:23" ht="18">
+    <row r="56" spans="20:23" ht="18" x14ac:dyDescent="0.2">
       <c r="T56" s="7"/>
       <c r="V56" s="7"/>
       <c r="W56" s="7"/>
     </row>
-    <row r="59" spans="20:23" ht="18">
+    <row r="59" spans="20:23" ht="18" x14ac:dyDescent="0.2">
       <c r="W59" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="A2:A21">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A21">
     <sortCondition ref="A2:A21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3346,15 +3347,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -3371,7 +3372,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="120.75" thickBot="1">
+    <row r="2" spans="1:5" ht="113" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>439</v>
       </c>
@@ -3388,7 +3389,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E4" s="2"/>
     </row>
   </sheetData>
@@ -3404,15 +3405,15 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" customWidth="1"/>
+    <col min="8" max="8" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -3477,7 +3478,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -3542,7 +3543,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -3607,7 +3608,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -3672,7 +3673,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -3737,7 +3738,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -3802,7 +3803,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -3867,7 +3868,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -3932,7 +3933,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -3997,7 +3998,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -4071,41 +4072,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AB93"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="Y56" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y54" sqref="Y54"/>
+      <selection pane="bottomRight" activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="21.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="21.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="36.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="49.7109375" style="1" customWidth="1"/>
-    <col min="21" max="22" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="49.6640625" style="1" customWidth="1"/>
+    <col min="21" max="22" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16" style="1" customWidth="1"/>
-    <col min="24" max="24" width="50.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="68.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="90.7109375" style="1" customWidth="1"/>
-    <col min="27" max="27" width="83.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="38.140625" customWidth="1"/>
+    <col min="24" max="24" width="50.83203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="68.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="90.6640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="83.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="18" customHeight="1" thickBot="1">
+    <row r="1" spans="1:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>159</v>
       </c>
@@ -4191,7 +4192,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" ht="15.75" thickTop="1">
+    <row r="2" spans="1:28" s="1" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4241,7 +4242,7 @@
         <v>SearchParameter-us-core-!example category search-category.html</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="1" customFormat="1">
+    <row r="3" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4288,7 +4289,7 @@
         <v>SearchParameter-us-core-!example code search-code.html</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="4" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4342,7 +4343,7 @@
         <v>SearchParameter-us-core-!example date search-date.html</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="1" customFormat="1" ht="29.25">
+    <row r="5" spans="1:28" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4401,7 +4402,7 @@
         <v>SearchParameter-us-core-!example patient search-patient.html</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="1" customFormat="1">
+    <row r="6" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4451,7 +4452,7 @@
         <v>SearchParameter-us-core-!example status search-status.html</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="15.75" customHeight="1">
+    <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4501,7 +4502,7 @@
         <v>SearchParameter-us-core-!patient-address.html</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4551,7 +4552,7 @@
         <v>SearchParameter-us-core-!patient-telecom.html</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4597,7 +4598,7 @@
         <v>SearchParameter-us-core-allergyintolerance-clinical-status.html</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="29.25">
+    <row r="10" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4656,7 +4657,7 @@
         <v>SearchParameter-us-core-allergyintolerance-patient.html</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4707,7 +4708,7 @@
         <v>SearchParameter-us-core-condition-category.html</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4755,7 +4756,7 @@
         <v>SearchParameter-us-core-condition-clinical-status.html</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4813,7 +4814,7 @@
         <v>SearchParameter-us-core-condition-patient.html</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="15.75" customHeight="1">
+    <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4866,7 +4867,7 @@
         <v>SearchParameter-us-core-encounter-id.html</v>
       </c>
     </row>
-    <row r="15" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="15" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4916,7 +4917,7 @@
         <v>SearchParameter-us-core-encounter-class.html</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="15.75" customHeight="1">
+    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4970,7 +4971,7 @@
         <v>SearchParameter-us-core-encounter-date.html</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="29.25">
+    <row r="17" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -5024,7 +5025,7 @@
         <v>SearchParameter-us-core-encounter-identifier.html</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -5082,7 +5083,7 @@
         <v>SearchParameter-us-core-encounter-patient.html</v>
       </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -5132,7 +5133,7 @@
         <v>SearchParameter-us-core-encounter-status.html</v>
       </c>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -5180,7 +5181,7 @@
         <v>SearchParameter-us-core-encounter-type.html</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -5230,7 +5231,7 @@
         <v>SearchParameter-us-core-patient-id.html</v>
       </c>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -5281,7 +5282,7 @@
         <v>SearchParameter-us-core-patient-birthdate.html</v>
       </c>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -5325,7 +5326,7 @@
         <v>SearchParameter-us-core-patient-family.html</v>
       </c>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -5374,7 +5375,7 @@
         <v>SearchParameter-us-core-patient-gender.html</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="15.75" customHeight="1">
+    <row r="25" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -5418,7 +5419,7 @@
         <v>SearchParameter-us-core-patient-given.html</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="15.75" customHeight="1">
+    <row r="26" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -5473,7 +5474,7 @@
         <v>SearchParameter-us-core-patient-identifier.html</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="15.75" customHeight="1">
+    <row r="27" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -5531,7 +5532,7 @@
         <v>SearchParameter-us-core-patient-name.html</v>
       </c>
     </row>
-    <row r="28" spans="1:28">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -5574,7 +5575,7 @@
         <v>SearchParameter-us-core-!questionnaire-_id.html</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="15.75" customHeight="1">
+    <row r="29" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -5619,7 +5620,7 @@
         <v>SearchParameter-us-core-!questionnaire-context-type-value.html</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="15.75" customHeight="1">
+    <row r="30" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -5669,7 +5670,7 @@
         <v>SearchParameter-us-core-!questionnaire-publisher.html</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="15.75" customHeight="1">
+    <row r="31" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -5716,7 +5717,7 @@
         <v>SearchParameter-us-core-!questionnaire-status.html</v>
       </c>
     </row>
-    <row r="32" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="32" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -5776,7 +5777,7 @@
         <v>SearchParameter-us-core-!questionnaire-title.html</v>
       </c>
     </row>
-    <row r="33" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="33" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -5821,7 +5822,7 @@
         <v>SearchParameter-us-core-!questionnaire-url.html</v>
       </c>
     </row>
-    <row r="34" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="34" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -5866,7 +5867,7 @@
         <v>SearchParameter-us-core-!questionnaire-version.html</v>
       </c>
     </row>
-    <row r="35" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="35" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -5917,7 +5918,7 @@
         <v>SearchParameter-us-core-condition-onset-date.html</v>
       </c>
     </row>
-    <row r="36" spans="1:28" s="1" customFormat="1">
+    <row r="36" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -5964,7 +5965,7 @@
         <v>SearchParameter-us-core-condition-code.html</v>
       </c>
     </row>
-    <row r="37" spans="1:28" s="1" customFormat="1">
+    <row r="37" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -6023,7 +6024,7 @@
         <v>SearchParameter-us-core-immunization-patient.html</v>
       </c>
     </row>
-    <row r="38" spans="1:28" s="1" customFormat="1">
+    <row r="38" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -6073,7 +6074,7 @@
         <v>SearchParameter-us-core-immunization-status.html</v>
       </c>
     </row>
-    <row r="39" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="39" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -6127,7 +6128,7 @@
         <v>SearchParameter-us-core-immunization-date.html</v>
       </c>
     </row>
-    <row r="40" spans="1:28" s="1" customFormat="1" ht="60">
+    <row r="40" spans="1:28" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -6180,7 +6181,7 @@
         <v>SearchParameter-us-core-documentreference-_id.html</v>
       </c>
     </row>
-    <row r="41" spans="1:28" s="1" customFormat="1">
+    <row r="41" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -6230,7 +6231,7 @@
         <v>SearchParameter-us-core-documentreference-status.html</v>
       </c>
     </row>
-    <row r="42" spans="1:28" s="1" customFormat="1" ht="43.5">
+    <row r="42" spans="1:28" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -6289,7 +6290,7 @@
         <v>SearchParameter-us-core-documentreference-patient.html</v>
       </c>
     </row>
-    <row r="43" spans="1:28" s="1" customFormat="1">
+    <row r="43" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -6339,7 +6340,7 @@
         <v>SearchParameter-us-core-documentreference-category.html</v>
       </c>
     </row>
-    <row r="44" spans="1:28" s="1" customFormat="1">
+    <row r="44" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -6386,7 +6387,7 @@
         <v>SearchParameter-us-core-documentreference-type.html</v>
       </c>
     </row>
-    <row r="45" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="45" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -6440,7 +6441,7 @@
         <v>SearchParameter-us-core-documentreference-date.html</v>
       </c>
     </row>
-    <row r="46" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="46" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -6493,7 +6494,7 @@
         <v>SearchParameter-us-core-documentreference-period.html</v>
       </c>
     </row>
-    <row r="47" spans="1:28" s="1" customFormat="1">
+    <row r="47" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -6543,7 +6544,7 @@
         <v>SearchParameter-us-core-diagnosticreport-status.html</v>
       </c>
     </row>
-    <row r="48" spans="1:28" s="1" customFormat="1">
+    <row r="48" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -6602,7 +6603,7 @@
         <v>SearchParameter-us-core-diagnosticreport-patient.html</v>
       </c>
     </row>
-    <row r="49" spans="1:28" s="1" customFormat="1">
+    <row r="49" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -6652,7 +6653,7 @@
         <v>SearchParameter-us-core-diagnosticreport-category.html</v>
       </c>
     </row>
-    <row r="50" spans="1:28" s="1" customFormat="1">
+    <row r="50" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -6702,7 +6703,7 @@
         <v>SearchParameter-us-core-diagnosticreport-code.html</v>
       </c>
     </row>
-    <row r="51" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="51" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -6756,7 +6757,7 @@
         <v>SearchParameter-us-core-diagnosticreport-date.html</v>
       </c>
     </row>
-    <row r="52" spans="1:28" s="1" customFormat="1">
+    <row r="52" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -6806,7 +6807,7 @@
         <v>SearchParameter-us-core-goal-lifecycle-status.html</v>
       </c>
     </row>
-    <row r="53" spans="1:28" s="1" customFormat="1">
+    <row r="53" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -6865,7 +6866,7 @@
         <v>SearchParameter-us-core-goal-patient.html</v>
       </c>
     </row>
-    <row r="54" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="54" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -6919,7 +6920,7 @@
         <v>SearchParameter-us-core-goal-target-date.html</v>
       </c>
     </row>
-    <row r="55" spans="1:28" s="1" customFormat="1">
+    <row r="55" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -6969,7 +6970,7 @@
         <v>SearchParameter-us-core-medicationrequest-status.html</v>
       </c>
     </row>
-    <row r="56" spans="1:28" s="1" customFormat="1" ht="43.5">
+    <row r="56" spans="1:28" s="1" customFormat="1" ht="46" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -7030,7 +7031,7 @@
         <v>SearchParameter-us-core-medicationrequest-patient.html</v>
       </c>
     </row>
-    <row r="57" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="57" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -7084,7 +7085,7 @@
         <v>SearchParameter-us-core-medicationrequest-authoredon.html</v>
       </c>
     </row>
-    <row r="58" spans="1:28" s="1" customFormat="1">
+    <row r="58" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -7134,7 +7135,7 @@
         <v>SearchParameter-us-core-medicationstatement-status.html</v>
       </c>
     </row>
-    <row r="59" spans="1:28" s="1" customFormat="1" ht="43.5">
+    <row r="59" spans="1:28" s="1" customFormat="1" ht="46" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -7194,7 +7195,7 @@
         <v>SearchParameter-us-core-medicationstatement-patient.html</v>
       </c>
     </row>
-    <row r="60" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="60" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -7248,7 +7249,7 @@
         <v>SearchParameter-us-core-medicationstatement-effective.html</v>
       </c>
     </row>
-    <row r="61" spans="1:28" s="1" customFormat="1">
+    <row r="61" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -7298,7 +7299,7 @@
         <v>SearchParameter-us-core-procedure-status.html</v>
       </c>
     </row>
-    <row r="62" spans="1:28" s="1" customFormat="1">
+    <row r="62" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -7356,7 +7357,7 @@
         <v>SearchParameter-us-core-procedure-patient.html</v>
       </c>
     </row>
-    <row r="63" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="63" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -7410,7 +7411,7 @@
         <v>SearchParameter-us-core-procedure-date.html</v>
       </c>
     </row>
-    <row r="64" spans="1:28" s="1" customFormat="1">
+    <row r="64" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -7460,7 +7461,7 @@
         <v>SearchParameter-us-core-procedure-code.html</v>
       </c>
     </row>
-    <row r="65" spans="1:28" s="1" customFormat="1">
+    <row r="65" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -7510,7 +7511,7 @@
         <v>SearchParameter-us-core-observation-status.html</v>
       </c>
     </row>
-    <row r="66" spans="1:28" s="1" customFormat="1">
+    <row r="66" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -7560,7 +7561,7 @@
         <v>SearchParameter-us-core-observation-category.html</v>
       </c>
     </row>
-    <row r="67" spans="1:28" s="1" customFormat="1">
+    <row r="67" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -7610,7 +7611,7 @@
         <v>SearchParameter-us-core-observation-code.html</v>
       </c>
     </row>
-    <row r="68" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="68" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -7664,7 +7665,7 @@
         <v>SearchParameter-us-core-observation-date.html</v>
       </c>
     </row>
-    <row r="69" spans="1:28" s="1" customFormat="1">
+    <row r="69" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -7723,7 +7724,7 @@
         <v>SearchParameter-us-core-observation-patient.html</v>
       </c>
     </row>
-    <row r="70" spans="1:28" s="1" customFormat="1">
+    <row r="70" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -7773,7 +7774,7 @@
         <v>SearchParameter-us-core-careplan-category.html</v>
       </c>
     </row>
-    <row r="71" spans="1:28" s="1" customFormat="1">
+    <row r="71" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -7820,7 +7821,7 @@
         <v>SearchParameter-us-core-!careplan-code.html</v>
       </c>
     </row>
-    <row r="72" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="72" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -7874,7 +7875,7 @@
         <v>SearchParameter-us-core-careplan-date.html</v>
       </c>
     </row>
-    <row r="73" spans="1:28" s="1" customFormat="1">
+    <row r="73" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -7933,7 +7934,7 @@
         <v>SearchParameter-us-core-careplan-patient.html</v>
       </c>
     </row>
-    <row r="74" spans="1:28" s="1" customFormat="1">
+    <row r="74" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -7983,7 +7984,7 @@
         <v>SearchParameter-us-core-careplan-status.html</v>
       </c>
     </row>
-    <row r="75" spans="1:28" s="1" customFormat="1">
+    <row r="75" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -8042,7 +8043,7 @@
         <v>SearchParameter-us-core-careteam-patient.html</v>
       </c>
     </row>
-    <row r="76" spans="1:28" s="1" customFormat="1">
+    <row r="76" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -8092,7 +8093,7 @@
         <v>SearchParameter-us-core-careteam-status.html</v>
       </c>
     </row>
-    <row r="77" spans="1:28" s="1" customFormat="1">
+    <row r="77" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -8151,7 +8152,7 @@
         <v>SearchParameter-us-core-device-patient.html</v>
       </c>
     </row>
-    <row r="78" spans="1:28" s="1" customFormat="1">
+    <row r="78" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -8193,7 +8194,7 @@
       <c r="Z78" s="5"/>
       <c r="AA78" s="12"/>
     </row>
-    <row r="79" spans="1:28" ht="18">
+    <row r="79" spans="1:28" ht="18" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -8247,7 +8248,7 @@
         <v>SearchParameter-us-core-location-name.html</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="18">
+    <row r="80" spans="1:28" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -8301,7 +8302,7 @@
         <v>SearchParameter-us-core-location-address.html</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="18">
+    <row r="81" spans="1:28" ht="18" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -8355,7 +8356,7 @@
         <v>SearchParameter-us-core-location-address-city.html</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="18">
+    <row r="82" spans="1:28" ht="18" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -8409,7 +8410,7 @@
         <v>SearchParameter-us-core-location-address-state.html</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="18">
+    <row r="83" spans="1:28" ht="18" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -8463,7 +8464,7 @@
         <v>SearchParameter-us-core-location-address-postalcode.html</v>
       </c>
     </row>
-    <row r="84" spans="1:28" s="1" customFormat="1" ht="18">
+    <row r="84" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -8517,7 +8518,7 @@
         <v>SearchParameter-us-core-organization-name.html</v>
       </c>
     </row>
-    <row r="85" spans="1:28" s="1" customFormat="1" ht="29.25">
+    <row r="85" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -8571,7 +8572,7 @@
         <v>SearchParameter-us-core-organization-address.html</v>
       </c>
     </row>
-    <row r="86" spans="1:28" s="1" customFormat="1" ht="18">
+    <row r="86" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -8625,7 +8626,7 @@
         <v>SearchParameter-us-core-!organization-address-city.html</v>
       </c>
     </row>
-    <row r="87" spans="1:28" s="1" customFormat="1" ht="18">
+    <row r="87" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -8679,7 +8680,7 @@
         <v>SearchParameter-us-core-!organization-adress-state.html</v>
       </c>
     </row>
-    <row r="88" spans="1:28" s="1" customFormat="1" ht="18">
+    <row r="88" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -8733,7 +8734,7 @@
         <v>SearchParameter-us-core-!organization-address-postalcode.html</v>
       </c>
     </row>
-    <row r="89" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="89" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -8790,7 +8791,7 @@
         <v>SearchParameter-us-core-practitioner-name.html</v>
       </c>
     </row>
-    <row r="90" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="90" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -8844,7 +8845,7 @@
         <v>SearchParameter-us-core-practitioner-identifier.html</v>
       </c>
     </row>
-    <row r="91" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="91" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -8901,7 +8902,7 @@
         <v>SearchParameter-us-core-practitionerrole-specialty.html</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="38.1" customHeight="1">
+    <row r="92" spans="1:28" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -8961,12 +8962,12 @@
         <v>SearchParameter-us-core-practitionerrole-practitioner.html</v>
       </c>
     </row>
-    <row r="93" spans="1:28">
+    <row r="93" spans="1:28" x14ac:dyDescent="0.2">
       <c r="Y93" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AB92" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
-  <sortState ref="A7:AA34">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AA34">
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8979,28 +8980,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="I41" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="H43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I68" sqref="I68"/>
+      <selection pane="bottomRight" activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="21.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" customWidth="1"/>
-    <col min="8" max="8" width="84.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="68.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="83.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="84.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="68.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="83.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1">
+    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>161</v>
       </c>
@@ -9032,7 +9033,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickTop="1">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -9057,7 +9058,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -9082,7 +9083,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -9107,7 +9108,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient and type</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -9132,7 +9133,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and type</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -9163,7 +9164,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified class and patient</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -9188,7 +9189,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -9213,7 +9214,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status and type</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -9239,7 +9240,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and type</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -9266,7 +9267,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -9292,7 +9293,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status and type</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -9317,7 +9318,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and type</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -9348,7 +9349,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified date and patient</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -9373,7 +9374,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and patient and type</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -9398,7 +9399,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and type</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -9429,7 +9430,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and type</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -9455,7 +9456,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified patient and status and type</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -9486,7 +9487,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and status</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -9513,7 +9514,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified status and type</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -9539,7 +9540,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -9564,7 +9565,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher and status</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -9590,7 +9591,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and status</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -9617,7 +9618,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -9644,7 +9645,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status and version</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -9671,7 +9672,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and version</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -9696,7 +9697,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and title and version</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -9721,7 +9722,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and version</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -9746,7 +9747,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified title and version</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -9777,7 +9778,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and family</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -9808,7 +9809,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and name</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -9839,7 +9840,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified family and gender</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -9870,7 +9871,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified gender and name</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -9903,7 +9904,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -9933,7 +9934,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -9963,7 +9964,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="1" customFormat="1">
+    <row r="36" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -9993,7 +9994,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -10023,7 +10024,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="1" customFormat="1">
+    <row r="38" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -10054,7 +10055,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="1" customFormat="1">
+    <row r="39" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -10085,7 +10086,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="1" customFormat="1">
+    <row r="40" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -10115,7 +10116,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="1" customFormat="1" ht="15.75">
+    <row r="41" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -10148,7 +10149,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="1" customFormat="1" ht="15.75">
+    <row r="42" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -10178,7 +10179,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="1" customFormat="1" ht="15.75">
+    <row r="43" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -10211,7 +10212,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="1" customFormat="1">
+    <row r="44" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -10241,7 +10242,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="1" customFormat="1">
+    <row r="45" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -10271,7 +10272,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="1" customFormat="1">
+    <row r="46" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -10301,7 +10302,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="1" customFormat="1">
+    <row r="47" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -10331,7 +10332,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="1" customFormat="1">
+    <row r="48" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -10361,7 +10362,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="1" customFormat="1">
+    <row r="49" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -10391,7 +10392,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="1" customFormat="1">
+    <row r="50" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -10422,7 +10423,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and lifecycle-status</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="1" customFormat="1">
+    <row r="51" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -10453,7 +10454,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and target-date</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="1" customFormat="1">
+    <row r="52" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -10483,7 +10484,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="1" customFormat="1">
+    <row r="53" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -10513,7 +10514,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="1" customFormat="1">
+    <row r="54" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -10544,7 +10545,7 @@
         <v>Fetches a bundle of all MedicationStatement resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="1" customFormat="1">
+    <row r="55" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -10574,7 +10575,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="1" customFormat="1">
+    <row r="56" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -10605,7 +10606,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="1" customFormat="1">
+    <row r="57" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -10636,7 +10637,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="1" customFormat="1">
+    <row r="58" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -10667,7 +10668,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="1" customFormat="1">
+    <row r="59" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -10699,7 +10700,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="1" customFormat="1">
+    <row r="60" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -10732,7 +10733,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="1" customFormat="1">
+    <row r="61" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -10762,7 +10763,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="62" spans="1:10" s="1" customFormat="1">
+    <row r="62" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -10795,7 +10796,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="1" customFormat="1">
+    <row r="63" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -10825,7 +10826,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="1" customFormat="1">
+    <row r="64" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -10855,7 +10856,7 @@
         <v>Fetches a bundle of all !Observation resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="1" customFormat="1">
+    <row r="65" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>58</v>
       </c>
@@ -10888,7 +10889,7 @@
         <v>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan`</v>
       </c>
     </row>
-    <row r="66" spans="1:16" s="1" customFormat="1">
+    <row r="66" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>59</v>
       </c>
@@ -10920,7 +10921,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="67" spans="1:16" s="1" customFormat="1">
+    <row r="67" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>61</v>
       </c>
@@ -10952,7 +10953,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="68" spans="1:16" s="1" customFormat="1">
+    <row r="68" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>62</v>
       </c>
@@ -10984,7 +10985,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="69" spans="1:16" s="1" customFormat="1">
+    <row r="69" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>63</v>
       </c>
@@ -11017,7 +11018,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="15.75">
+    <row r="70" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>64</v>
       </c>
@@ -11056,7 +11057,7 @@
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
     </row>
-    <row r="71" spans="1:16" s="1" customFormat="1">
+    <row r="71" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>58</v>
       </c>
@@ -11089,7 +11090,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and category and status</v>
       </c>
     </row>
-    <row r="72" spans="1:16" s="1" customFormat="1">
+    <row r="72" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>59</v>
       </c>
@@ -11122,7 +11123,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="73" spans="1:16" s="1" customFormat="1">
+    <row r="73" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>60</v>
       </c>
@@ -11155,7 +11156,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="74" spans="1:16" s="1" customFormat="1">
+    <row r="74" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>61</v>
       </c>
@@ -11188,7 +11189,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="75" spans="1:16" s="1" customFormat="1">
+    <row r="75" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>62</v>
       </c>
@@ -11218,7 +11219,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="76" spans="1:16" s="1" customFormat="1">
+    <row r="76" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>39</v>
       </c>
@@ -11249,7 +11250,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and status. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="77" spans="1:16" s="1" customFormat="1">
+    <row r="77" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>43</v>
       </c>
@@ -11278,7 +11279,7 @@
         <v>Fetches a bundle of all !DocumentReference resources for the specified patient and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="78" spans="1:16" s="1" customFormat="1">
+    <row r="78" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>40</v>
       </c>
@@ -11311,7 +11312,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="79" spans="1:16" s="1" customFormat="1" ht="15.75">
+    <row r="79" spans="1:16" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>42</v>
       </c>
@@ -11344,7 +11345,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="80" spans="1:16" s="1" customFormat="1">
+    <row r="80" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>41</v>
       </c>
@@ -11374,7 +11375,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="1" customFormat="1">
+    <row r="81" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>43</v>
       </c>
@@ -11405,7 +11406,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and type and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="82" spans="1:10" s="1" customFormat="1">
+    <row r="82" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
add fhir client folder
</commit_message>
<xml_diff>
--- a/SP/uscore-server.xlsx
+++ b/SP/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/Python/MyNotebooks/SP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE202E67-5A9C-864C-8FC3-17E5065A131A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83377B6-BBD4-BA4E-9B15-89CB3080F6FE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -1345,9 +1345,6 @@
     <t>US Core Organization Profile</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-pediatric-weight</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</t>
   </si>
   <si>
@@ -1387,9 +1384,6 @@
     <t>US Core Location Profile</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-pediatric-bmi</t>
-  </si>
-  <si>
     <t>US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
   </si>
   <si>
@@ -1402,12 +1396,6 @@
     <t>US Core Device Profile</t>
   </si>
   <si>
-    <t>US Core Pediatric Weight Observation Profile</t>
-  </si>
-  <si>
-    <t>US Core Pediatric BMI Observation Profile</t>
-  </si>
-  <si>
     <t>US Core AllergyIntolerance Profile</t>
   </si>
   <si>
@@ -1514,10 +1502,6 @@
   </si>
   <si>
     <t>This Section describes the expected capabilities of the US Core Server actor which is responsible for providing responses to the queries submitted by the US Core Requestors. The complete list of FHIR profiles, RESTful operations, and search parameters supported by US Core Servers are defined. Systems implementing this capability statement should meet the ONC 2015 Common Clinical Data Set (CCDS) access requirement for Patient Selection 170.315(g)(7) and Application Access - Data Category Request 170.315(g)(8) and and the latest proposed ONC [U.S. Core Data for Interoperability (USCDI)].  US Core Clients have the option of choosing from this list to access necessary data based on their local use cases and other contextual requirements.</t>
-  </si>
-  <si>
-    <t>A server **SHALL** be capable of responding to a $docref operation and  capable of returning at least a reference to a generated CCD document, if available. **MAY** provide references to other generated and existing document types as well. If a context date range is supplied the server ** SHOULD**  provide references to any document that falls within the date range If no date range is supplied, then the server **SHALL** provide references to last or current encounter.  **SHOULD** document what resources, if any, are returned as included resources
-`GET [base]/DocumentReference/$docref?patient=[id]`</t>
   </si>
   <si>
     <t>The MedicationStatement and MedicationRequest resources can represent a medication, using an external reference to a Medication resource. If an external Medication Resource is used in a MedicationStatement or a MedicationRequest, then the READ and SEARCH Criteria  **SHALL**  be supported.</t>
@@ -1597,6 +1581,22 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-lab</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/pediatric-bmi-for-age</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/pediatric-weight-for-height</t>
+  </si>
+  <si>
+    <t>US Core Pediatric BMI for Age Observation Profile</t>
+  </si>
+  <si>
+    <t>US Core Pediatric Weight  for Height Observation Profile</t>
+  </si>
+  <si>
+    <t>A server **SHALL** be capable of responding to a $docref operation and  capable of returning at least a reference to a generated CCD document, if available. **MAY** provide references to other 'on-demand' and 'stable' documents (or 'delayed/deferred assembly') that meet the query parameters as well. If a context date range is supplied the server ** SHOULD**  provide references to any document that falls within the date range If no date range is supplied, then the server **SHALL** provide references to last or current encounter.  **SHOULD** document what resources, if any, are returned as included resources
+`GET [base]/DocumentReference/$docref?patient=[id]`</t>
   </si>
 </sst>
 </file>
@@ -2065,7 +2065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -2088,7 +2088,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -2096,7 +2096,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2104,7 +2104,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2128,7 +2128,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
     </row>
   </sheetData>
@@ -2163,8 +2163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2224,7 +2224,7 @@
         <v>392</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -2254,7 +2254,7 @@
         <v>83</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -2344,7 +2344,7 @@
         <v>404</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -2370,11 +2370,11 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>407</v>
+      <c r="A14" s="11" t="s">
+        <v>486</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>426</v>
+        <v>488</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -2386,10 +2386,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>408</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>409</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
@@ -2401,25 +2401,25 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>411</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>412</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -2434,7 +2434,7 @@
         <v>203</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
@@ -2446,10 +2446,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>414</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>415</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>13</v>
@@ -2464,7 +2464,7 @@
         <v>261</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>13</v>
@@ -2476,10 +2476,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>418</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>13</v>
@@ -2491,10 +2491,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
@@ -2505,11 +2505,11 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>421</v>
+      <c r="A23" s="11" t="s">
+        <v>485</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>427</v>
+        <v>487</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>13</v>
@@ -2524,7 +2524,7 @@
         <v>202</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>13</v>
@@ -2539,7 +2539,7 @@
         <v>81</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>13</v>
@@ -2595,49 +2595,49 @@
         <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="F1" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="H1" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>461</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="R1" t="s">
         <v>19</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>358</v>
@@ -2646,10 +2646,10 @@
         <v>359</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="X1" t="s">
         <v>20</v>
@@ -2756,7 +2756,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>21</v>
@@ -2823,13 +2823,13 @@
     </row>
     <row r="13" spans="1:24" ht="80" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="R13" s="1" t="s">
         <v>21</v>
@@ -2846,7 +2846,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>21</v>
@@ -2866,7 +2866,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>21</v>
@@ -2875,7 +2875,7 @@
         <v>78</v>
       </c>
       <c r="U15" s="7" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
@@ -2999,8 +2999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3028,12 +3028,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="113" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="B2" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>191</v>
@@ -3042,7 +3042,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>464</v>
+        <v>489</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -3074,64 +3074,64 @@
         <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>445</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
@@ -3729,13 +3729,13 @@
   <dimension ref="A1:AB93"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="T78" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="AA41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V91" sqref="V91"/>
+      <selection pane="bottomRight" activeCell="AB54" sqref="AB54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="21.5" style="1" customWidth="1"/>
@@ -3762,7 +3762,7 @@
     <col min="28" max="28" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>151</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>SearchParameter-us-core-!example category search-category.html</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>SearchParameter-us-core-!example code search-code.html</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>SearchParameter-us-core-!example date search-date.html</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>SearchParameter-us-core-!example patient search-patient.html</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>SearchParameter-us-core-!example status search-status.html</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>SearchParameter-us-core-!patient-address.html</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>SearchParameter-us-core-!patient-telecom.html</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4254,7 +4254,7 @@
         <v>SearchParameter-us-core-allergyintolerance-clinical-status.html</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4313,7 +4313,7 @@
         <v>SearchParameter-us-core-allergyintolerance-patient.html</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>SearchParameter-us-core-condition-category.html</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>SearchParameter-us-core-condition-clinical-status.html</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4470,7 +4470,7 @@
         <v>SearchParameter-us-core-condition-patient.html</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4523,7 +4523,7 @@
         <v>SearchParameter-us-core-encounter-id.html</v>
       </c>
     </row>
-    <row r="15" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>SearchParameter-us-core-encounter-class.html</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>SearchParameter-us-core-encounter-date.html</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>SearchParameter-us-core-encounter-identifier.html</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>SearchParameter-us-core-encounter-patient.html</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4789,7 +4789,7 @@
         <v>SearchParameter-us-core-encounter-status.html</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4837,7 +4837,7 @@
         <v>SearchParameter-us-core-encounter-type.html</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -4887,7 +4887,7 @@
         <v>SearchParameter-us-core-patient-id.html</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -4938,7 +4938,7 @@
         <v>SearchParameter-us-core-patient-birthdate.html</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -4982,7 +4982,7 @@
         <v>SearchParameter-us-core-patient-family.html</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>SearchParameter-us-core-patient-gender.html</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -5075,7 +5075,7 @@
         <v>SearchParameter-us-core-patient-given.html</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>SearchParameter-us-core-patient-identifier.html</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>SearchParameter-us-core-patient-name.html</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>SearchParameter-us-core-!questionnaire-_id.html</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>SearchParameter-us-core-!questionnaire-context-type-value.html</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -5326,7 +5326,7 @@
         <v>SearchParameter-us-core-!questionnaire-publisher.html</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>SearchParameter-us-core-!questionnaire-status.html</v>
       </c>
     </row>
-    <row r="32" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -5433,7 +5433,7 @@
         <v>SearchParameter-us-core-!questionnaire-title.html</v>
       </c>
     </row>
-    <row r="33" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>SearchParameter-us-core-!questionnaire-url.html</v>
       </c>
     </row>
-    <row r="34" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -5523,7 +5523,7 @@
         <v>SearchParameter-us-core-!questionnaire-version.html</v>
       </c>
     </row>
-    <row r="35" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -5574,7 +5574,7 @@
         <v>SearchParameter-us-core-condition-onset-date.html</v>
       </c>
     </row>
-    <row r="36" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>SearchParameter-us-core-condition-code.html</v>
       </c>
     </row>
-    <row r="37" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -5680,7 +5680,7 @@
         <v>SearchParameter-us-core-immunization-patient.html</v>
       </c>
     </row>
-    <row r="38" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>SearchParameter-us-core-immunization-status.html</v>
       </c>
     </row>
-    <row r="39" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>SearchParameter-us-core-immunization-date.html</v>
       </c>
     </row>
-    <row r="40" spans="1:28" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>SearchParameter-us-core-documentreference-_id.html</v>
       </c>
     </row>
-    <row r="41" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -5887,7 +5887,7 @@
         <v>SearchParameter-us-core-documentreference-status.html</v>
       </c>
     </row>
-    <row r="42" spans="1:28" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -5946,7 +5946,7 @@
         <v>SearchParameter-us-core-documentreference-patient.html</v>
       </c>
     </row>
-    <row r="43" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -5996,7 +5996,7 @@
         <v>SearchParameter-us-core-documentreference-category.html</v>
       </c>
     </row>
-    <row r="44" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -6043,7 +6043,7 @@
         <v>SearchParameter-us-core-documentreference-type.html</v>
       </c>
     </row>
-    <row r="45" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -6097,7 +6097,7 @@
         <v>SearchParameter-us-core-documentreference-date.html</v>
       </c>
     </row>
-    <row r="46" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -6150,7 +6150,7 @@
         <v>SearchParameter-us-core-documentreference-period.html</v>
       </c>
     </row>
-    <row r="47" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -6200,7 +6200,7 @@
         <v>SearchParameter-us-core-diagnosticreport-status.html</v>
       </c>
     </row>
-    <row r="48" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -6259,7 +6259,7 @@
         <v>SearchParameter-us-core-diagnosticreport-patient.html</v>
       </c>
     </row>
-    <row r="49" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -6309,7 +6309,7 @@
         <v>SearchParameter-us-core-diagnosticreport-category.html</v>
       </c>
     </row>
-    <row r="50" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -6359,7 +6359,7 @@
         <v>SearchParameter-us-core-diagnosticreport-code.html</v>
       </c>
     </row>
-    <row r="51" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -6413,7 +6413,7 @@
         <v>SearchParameter-us-core-diagnosticreport-date.html</v>
       </c>
     </row>
-    <row r="52" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -6463,7 +6463,7 @@
         <v>SearchParameter-us-core-goal-lifecycle-status.html</v>
       </c>
     </row>
-    <row r="53" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>SearchParameter-us-core-goal-patient.html</v>
       </c>
     </row>
-    <row r="54" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -6530,7 +6530,7 @@
         <v>193</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>34</v>
@@ -6576,7 +6576,7 @@
         <v>SearchParameter-us-core-goal-target-date.html</v>
       </c>
     </row>
-    <row r="55" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -6626,7 +6626,7 @@
         <v>SearchParameter-us-core-medicationrequest-status.html</v>
       </c>
     </row>
-    <row r="56" spans="1:28" s="1" customFormat="1" ht="46" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -6687,7 +6687,7 @@
         <v>SearchParameter-us-core-medicationrequest-patient.html</v>
       </c>
     </row>
-    <row r="57" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -6741,7 +6741,7 @@
         <v>SearchParameter-us-core-medicationrequest-authoredon.html</v>
       </c>
     </row>
-    <row r="58" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -6791,7 +6791,7 @@
         <v>SearchParameter-us-core-medicationstatement-status.html</v>
       </c>
     </row>
-    <row r="59" spans="1:28" s="1" customFormat="1" ht="46" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -6831,7 +6831,7 @@
         <v>62</v>
       </c>
       <c r="V59" s="7" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="X59" s="1" t="s">
         <v>101</v>
@@ -6851,7 +6851,7 @@
         <v>SearchParameter-us-core-medicationstatement-patient.html</v>
       </c>
     </row>
-    <row r="60" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -6905,7 +6905,7 @@
         <v>SearchParameter-us-core-medicationstatement-effective.html</v>
       </c>
     </row>
-    <row r="61" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -6955,7 +6955,7 @@
         <v>SearchParameter-us-core-procedure-status.html</v>
       </c>
     </row>
-    <row r="62" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -7013,7 +7013,7 @@
         <v>SearchParameter-us-core-procedure-patient.html</v>
       </c>
     </row>
-    <row r="63" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -7067,7 +7067,7 @@
         <v>SearchParameter-us-core-procedure-date.html</v>
       </c>
     </row>
-    <row r="64" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -7117,7 +7117,7 @@
         <v>SearchParameter-us-core-procedure-code.html</v>
       </c>
     </row>
-    <row r="65" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -7167,7 +7167,7 @@
         <v>SearchParameter-us-core-observation-status.html</v>
       </c>
     </row>
-    <row r="66" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -7217,7 +7217,7 @@
         <v>SearchParameter-us-core-observation-category.html</v>
       </c>
     </row>
-    <row r="67" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -7267,7 +7267,7 @@
         <v>SearchParameter-us-core-observation-code.html</v>
       </c>
     </row>
-    <row r="68" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -7321,7 +7321,7 @@
         <v>SearchParameter-us-core-observation-date.html</v>
       </c>
     </row>
-    <row r="69" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -7380,7 +7380,7 @@
         <v>SearchParameter-us-core-observation-patient.html</v>
       </c>
     </row>
-    <row r="70" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -7430,7 +7430,7 @@
         <v>SearchParameter-us-core-careplan-category.html</v>
       </c>
     </row>
-    <row r="71" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -7477,7 +7477,7 @@
         <v>SearchParameter-us-core-!careplan-code.html</v>
       </c>
     </row>
-    <row r="72" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -7531,7 +7531,7 @@
         <v>SearchParameter-us-core-careplan-date.html</v>
       </c>
     </row>
-    <row r="73" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -7590,7 +7590,7 @@
         <v>SearchParameter-us-core-careplan-patient.html</v>
       </c>
     </row>
-    <row r="74" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -7640,7 +7640,7 @@
         <v>SearchParameter-us-core-careplan-status.html</v>
       </c>
     </row>
-    <row r="75" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -7699,7 +7699,7 @@
         <v>SearchParameter-us-core-careteam-patient.html</v>
       </c>
     </row>
-    <row r="76" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -7749,7 +7749,7 @@
         <v>SearchParameter-us-core-careteam-status.html</v>
       </c>
     </row>
-    <row r="77" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -7808,7 +7808,7 @@
         <v>SearchParameter-us-core-device-patient.html</v>
       </c>
     </row>
-    <row r="78" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -7849,8 +7849,12 @@
       </c>
       <c r="Z78" s="5"/>
       <c r="AA78" s="12"/>
-    </row>
-    <row r="79" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+      <c r="AB78" s="1" t="str">
+        <f t="shared" si="48"/>
+        <v>SearchParameter-us-core-device-type.html</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -7904,7 +7908,7 @@
         <v>SearchParameter-us-core-location-name.html</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -7958,7 +7962,7 @@
         <v>SearchParameter-us-core-location-address.html</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -8012,7 +8016,7 @@
         <v>SearchParameter-us-core-location-address-city.html</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -8066,7 +8070,7 @@
         <v>SearchParameter-us-core-location-address-state.html</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -8120,7 +8124,7 @@
         <v>SearchParameter-us-core-location-address-postalcode.html</v>
       </c>
     </row>
-    <row r="84" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -8174,7 +8178,7 @@
         <v>SearchParameter-us-core-organization-name.html</v>
       </c>
     </row>
-    <row r="85" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -8228,7 +8232,7 @@
         <v>SearchParameter-us-core-organization-address.html</v>
       </c>
     </row>
-    <row r="86" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -8282,7 +8286,7 @@
         <v>SearchParameter-us-core-!organization-address-city.html</v>
       </c>
     </row>
-    <row r="87" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -8336,7 +8340,7 @@
         <v>SearchParameter-us-core-!organization-adress-state.html</v>
       </c>
     </row>
-    <row r="88" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -8390,7 +8394,7 @@
         <v>SearchParameter-us-core-!organization-address-postalcode.html</v>
       </c>
     </row>
-    <row r="89" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -8447,7 +8451,7 @@
         <v>SearchParameter-us-core-practitioner-name.html</v>
       </c>
     </row>
-    <row r="90" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -8501,7 +8505,7 @@
         <v>SearchParameter-us-core-practitioner-identifier.html</v>
       </c>
     </row>
-    <row r="91" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -8558,7 +8562,7 @@
         <v>SearchParameter-us-core-practitionerrole-specialty.html</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -8618,7 +8622,7 @@
         <v>SearchParameter-us-core-practitionerrole-practitioner.html</v>
       </c>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y93" s="5"/>
     </row>
   </sheetData>
@@ -10091,7 +10095,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>78</v>
@@ -10103,7 +10107,7 @@
         <v>223</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="J51" s="5" t="str">
         <f t="shared" ref="J51" si="6">"Fetches a bundle of all "&amp;B51&amp;" resources for the specified "&amp;SUBSTITUTE(D51,","," and ")</f>
@@ -10134,7 +10138,7 @@
         <v>199</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="J52" s="5" t="s">
         <v>256</v>
@@ -10164,7 +10168,7 @@
         <v>252</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="J53" s="5" t="s">
         <v>257</v>
@@ -10194,7 +10198,7 @@
         <v>201</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="J54" s="5" t="str">
         <f t="shared" si="4"/>
@@ -10225,7 +10229,7 @@
         <v>253</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="J55" s="5" t="s">
         <v>258</v>
@@ -10332,7 +10336,7 @@
         <v>196</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>262</v>
@@ -10364,7 +10368,7 @@
         <v>196</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>155</v>
@@ -10397,7 +10401,7 @@
         <v>196</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>157</v>
@@ -10427,7 +10431,7 @@
         <v>196</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>208</v>
@@ -10460,7 +10464,7 @@
         <v>196</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>238</v>
@@ -10490,7 +10494,7 @@
         <v>361</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>126</v>
@@ -10571,7 +10575,7 @@
         <v>266</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="J66" s="5" t="s">
         <v>270</v>
@@ -10635,7 +10639,7 @@
         <v>265</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="J68" s="5" t="s">
         <v>272</v>
@@ -11025,7 +11029,7 @@
         <v>339</v>
       </c>
       <c r="I80" s="5" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="J80" s="5" t="s">
         <v>336</v>
@@ -11055,7 +11059,7 @@
         <v>340</v>
       </c>
       <c r="I81" s="5" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="J81" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B81&amp;" resources for the specified "&amp;SUBSTITUTE(D81,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
@@ -11083,13 +11087,13 @@
         <v>116</v>
       </c>
       <c r="H82" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="I82" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="J82" s="5" t="s">
         <v>451</v>
-      </c>
-      <c r="I82" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="J82" s="5" t="s">
-        <v>455</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated boilerplate to sp descriptionsm  added temp soln for  interaction documentation to cap statement
</commit_message>
<xml_diff>
--- a/SP/uscore-server.xlsx
+++ b/SP/uscore-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/Python/MyNotebooks/SP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Python\MyNotebooks\SP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83377B6-BBD4-BA4E-9B15-89CB3080F6FE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58BBE97-139D-4E41-A788-7017406B24B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -107,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="492">
   <si>
     <t>Element</t>
   </si>
@@ -1501,9 +1500,6 @@
     <t>conditionalDelete</t>
   </si>
   <si>
-    <t>This Section describes the expected capabilities of the US Core Server actor which is responsible for providing responses to the queries submitted by the US Core Requestors. The complete list of FHIR profiles, RESTful operations, and search parameters supported by US Core Servers are defined. Systems implementing this capability statement should meet the ONC 2015 Common Clinical Data Set (CCDS) access requirement for Patient Selection 170.315(g)(7) and Application Access - Data Category Request 170.315(g)(8) and and the latest proposed ONC [U.S. Core Data for Interoperability (USCDI)].  US Core Clients have the option of choosing from this list to access necessary data based on their local use cases and other contextual requirements.</t>
-  </si>
-  <si>
     <t>The MedicationStatement and MedicationRequest resources can represent a medication, using an external reference to a Medication resource. If an external Medication Resource is used in a MedicationStatement or a MedicationRequest, then the READ and SEARCH Criteria  **SHALL**  be supported.</t>
   </si>
   <si>
@@ -1597,13 +1593,25 @@
   <si>
     <t>A server **SHALL** be capable of responding to a $docref operation and  capable of returning at least a reference to a generated CCD document, if available. **MAY** provide references to other 'on-demand' and 'stable' documents (or 'delayed/deferred assembly') that meet the query parameters as well. If a context date range is supplied the server ** SHOULD**  provide references to any document that falls within the date range If no date range is supplied, then the server **SHALL** provide references to last or current encounter.  **SHOULD** document what resources, if any, are returned as included resources
 `GET [base]/DocumentReference/$docref?patient=[id]`</t>
+  </si>
+  <si>
+    <t>doc_DiagnosticReport</t>
+  </si>
+  <si>
+    <t>This conformance expectation applies **only**  to the *US Core DiagnosticReport Profile for Report and Note exchange* profile.  The conformance expectation for the *US Core DiagnosticReport Profile for Laboratory Results Reporting* is  **MAY**.</t>
+  </si>
+  <si>
+    <t>This Section describes the expected capabilities of the US Core Server actor which is responsible for providing responses to the queries submitted by the US Core Requestors. The complete list of FHIR profiles, RESTful operations, and search parameters supported by US Core Servers are defined. Systems implementing this capability statement should meet the ONC 2015 Common Clinical Data Set (CCDS) access requirement for Patient Selection 170.315(g)(7) and Application Access - Data Category Request 170.315(g)(8) and and the latest proposed ONC [U.S. Core Data for Interoperability (USCDI)].  US Core Clients have the option of choosing from this list to access necessary data based on their local use cases and other contextual requirements.
+*NOTE* : The [capabilitystatement-expectation](http://hl7.org/fhir/R4/extension-capabilitystatement-expectation.html) extension is used throughout this resource to formally express implementer expectations for the various elements.   This guide extends the usage context of this extension  to apply to these additional elements:
+- CapabilityStatement.rest.resource
+- [capabilitystatement-search-parameter-combination](http://hl7.org/fhir/R4/extension-capabilitystatement-search-parameter-combination.html) extension</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2066,16 +2074,16 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="95.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="95.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2083,31 +2091,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="105" customHeight="1">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2115,7 +2123,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="351.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="351.75" customHeight="1">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2123,12 +2131,12 @@
         <v>387</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="103.5" customHeight="1">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -2144,9 +2152,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -2167,15 +2175,15 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="94" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -2189,7 +2197,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>388</v>
       </c>
@@ -2204,7 +2212,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>390</v>
       </c>
@@ -2219,7 +2227,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>392</v>
       </c>
@@ -2234,7 +2242,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>393</v>
       </c>
@@ -2249,7 +2257,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>83</v>
       </c>
@@ -2264,7 +2272,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>395</v>
       </c>
@@ -2279,7 +2287,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>308</v>
       </c>
@@ -2294,7 +2302,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>398</v>
       </c>
@@ -2309,7 +2317,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>400</v>
       </c>
@@ -2324,7 +2332,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>402</v>
       </c>
@@ -2339,7 +2347,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>404</v>
       </c>
@@ -2354,7 +2362,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>405</v>
       </c>
@@ -2369,12 +2377,12 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="11" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -2384,7 +2392,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>407</v>
       </c>
@@ -2399,7 +2407,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>409</v>
       </c>
@@ -2414,12 +2422,12 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -2429,7 +2437,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
         <v>203</v>
       </c>
@@ -2444,7 +2452,7 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>413</v>
       </c>
@@ -2459,7 +2467,7 @@
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
         <v>261</v>
       </c>
@@ -2474,7 +2482,7 @@
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
         <v>416</v>
       </c>
@@ -2489,7 +2497,7 @@
       </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
         <v>418</v>
       </c>
@@ -2504,12 +2512,12 @@
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="11" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>13</v>
@@ -2519,7 +2527,7 @@
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
         <v>202</v>
       </c>
@@ -2534,7 +2542,7 @@
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
         <v>81</v>
       </c>
@@ -2566,22 +2574,22 @@
       <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="12" width="17.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5" style="1" customWidth="1"/>
-    <col min="14" max="17" width="17.5" style="1" customWidth="1"/>
-    <col min="18" max="19" width="20.5" style="1" customWidth="1"/>
-    <col min="20" max="23" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.42578125" style="1" customWidth="1"/>
+    <col min="14" max="17" width="17.42578125" style="1" customWidth="1"/>
+    <col min="18" max="19" width="20.42578125" style="1" customWidth="1"/>
+    <col min="20" max="23" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="18" thickBot="1">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2595,49 +2603,49 @@
         <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F1" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H1" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>452</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>453</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>457</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>458</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="R1" t="s">
         <v>19</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>358</v>
@@ -2655,7 +2663,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="38.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="38.25" customHeight="1" thickTop="1">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -2675,7 +2683,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24">
       <c r="A3" s="1" t="s">
         <v>259</v>
       </c>
@@ -2689,7 +2697,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24">
       <c r="A4" s="1" t="s">
         <v>273</v>
       </c>
@@ -2703,7 +2711,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24">
       <c r="A5" s="1" t="s">
         <v>148</v>
       </c>
@@ -2720,7 +2728,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24">
       <c r="A6" s="1" t="s">
         <v>277</v>
       </c>
@@ -2734,7 +2742,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24">
       <c r="A7" s="1" t="s">
         <v>192</v>
       </c>
@@ -2748,7 +2756,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="64" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" ht="75">
       <c r="A8" s="1" t="s">
         <v>191</v>
       </c>
@@ -2756,7 +2764,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>21</v>
@@ -2765,7 +2773,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -2779,7 +2787,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24">
       <c r="A10" s="1" t="s">
         <v>193</v>
       </c>
@@ -2793,7 +2801,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24">
       <c r="A11" s="1" t="s">
         <v>172</v>
       </c>
@@ -2807,7 +2815,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24">
       <c r="A12" s="1" t="s">
         <v>278</v>
       </c>
@@ -2821,7 +2829,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="80" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" ht="105">
       <c r="A13" s="1" t="s">
         <v>411</v>
       </c>
@@ -2829,7 +2837,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="R13" s="1" t="s">
         <v>21</v>
@@ -2838,7 +2846,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="288" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" ht="315">
       <c r="A14" s="1" t="s">
         <v>194</v>
       </c>
@@ -2846,7 +2854,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>21</v>
@@ -2858,7 +2866,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="288" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" ht="315">
       <c r="A15" s="1" t="s">
         <v>197</v>
       </c>
@@ -2866,7 +2874,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>21</v>
@@ -2878,7 +2886,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24">
       <c r="A16" s="1" t="s">
         <v>196</v>
       </c>
@@ -2892,7 +2900,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21">
       <c r="A17" s="1" t="s">
         <v>292</v>
       </c>
@@ -2906,7 +2914,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -2920,7 +2928,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21">
       <c r="A19" s="1" t="s">
         <v>299</v>
       </c>
@@ -2934,7 +2942,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21">
       <c r="A20" s="1" t="s">
         <v>302</v>
       </c>
@@ -2951,7 +2959,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21">
       <c r="A21" s="1" t="s">
         <v>195</v>
       </c>
@@ -2965,28 +2973,28 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21">
       <c r="A22"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21">
       <c r="A23"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21">
       <c r="A24"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21">
       <c r="A25"/>
     </row>
-    <row r="56" spans="20:23" ht="18" x14ac:dyDescent="0.2">
+    <row r="56" spans="20:23" ht="18">
       <c r="T56" s="7"/>
       <c r="V56" s="7"/>
       <c r="W56" s="7"/>
     </row>
-    <row r="59" spans="20:23" ht="18" x14ac:dyDescent="0.2">
+    <row r="59" spans="20:23" ht="18">
       <c r="W59" s="7"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A21">
+  <sortState ref="A2:A21">
     <sortCondition ref="A2:A21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2999,19 +3007,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -3028,7 +3036,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="135.75" thickBot="1">
       <c r="A2" s="15" t="s">
         <v>425</v>
       </c>
@@ -3042,10 +3050,10 @@
         <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="E4" s="2"/>
     </row>
   </sheetData>
@@ -3055,21 +3063,22 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.1640625" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -3089,52 +3098,55 @@
         <v>430</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="135">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -3153,14 +3165,14 @@
       <c r="F2" t="s">
         <v>34</v>
       </c>
-      <c r="G2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" t="s">
-        <v>34</v>
+      <c r="G2" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="J2" t="s">
         <v>34</v>
@@ -3198,8 +3210,11 @@
       <c r="U2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3218,9 +3233,6 @@
       <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
       <c r="H3" t="s">
         <v>13</v>
       </c>
@@ -3263,8 +3275,11 @@
       <c r="U3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -3283,9 +3298,6 @@
       <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
       <c r="H4" t="s">
         <v>13</v>
       </c>
@@ -3328,8 +3340,11 @@
       <c r="U4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -3348,9 +3363,6 @@
       <c r="F5" t="s">
         <v>78</v>
       </c>
-      <c r="G5" t="s">
-        <v>78</v>
-      </c>
       <c r="H5" t="s">
         <v>78</v>
       </c>
@@ -3393,8 +3405,11 @@
       <c r="U5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -3413,11 +3428,8 @@
       <c r="F6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>34</v>
@@ -3458,8 +3470,11 @@
       <c r="U6" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -3478,9 +3493,6 @@
       <c r="F7" t="s">
         <v>34</v>
       </c>
-      <c r="G7" t="s">
-        <v>34</v>
-      </c>
       <c r="H7" t="s">
         <v>34</v>
       </c>
@@ -3523,8 +3535,11 @@
       <c r="U7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -3543,9 +3558,6 @@
       <c r="F8" t="s">
         <v>34</v>
       </c>
-      <c r="G8" t="s">
-        <v>34</v>
-      </c>
       <c r="H8" t="s">
         <v>34</v>
       </c>
@@ -3588,8 +3600,11 @@
       <c r="U8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -3608,9 +3623,6 @@
       <c r="F9" t="s">
         <v>78</v>
       </c>
-      <c r="G9" t="s">
-        <v>78</v>
-      </c>
       <c r="H9" t="s">
         <v>78</v>
       </c>
@@ -3653,8 +3665,11 @@
       <c r="U9" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -3673,9 +3688,6 @@
       <c r="F10" t="s">
         <v>34</v>
       </c>
-      <c r="G10" t="s">
-        <v>34</v>
-      </c>
       <c r="H10" t="s">
         <v>34</v>
       </c>
@@ -3716,6 +3728,9 @@
         <v>34</v>
       </c>
       <c r="U10" t="s">
+        <v>34</v>
+      </c>
+      <c r="V10" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3728,41 +3743,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AB93"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="AA41" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="Y41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB54" sqref="AB54"/>
+      <selection pane="bottomRight" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="21.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="21.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="36.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" style="1" customWidth="1"/>
     <col min="16" max="16" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="49.6640625" style="1" customWidth="1"/>
-    <col min="21" max="22" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="49.7109375" style="1" customWidth="1"/>
+    <col min="21" max="22" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16" style="1" customWidth="1"/>
-    <col min="24" max="24" width="50.83203125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="68.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="90.6640625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="83.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="38.1640625" customWidth="1"/>
+    <col min="24" max="24" width="50.85546875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="68.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="90.7109375" style="1" customWidth="1"/>
+    <col min="27" max="27" width="83.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="18.95" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>151</v>
       </c>
@@ -3848,7 +3863,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1" thickTop="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3898,7 +3913,7 @@
         <v>SearchParameter-us-core-!example category search-category.html</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3945,7 +3960,7 @@
         <v>SearchParameter-us-core-!example code search-code.html</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3999,7 +4014,7 @@
         <v>SearchParameter-us-core-!example date search-date.html</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4058,7 +4073,7 @@
         <v>SearchParameter-us-core-!example patient search-patient.html</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4108,7 +4123,7 @@
         <v>SearchParameter-us-core-!example status search-status.html</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" ht="18.95" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4158,7 +4173,7 @@
         <v>SearchParameter-us-core-!patient-address.html</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" ht="18.95" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4208,7 +4223,7 @@
         <v>SearchParameter-us-core-!patient-telecom.html</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" ht="18.95" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4254,7 +4269,7 @@
         <v>SearchParameter-us-core-allergyintolerance-clinical-status.html</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" ht="18.95" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4313,7 +4328,7 @@
         <v>SearchParameter-us-core-allergyintolerance-patient.html</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="18.95" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4364,7 +4379,7 @@
         <v>SearchParameter-us-core-condition-category.html</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="18.95" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4412,7 +4427,7 @@
         <v>SearchParameter-us-core-condition-clinical-status.html</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="18.95" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4470,7 +4485,7 @@
         <v>SearchParameter-us-core-condition-patient.html</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="18.95" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4523,7 +4538,7 @@
         <v>SearchParameter-us-core-encounter-id.html</v>
       </c>
     </row>
-    <row r="15" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4573,7 +4588,7 @@
         <v>SearchParameter-us-core-encounter-class.html</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="18.95" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4627,7 +4642,7 @@
         <v>SearchParameter-us-core-encounter-date.html</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" ht="18.95" customHeight="1">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4681,7 +4696,7 @@
         <v>SearchParameter-us-core-encounter-identifier.html</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" ht="18.95" customHeight="1">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4739,7 +4754,7 @@
         <v>SearchParameter-us-core-encounter-patient.html</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" ht="18.95" customHeight="1">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4789,7 +4804,7 @@
         <v>SearchParameter-us-core-encounter-status.html</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" ht="18.95" customHeight="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4837,7 +4852,7 @@
         <v>SearchParameter-us-core-encounter-type.html</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" ht="18.95" customHeight="1">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -4887,7 +4902,7 @@
         <v>SearchParameter-us-core-patient-id.html</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" ht="18.95" customHeight="1">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -4938,7 +4953,7 @@
         <v>SearchParameter-us-core-patient-birthdate.html</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" ht="18.95" customHeight="1">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -4982,7 +4997,7 @@
         <v>SearchParameter-us-core-patient-family.html</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" ht="18.95" customHeight="1">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -5031,7 +5046,7 @@
         <v>SearchParameter-us-core-patient-gender.html</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" ht="18.95" customHeight="1">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -5075,7 +5090,7 @@
         <v>SearchParameter-us-core-patient-given.html</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" ht="18.95" customHeight="1">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -5130,7 +5145,7 @@
         <v>SearchParameter-us-core-patient-identifier.html</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" ht="18.95" customHeight="1">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -5188,7 +5203,7 @@
         <v>SearchParameter-us-core-patient-name.html</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" ht="18.95" customHeight="1">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -5231,7 +5246,7 @@
         <v>SearchParameter-us-core-!questionnaire-_id.html</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" ht="18.95" customHeight="1">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -5276,7 +5291,7 @@
         <v>SearchParameter-us-core-!questionnaire-context-type-value.html</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" ht="18.95" customHeight="1">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -5326,7 +5341,7 @@
         <v>SearchParameter-us-core-!questionnaire-publisher.html</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" ht="18.95" customHeight="1">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -5373,7 +5388,7 @@
         <v>SearchParameter-us-core-!questionnaire-status.html</v>
       </c>
     </row>
-    <row r="32" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -5433,7 +5448,7 @@
         <v>SearchParameter-us-core-!questionnaire-title.html</v>
       </c>
     </row>
-    <row r="33" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -5478,7 +5493,7 @@
         <v>SearchParameter-us-core-!questionnaire-url.html</v>
       </c>
     </row>
-    <row r="34" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -5523,7 +5538,7 @@
         <v>SearchParameter-us-core-!questionnaire-version.html</v>
       </c>
     </row>
-    <row r="35" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -5574,7 +5589,7 @@
         <v>SearchParameter-us-core-condition-onset-date.html</v>
       </c>
     </row>
-    <row r="36" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -5621,7 +5636,7 @@
         <v>SearchParameter-us-core-condition-code.html</v>
       </c>
     </row>
-    <row r="37" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -5680,7 +5695,7 @@
         <v>SearchParameter-us-core-immunization-patient.html</v>
       </c>
     </row>
-    <row r="38" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -5730,7 +5745,7 @@
         <v>SearchParameter-us-core-immunization-status.html</v>
       </c>
     </row>
-    <row r="39" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -5784,7 +5799,7 @@
         <v>SearchParameter-us-core-immunization-date.html</v>
       </c>
     </row>
-    <row r="40" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -5837,7 +5852,7 @@
         <v>SearchParameter-us-core-documentreference-_id.html</v>
       </c>
     </row>
-    <row r="41" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -5887,7 +5902,7 @@
         <v>SearchParameter-us-core-documentreference-status.html</v>
       </c>
     </row>
-    <row r="42" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -5946,7 +5961,7 @@
         <v>SearchParameter-us-core-documentreference-patient.html</v>
       </c>
     </row>
-    <row r="43" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -5996,7 +6011,7 @@
         <v>SearchParameter-us-core-documentreference-category.html</v>
       </c>
     </row>
-    <row r="44" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -6043,7 +6058,7 @@
         <v>SearchParameter-us-core-documentreference-type.html</v>
       </c>
     </row>
-    <row r="45" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -6097,7 +6112,7 @@
         <v>SearchParameter-us-core-documentreference-date.html</v>
       </c>
     </row>
-    <row r="46" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -6150,7 +6165,7 @@
         <v>SearchParameter-us-core-documentreference-period.html</v>
       </c>
     </row>
-    <row r="47" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -6200,7 +6215,7 @@
         <v>SearchParameter-us-core-diagnosticreport-status.html</v>
       </c>
     </row>
-    <row r="48" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -6259,7 +6274,7 @@
         <v>SearchParameter-us-core-diagnosticreport-patient.html</v>
       </c>
     </row>
-    <row r="49" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -6309,7 +6324,7 @@
         <v>SearchParameter-us-core-diagnosticreport-category.html</v>
       </c>
     </row>
-    <row r="50" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -6359,7 +6374,7 @@
         <v>SearchParameter-us-core-diagnosticreport-code.html</v>
       </c>
     </row>
-    <row r="51" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -6413,7 +6428,7 @@
         <v>SearchParameter-us-core-diagnosticreport-date.html</v>
       </c>
     </row>
-    <row r="52" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -6463,7 +6478,7 @@
         <v>SearchParameter-us-core-goal-lifecycle-status.html</v>
       </c>
     </row>
-    <row r="53" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -6522,7 +6537,7 @@
         <v>SearchParameter-us-core-goal-patient.html</v>
       </c>
     </row>
-    <row r="54" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -6530,7 +6545,7 @@
         <v>193</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>34</v>
@@ -6576,7 +6591,7 @@
         <v>SearchParameter-us-core-goal-target-date.html</v>
       </c>
     </row>
-    <row r="55" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -6626,7 +6641,7 @@
         <v>SearchParameter-us-core-medicationrequest-status.html</v>
       </c>
     </row>
-    <row r="56" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -6687,7 +6702,7 @@
         <v>SearchParameter-us-core-medicationrequest-patient.html</v>
       </c>
     </row>
-    <row r="57" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -6741,7 +6756,7 @@
         <v>SearchParameter-us-core-medicationrequest-authoredon.html</v>
       </c>
     </row>
-    <row r="58" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -6791,7 +6806,7 @@
         <v>SearchParameter-us-core-medicationstatement-status.html</v>
       </c>
     </row>
-    <row r="59" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -6851,7 +6866,7 @@
         <v>SearchParameter-us-core-medicationstatement-patient.html</v>
       </c>
     </row>
-    <row r="60" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -6905,7 +6920,7 @@
         <v>SearchParameter-us-core-medicationstatement-effective.html</v>
       </c>
     </row>
-    <row r="61" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -6955,7 +6970,7 @@
         <v>SearchParameter-us-core-procedure-status.html</v>
       </c>
     </row>
-    <row r="62" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -7013,7 +7028,7 @@
         <v>SearchParameter-us-core-procedure-patient.html</v>
       </c>
     </row>
-    <row r="63" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -7067,7 +7082,7 @@
         <v>SearchParameter-us-core-procedure-date.html</v>
       </c>
     </row>
-    <row r="64" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -7117,7 +7132,7 @@
         <v>SearchParameter-us-core-procedure-code.html</v>
       </c>
     </row>
-    <row r="65" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -7167,7 +7182,7 @@
         <v>SearchParameter-us-core-observation-status.html</v>
       </c>
     </row>
-    <row r="66" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -7217,7 +7232,7 @@
         <v>SearchParameter-us-core-observation-category.html</v>
       </c>
     </row>
-    <row r="67" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -7267,7 +7282,7 @@
         <v>SearchParameter-us-core-observation-code.html</v>
       </c>
     </row>
-    <row r="68" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -7321,7 +7336,7 @@
         <v>SearchParameter-us-core-observation-date.html</v>
       </c>
     </row>
-    <row r="69" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -7380,7 +7395,7 @@
         <v>SearchParameter-us-core-observation-patient.html</v>
       </c>
     </row>
-    <row r="70" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -7430,7 +7445,7 @@
         <v>SearchParameter-us-core-careplan-category.html</v>
       </c>
     </row>
-    <row r="71" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -7477,7 +7492,7 @@
         <v>SearchParameter-us-core-!careplan-code.html</v>
       </c>
     </row>
-    <row r="72" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -7531,7 +7546,7 @@
         <v>SearchParameter-us-core-careplan-date.html</v>
       </c>
     </row>
-    <row r="73" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -7590,7 +7605,7 @@
         <v>SearchParameter-us-core-careplan-patient.html</v>
       </c>
     </row>
-    <row r="74" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -7640,7 +7655,7 @@
         <v>SearchParameter-us-core-careplan-status.html</v>
       </c>
     </row>
-    <row r="75" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -7699,7 +7714,7 @@
         <v>SearchParameter-us-core-careteam-patient.html</v>
       </c>
     </row>
-    <row r="76" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -7749,7 +7764,7 @@
         <v>SearchParameter-us-core-careteam-status.html</v>
       </c>
     </row>
-    <row r="77" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -7808,7 +7823,7 @@
         <v>SearchParameter-us-core-device-patient.html</v>
       </c>
     </row>
-    <row r="78" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -7854,7 +7869,7 @@
         <v>SearchParameter-us-core-device-type.html</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:28" ht="18.95" customHeight="1">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -7908,7 +7923,7 @@
         <v>SearchParameter-us-core-location-name.html</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:28" ht="18.95" customHeight="1">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -7962,7 +7977,7 @@
         <v>SearchParameter-us-core-location-address.html</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:28" ht="18.95" customHeight="1">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -8016,7 +8031,7 @@
         <v>SearchParameter-us-core-location-address-city.html</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:28" ht="18.95" customHeight="1">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -8070,7 +8085,7 @@
         <v>SearchParameter-us-core-location-address-state.html</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:28" ht="18.95" customHeight="1">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -8124,7 +8139,7 @@
         <v>SearchParameter-us-core-location-address-postalcode.html</v>
       </c>
     </row>
-    <row r="84" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -8178,7 +8193,7 @@
         <v>SearchParameter-us-core-organization-name.html</v>
       </c>
     </row>
-    <row r="85" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -8232,7 +8247,7 @@
         <v>SearchParameter-us-core-organization-address.html</v>
       </c>
     </row>
-    <row r="86" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -8286,7 +8301,7 @@
         <v>SearchParameter-us-core-!organization-address-city.html</v>
       </c>
     </row>
-    <row r="87" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -8340,7 +8355,7 @@
         <v>SearchParameter-us-core-!organization-adress-state.html</v>
       </c>
     </row>
-    <row r="88" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -8394,7 +8409,7 @@
         <v>SearchParameter-us-core-!organization-address-postalcode.html</v>
       </c>
     </row>
-    <row r="89" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -8451,7 +8466,7 @@
         <v>SearchParameter-us-core-practitioner-name.html</v>
       </c>
     </row>
-    <row r="90" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -8505,7 +8520,7 @@
         <v>SearchParameter-us-core-practitioner-identifier.html</v>
       </c>
     </row>
-    <row r="91" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -8562,7 +8577,7 @@
         <v>SearchParameter-us-core-practitionerrole-specialty.html</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:28" ht="18.95" customHeight="1">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -8622,12 +8637,12 @@
         <v>SearchParameter-us-core-practitionerrole-practitioner.html</v>
       </c>
     </row>
-    <row r="93" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:28" ht="18.95" customHeight="1">
       <c r="Y93" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AB92" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AA34">
+  <sortState ref="A7:AA34">
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8647,21 +8662,21 @@
       <selection pane="bottomRight" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="21.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" customWidth="1"/>
-    <col min="8" max="8" width="84.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="68.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="83.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="84.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="68.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="83.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>153</v>
       </c>
@@ -8693,7 +8708,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickTop="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -8718,7 +8733,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -8743,7 +8758,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -8768,7 +8783,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient and type</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -8793,7 +8808,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and type</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -8824,7 +8839,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified class and patient</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -8849,7 +8864,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -8874,7 +8889,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status and type</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -8900,7 +8915,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and type</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -8927,7 +8942,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -8953,7 +8968,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status and type</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -8978,7 +8993,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and type</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -9009,7 +9024,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified date and patient</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -9034,7 +9049,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and patient and type</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -9059,7 +9074,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and type</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -9090,7 +9105,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and type</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -9116,7 +9131,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified patient and status and type</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -9147,7 +9162,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and status</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -9174,7 +9189,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified status and type</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -9200,7 +9215,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -9225,7 +9240,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher and status</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -9251,7 +9266,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and status</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -9278,7 +9293,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -9305,7 +9320,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status and version</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -9332,7 +9347,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and version</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -9357,7 +9372,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and title and version</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -9382,7 +9397,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and version</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -9407,7 +9422,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified title and version</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -9438,7 +9453,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and family</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -9469,7 +9484,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and name</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -9500,7 +9515,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified family and gender</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -9531,7 +9546,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified gender and name</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -9564,7 +9579,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -9594,7 +9609,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -9624,7 +9639,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" s="1" customFormat="1">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -9654,7 +9669,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -9684,7 +9699,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" s="1" customFormat="1">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -9715,7 +9730,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" s="1" customFormat="1">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -9746,7 +9761,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" s="1" customFormat="1">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -9776,7 +9791,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" s="1" customFormat="1" ht="15.75">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -9809,7 +9824,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" s="1" customFormat="1" ht="15.75">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -9839,7 +9854,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" s="1" customFormat="1" ht="15.75">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -9872,7 +9887,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" s="1" customFormat="1">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -9902,7 +9917,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" s="1" customFormat="1">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -9932,7 +9947,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" s="1" customFormat="1">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -9962,7 +9977,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" s="1" customFormat="1">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -9992,7 +10007,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" s="1" customFormat="1">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -10022,7 +10037,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" s="1" customFormat="1">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -10052,7 +10067,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" s="1" customFormat="1">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -10083,7 +10098,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and lifecycle-status</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" s="1" customFormat="1">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -10095,7 +10110,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>78</v>
@@ -10107,14 +10122,14 @@
         <v>223</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="J51" s="5" t="str">
         <f t="shared" ref="J51" si="6">"Fetches a bundle of all "&amp;B51&amp;" resources for the specified "&amp;SUBSTITUTE(D51,","," and ")</f>
         <v>Fetches a bundle of all Goal resources for the specified patient and target-date</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" s="1" customFormat="1">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -10138,13 +10153,13 @@
         <v>199</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="J52" s="5" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" s="1" customFormat="1">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -10168,13 +10183,13 @@
         <v>252</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="J53" s="5" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" s="1" customFormat="1">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -10198,14 +10213,14 @@
         <v>201</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="J54" s="5" t="str">
         <f t="shared" si="4"/>
         <v>Fetches a bundle of all MedicationStatement resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" s="1" customFormat="1">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -10229,13 +10244,13 @@
         <v>253</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="J55" s="5" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" s="1" customFormat="1">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -10266,7 +10281,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" s="1" customFormat="1">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -10297,7 +10312,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" s="1" customFormat="1">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -10328,7 +10343,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" s="1" customFormat="1">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -10336,7 +10351,7 @@
         <v>196</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>262</v>
@@ -10360,7 +10375,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" s="1" customFormat="1">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -10368,7 +10383,7 @@
         <v>196</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>155</v>
@@ -10393,7 +10408,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" s="1" customFormat="1">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -10401,7 +10416,7 @@
         <v>196</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>157</v>
@@ -10423,7 +10438,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="62" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" s="1" customFormat="1">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -10431,7 +10446,7 @@
         <v>196</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>208</v>
@@ -10456,7 +10471,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" s="1" customFormat="1">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -10464,7 +10479,7 @@
         <v>196</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>238</v>
@@ -10486,7 +10501,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" s="1" customFormat="1">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -10494,7 +10509,7 @@
         <v>361</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>126</v>
@@ -10516,7 +10531,7 @@
         <v>Fetches a bundle of all !Observation resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" s="1" customFormat="1">
       <c r="A65" s="1">
         <v>58</v>
       </c>
@@ -10549,7 +10564,7 @@
         <v>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan`</v>
       </c>
     </row>
-    <row r="66" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" s="1" customFormat="1">
       <c r="A66" s="1">
         <v>59</v>
       </c>
@@ -10575,13 +10590,13 @@
         <v>266</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="J66" s="5" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="67" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" s="1" customFormat="1">
       <c r="A67" s="1">
         <v>61</v>
       </c>
@@ -10613,7 +10628,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="68" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" s="1" customFormat="1">
       <c r="A68" s="1">
         <v>62</v>
       </c>
@@ -10639,13 +10654,13 @@
         <v>265</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="J68" s="5" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="69" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" s="1" customFormat="1">
       <c r="A69" s="1">
         <v>63</v>
       </c>
@@ -10678,7 +10693,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" ht="15.75">
       <c r="A70" s="1">
         <v>64</v>
       </c>
@@ -10717,7 +10732,7 @@
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
     </row>
-    <row r="71" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" s="1" customFormat="1">
       <c r="A71" s="1">
         <v>58</v>
       </c>
@@ -10750,7 +10765,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and category and status</v>
       </c>
     </row>
-    <row r="72" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" s="1" customFormat="1">
       <c r="A72" s="1">
         <v>59</v>
       </c>
@@ -10783,7 +10798,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="73" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" s="1" customFormat="1">
       <c r="A73" s="1">
         <v>60</v>
       </c>
@@ -10816,7 +10831,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="74" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" s="1" customFormat="1">
       <c r="A74" s="1">
         <v>61</v>
       </c>
@@ -10849,7 +10864,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="75" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" s="1" customFormat="1">
       <c r="A75" s="1">
         <v>62</v>
       </c>
@@ -10879,7 +10894,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="76" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" s="1" customFormat="1">
       <c r="A76" s="1">
         <v>39</v>
       </c>
@@ -10910,7 +10925,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and status. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="77" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" s="1" customFormat="1">
       <c r="A77" s="1">
         <v>43</v>
       </c>
@@ -10939,7 +10954,7 @@
         <v>Fetches a bundle of all !DocumentReference resources for the specified patient and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="78" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" s="1" customFormat="1">
       <c r="A78" s="1">
         <v>40</v>
       </c>
@@ -10972,7 +10987,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="79" spans="1:16" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" s="1" customFormat="1" ht="15.75">
       <c r="A79" s="1">
         <v>42</v>
       </c>
@@ -11005,7 +11020,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="80" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" s="1" customFormat="1">
       <c r="A80" s="1">
         <v>41</v>
       </c>
@@ -11035,7 +11050,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" s="1" customFormat="1">
       <c r="A81" s="1">
         <v>43</v>
       </c>
@@ -11066,7 +11081,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and type and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="82" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" s="1" customFormat="1">
       <c r="A82" s="1">
         <v>41</v>
       </c>

</xml_diff>